<commit_message>
Freitag 10 03 2023
</commit_message>
<xml_diff>
--- a/abkuerzungen.xlsx
+++ b/abkuerzungen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\ストレージ\MarkDown\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2A7F7991-25E7-48B7-8A9E-1A10C5FF4D34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17759FC4-793F-4399-AA92-887744DC6DE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2790" yWindow="105" windowWidth="18435" windowHeight="15495" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1859" uniqueCount="1175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1874" uniqueCount="1190">
   <si>
     <t>NAS</t>
   </si>
@@ -5006,12 +5006,63 @@
   <si>
     <t>energy assisted perpendicular magnetic recording</t>
   </si>
+  <si>
+    <t>SSDP</t>
+  </si>
+  <si>
+    <t>Simple Service Discovery Protocol</t>
+  </si>
+  <si>
+    <t>apipa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Automatic Private IP Addressing </t>
+  </si>
+  <si>
+    <t>Request for Comments</t>
+  </si>
+  <si>
+    <t>rfc</t>
+  </si>
+  <si>
+    <t>IHL</t>
+  </si>
+  <si>
+    <t>IP header length </t>
+  </si>
+  <si>
+    <t>poof</t>
+  </si>
+  <si>
+    <t>pong</t>
+  </si>
+  <si>
+    <t>ping pong</t>
+  </si>
+  <si>
+    <t>Passive Observation Of Failures</t>
+  </si>
+  <si>
+    <t>When a host sees a
+     multicast query, but does not see the corresponding multicast
+     response, it can use this information to promptly delete stale data
+     from its cache.  To achieve the same level of user-interface
+     quality and responsiveness without multicast responses would
+     require lower cache lifetimes and more frequent network polling,
+     resulting in a higher packet rate.</t>
+  </si>
+  <si>
+    <t>Explicit Congestion Notification ()</t>
+  </si>
+  <si>
+    <t>ECN</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="121">
+  <fonts count="122">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5698,6 +5749,12 @@
       <color rgb="FF585961"/>
       <name val="Roboto"/>
     </font>
+    <font>
+      <sz val="19"/>
+      <color rgb="FF212529"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -5726,7 +5783,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="173">
+  <cellXfs count="175">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -6156,6 +6213,12 @@
     <xf numFmtId="0" fontId="120" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="121" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -6311,8 +6374,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00096219-7411-470E-8817-26E819582D2F}" name="Table1" displayName="Table1" ref="A1:F369" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:F369" xr:uid="{00096219-7411-470E-8817-26E819582D2F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00096219-7411-470E-8817-26E819582D2F}" name="Table1" displayName="Table1" ref="A1:F376" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:F376" xr:uid="{00096219-7411-470E-8817-26E819582D2F}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D299">
     <sortCondition ref="A1:A299"/>
   </sortState>
@@ -6591,10 +6654,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:XFD369"/>
+  <dimension ref="A1:XFD376"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A367" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B369" sqref="B369"/>
+    <sheetView tabSelected="1" topLeftCell="A363" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B376" sqref="B376"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="28.5"/>
@@ -13217,7 +13280,7 @@
       <c r="E364" s="122"/>
       <c r="F364" s="163"/>
     </row>
-    <row r="365" spans="1:6" customFormat="1" ht="27.75">
+    <row r="365" spans="1:6" ht="27.75">
       <c r="A365" s="108" t="s">
         <v>1166</v>
       </c>
@@ -13229,7 +13292,7 @@
       <c r="E365" s="122"/>
       <c r="F365" s="163"/>
     </row>
-    <row r="366" spans="1:6" customFormat="1" ht="75">
+    <row r="366" spans="1:6" ht="75">
       <c r="A366" s="108" t="s">
         <v>1169</v>
       </c>
@@ -13243,7 +13306,7 @@
       <c r="E366" s="122"/>
       <c r="F366" s="163"/>
     </row>
-    <row r="367" spans="1:6" customFormat="1">
+    <row r="367" spans="1:6">
       <c r="A367" s="108" t="s">
         <v>1173</v>
       </c>
@@ -13276,6 +13339,92 @@
       <c r="D369" s="117"/>
       <c r="E369" s="122"/>
       <c r="F369" s="163"/>
+    </row>
+    <row r="370" spans="1:6">
+      <c r="A370" s="108" t="s">
+        <v>1175</v>
+      </c>
+      <c r="B370" s="109" t="s">
+        <v>1176</v>
+      </c>
+      <c r="C370" s="110"/>
+      <c r="D370" s="117"/>
+      <c r="E370" s="122"/>
+      <c r="F370" s="163"/>
+    </row>
+    <row r="371" spans="1:6">
+      <c r="A371" s="108" t="s">
+        <v>1177</v>
+      </c>
+      <c r="B371" s="109" t="s">
+        <v>1178</v>
+      </c>
+      <c r="C371" s="110"/>
+      <c r="D371" s="117"/>
+      <c r="E371" s="122"/>
+      <c r="F371" s="163"/>
+    </row>
+    <row r="372" spans="1:6" ht="27.75">
+      <c r="A372" s="108" t="s">
+        <v>1180</v>
+      </c>
+      <c r="B372" s="109" t="s">
+        <v>1179</v>
+      </c>
+      <c r="C372" s="110"/>
+      <c r="D372" s="117"/>
+      <c r="E372" s="122"/>
+      <c r="F372" s="163"/>
+    </row>
+    <row r="373" spans="1:6" ht="29.25">
+      <c r="A373" s="169" t="s">
+        <v>1181</v>
+      </c>
+      <c r="B373" s="173" t="s">
+        <v>1182</v>
+      </c>
+      <c r="C373" s="110"/>
+      <c r="D373" s="117"/>
+      <c r="E373" s="122"/>
+      <c r="F373" s="163"/>
+    </row>
+    <row r="374" spans="1:6" ht="135">
+      <c r="A374" s="108" t="s">
+        <v>1183</v>
+      </c>
+      <c r="B374" s="109" t="s">
+        <v>1186</v>
+      </c>
+      <c r="C374" s="110"/>
+      <c r="D374" s="117" t="s">
+        <v>1187</v>
+      </c>
+      <c r="E374" s="122"/>
+      <c r="F374" s="163"/>
+    </row>
+    <row r="375" spans="1:6" ht="27.75">
+      <c r="A375" s="108" t="s">
+        <v>1184</v>
+      </c>
+      <c r="B375" s="109"/>
+      <c r="C375" s="110"/>
+      <c r="D375" s="117" t="s">
+        <v>1185</v>
+      </c>
+      <c r="E375" s="122"/>
+      <c r="F375" s="163"/>
+    </row>
+    <row r="376" spans="1:6" ht="83.25">
+      <c r="A376" s="108" t="s">
+        <v>1189</v>
+      </c>
+      <c r="B376" s="174" t="s">
+        <v>1188</v>
+      </c>
+      <c r="C376" s="110"/>
+      <c r="D376" s="117"/>
+      <c r="E376" s="122"/>
+      <c r="F376" s="163"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:D283">

</xml_diff>

<commit_message>
added more from kb
</commit_message>
<xml_diff>
--- a/abkuerzungen.xlsx
+++ b/abkuerzungen.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\ストレージ\MarkDown\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAAD52DE-6162-42EE-B40D-2C99DC3FBC1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D50C565-5977-46C8-A6B1-8437F09094BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30" yWindow="270" windowWidth="19065" windowHeight="15495" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="105" windowWidth="19065" windowHeight="15495" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2048" uniqueCount="1323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2056" uniqueCount="1331">
   <si>
     <t>NAS</t>
   </si>
@@ -5499,6 +5499,48 @@
   </si>
   <si>
     <t xml:space="preserve">accelerated grafic ports </t>
+  </si>
+  <si>
+    <t>CRUD </t>
+  </si>
+  <si>
+    <t>is an acronym for ways one can operate on stored data. It is a mnemonic for the four basic functions of persistent storage.</t>
+  </si>
+  <si>
+    <t>FQDn</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> *** is the complete address of an internet host or computer. It provides its exact location within the domain name system (DNS) by specifying the hostname, domain name and top-level domain (TLD)</t>
+  </si>
+  <si>
+    <t>TLD</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> top-level domain</t>
+  </si>
+  <si>
+    <t>fully qualified domain name</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF202124"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Create Read Update Delete</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF202124"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
   </si>
 </sst>
 </file>
@@ -6304,7 +6346,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="174">
+  <cellXfs count="175">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -6735,6 +6777,7 @@
     <xf numFmtId="0" fontId="133" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="107" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -7170,9 +7213,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:XFD436"/>
+  <dimension ref="A1:XFD439"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A425" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A429" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B436" sqref="B436"/>
     </sheetView>
   </sheetViews>
@@ -14524,7 +14567,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="423" spans="1:4">
+    <row r="423" spans="1:4" ht="30">
       <c r="A423" s="2" t="s">
         <v>1297</v>
       </c>
@@ -14694,6 +14737,36 @@
       </c>
       <c r="B436" s="4" t="s">
         <v>1322</v>
+      </c>
+    </row>
+    <row r="437" spans="1:4" ht="30">
+      <c r="A437" s="174" t="s">
+        <v>1323</v>
+      </c>
+      <c r="B437" s="174" t="s">
+        <v>1330</v>
+      </c>
+      <c r="D437" s="3" t="s">
+        <v>1324</v>
+      </c>
+    </row>
+    <row r="438" spans="1:4" ht="60">
+      <c r="A438" s="2" t="s">
+        <v>1325</v>
+      </c>
+      <c r="B438" s="4" t="s">
+        <v>1329</v>
+      </c>
+      <c r="D438" s="3" t="s">
+        <v>1326</v>
+      </c>
+    </row>
+    <row r="439" spans="1:4">
+      <c r="A439" s="2" t="s">
+        <v>1327</v>
+      </c>
+      <c r="B439" s="4" t="s">
+        <v>1328</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
didnt save last night
</commit_message>
<xml_diff>
--- a/abkuerzungen.xlsx
+++ b/abkuerzungen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\ストレージ\MarkDown\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D50C565-5977-46C8-A6B1-8437F09094BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D6744B9-2216-4038-816A-FC7E9D40E8A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="105" windowWidth="19065" windowHeight="15495" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2056" uniqueCount="1331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2116" uniqueCount="1390">
   <si>
     <t>NAS</t>
   </si>
@@ -5542,12 +5542,200 @@
       <t xml:space="preserve"> </t>
     </r>
   </si>
+  <si>
+    <t>ePVO</t>
+  </si>
+  <si>
+    <t>E-Privacy-Verordnung</t>
+  </si>
+  <si>
+    <t>TMG</t>
+  </si>
+  <si>
+    <t>Telemediengesetz</t>
+  </si>
+  <si>
+    <t>bdsg</t>
+  </si>
+  <si>
+    <t>Bundesdatenschutzgesetz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">isb </t>
+  </si>
+  <si>
+    <r>
+      <t>Informationssicherheitsbeauftragter</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF4D5156"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <t>it-sig</t>
+  </si>
+  <si>
+    <t>IT-Sicherheitsgesetz</t>
+  </si>
+  <si>
+    <t>BSIG</t>
+  </si>
+  <si>
+    <t>Gesetz über das Bundesamt für Sicherheit in der Informationstechnik</t>
+  </si>
+  <si>
+    <t>ISMS</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> information security management system</t>
+  </si>
+  <si>
+    <t>VSDI</t>
+  </si>
+  <si>
+    <t>Verband Sichere Digitale Identität</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(VSDI) versteht sich als praxisnahes Kompetenz-Netzwerk für Politik, Verwaltung und Wirtschaft, das die Transformation von analogen zu digitalen Identitäten vorantreibt. </t>
+  </si>
+  <si>
+    <t>BSI</t>
+  </si>
+  <si>
+    <t>Bundesamt für Sicherheit in der Informationstechnik</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AIT </t>
+  </si>
+  <si>
+    <t xml:space="preserve">FSK ???? </t>
+  </si>
+  <si>
+    <t>LTFS</t>
+  </si>
+  <si>
+    <t>Linear Tape File System</t>
+  </si>
+  <si>
+    <t>BER</t>
+  </si>
+  <si>
+    <t>Bit error rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*** is the number of received bits of a data stream over a communication channel that have been altered due to noise, interference, distortion or bit synchronization errors. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Media Recognition System </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MRS </t>
+  </si>
+  <si>
+    <t>VXA</t>
+  </si>
+  <si>
+    <t>??</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*** is a tape backup format originally created by Ecrix and now owned by Tandberg Data. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">LTO </t>
+  </si>
+  <si>
+    <t>Linear Tape-Open</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*** technology originally developed in the late 1990s as an open standards alternative to the proprietary magnetic tape formats that were available at the time.     </t>
+  </si>
+  <si>
+    <t>DLT</t>
+  </si>
+  <si>
+    <t>FSK</t>
+  </si>
+  <si>
+    <t>Digital Linear Tape</t>
+  </si>
+  <si>
+    <t xml:space="preserve">***  (previously called CompacTape) is a magnetic-tape data storage technology developed by Digital Equipment Corporation </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SLR </t>
+  </si>
+  <si>
+    <t>Scalable Linear Recording</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*** is the name used by Tandberg Data for its line of QIC based tape drives. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DDS </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> is a computer data storage technology that is based upon the Digital Audio Tape (DAT) format that was developed during the 1980s. </t>
+  </si>
+  <si>
+    <t>Digital Data Storage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DCC </t>
+  </si>
+  <si>
+    <t>Digital Compact Cassette</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> *** is a magnetic tape sound recording format introduced by Philips and Matsushita Electric in late 1992 </t>
+  </si>
+  <si>
+    <t>DAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Digital Audio Tape</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> *** ist ein digitales Audio-Magnetband (Tonband) für entsprechende Audiorekorder.    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">QIC </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quarter-inch cartridge </t>
+  </si>
+  <si>
+    <t xml:space="preserve">*** is a magnetic tape data storage format introduced by 3M in 1972,[1] with derivatives still in use as of 2016. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> *** ist ein Magnetband-System zur Datenspeicherung. </t>
+  </si>
+  <si>
+    <t>Advanced Intelligent Tape</t>
+  </si>
+  <si>
+    <t>**** is a file system that allows files stored on magnetic tape to be accessed in a similar fashion to those on disk or removable flash drives.</t>
+  </si>
+  <si>
+    <t>CLSID</t>
+  </si>
+  <si>
+    <t>class identifier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">***** is a serial number that represents a unique ID for any application component in Windows. In practice, this means all registry entries for an application component can usually be found under the registry key HKEY_CLASSES_ROOT\CLSID{CLSID value}. </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="134">
+  <fonts count="137">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -6318,6 +6506,25 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FF4D5156"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF4D5156"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="17"/>
+      <color rgb="FF202124"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -6346,7 +6553,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="175">
+  <cellXfs count="178">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -6778,6 +6985,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="107" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="112" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="134" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="136" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -7213,10 +7423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:XFD439"/>
+  <dimension ref="A1:XFD462"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A429" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B436" sqref="B436"/>
+    <sheetView tabSelected="1" topLeftCell="A455" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D465" sqref="D465"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="28.5"/>
@@ -14767,6 +14977,232 @@
       </c>
       <c r="B439" s="4" t="s">
         <v>1328</v>
+      </c>
+    </row>
+    <row r="440" spans="1:4">
+      <c r="A440" s="2" t="s">
+        <v>1331</v>
+      </c>
+      <c r="B440" s="151" t="s">
+        <v>1332</v>
+      </c>
+    </row>
+    <row r="441" spans="1:4">
+      <c r="A441" s="2" t="s">
+        <v>1333</v>
+      </c>
+      <c r="B441" s="175" t="s">
+        <v>1334</v>
+      </c>
+    </row>
+    <row r="442" spans="1:4">
+      <c r="A442" s="2" t="s">
+        <v>1335</v>
+      </c>
+      <c r="B442" s="4" t="s">
+        <v>1336</v>
+      </c>
+    </row>
+    <row r="443" spans="1:4">
+      <c r="A443" s="2" t="s">
+        <v>1337</v>
+      </c>
+      <c r="B443" s="176" t="s">
+        <v>1338</v>
+      </c>
+    </row>
+    <row r="444" spans="1:4">
+      <c r="A444" s="2" t="s">
+        <v>1339</v>
+      </c>
+      <c r="B444" s="4" t="s">
+        <v>1340</v>
+      </c>
+    </row>
+    <row r="445" spans="1:4" ht="45">
+      <c r="A445" s="2" t="s">
+        <v>1341</v>
+      </c>
+      <c r="B445" s="4" t="s">
+        <v>1342</v>
+      </c>
+    </row>
+    <row r="446" spans="1:4" ht="30">
+      <c r="A446" s="177" t="s">
+        <v>1343</v>
+      </c>
+      <c r="B446" s="4" t="s">
+        <v>1344</v>
+      </c>
+    </row>
+    <row r="447" spans="1:4" ht="45">
+      <c r="A447" s="2" t="s">
+        <v>1345</v>
+      </c>
+      <c r="B447" s="4" t="s">
+        <v>1346</v>
+      </c>
+      <c r="D447" s="3" t="s">
+        <v>1347</v>
+      </c>
+    </row>
+    <row r="448" spans="1:4" ht="30">
+      <c r="A448" s="2" t="s">
+        <v>1348</v>
+      </c>
+      <c r="B448" s="4" t="s">
+        <v>1349</v>
+      </c>
+    </row>
+    <row r="449" spans="1:4" ht="15.75">
+      <c r="A449" s="171" t="s">
+        <v>1350</v>
+      </c>
+      <c r="B449" s="4" t="s">
+        <v>1385</v>
+      </c>
+      <c r="D449" s="3" t="s">
+        <v>1384</v>
+      </c>
+    </row>
+    <row r="450" spans="1:4" ht="30">
+      <c r="A450" s="2" t="s">
+        <v>1381</v>
+      </c>
+      <c r="B450" s="4" t="s">
+        <v>1382</v>
+      </c>
+      <c r="D450" s="3" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="451" spans="1:4" ht="30">
+      <c r="A451" s="2" t="s">
+        <v>1378</v>
+      </c>
+      <c r="B451" s="4" t="s">
+        <v>1379</v>
+      </c>
+      <c r="D451" s="3" t="s">
+        <v>1380</v>
+      </c>
+    </row>
+    <row r="452" spans="1:4" ht="30">
+      <c r="A452" s="2" t="s">
+        <v>1375</v>
+      </c>
+      <c r="B452" s="4" t="s">
+        <v>1376</v>
+      </c>
+      <c r="D452" s="3" t="s">
+        <v>1377</v>
+      </c>
+    </row>
+    <row r="453" spans="1:4" ht="45">
+      <c r="A453" s="2" t="s">
+        <v>1372</v>
+      </c>
+      <c r="B453" s="4" t="s">
+        <v>1374</v>
+      </c>
+      <c r="D453" s="3" t="s">
+        <v>1373</v>
+      </c>
+    </row>
+    <row r="454" spans="1:4" ht="30">
+      <c r="A454" s="2" t="s">
+        <v>1369</v>
+      </c>
+      <c r="B454" s="4" t="s">
+        <v>1370</v>
+      </c>
+      <c r="D454" s="3" t="s">
+        <v>1371</v>
+      </c>
+    </row>
+    <row r="455" spans="1:4" ht="30">
+      <c r="A455" s="2" t="s">
+        <v>1365</v>
+      </c>
+      <c r="B455" s="4" t="s">
+        <v>1367</v>
+      </c>
+      <c r="D455" s="3" t="s">
+        <v>1368</v>
+      </c>
+    </row>
+    <row r="456" spans="1:4">
+      <c r="A456" s="2" t="s">
+        <v>1366</v>
+      </c>
+      <c r="D456" s="3" t="s">
+        <v>1351</v>
+      </c>
+    </row>
+    <row r="457" spans="1:4" ht="45">
+      <c r="A457" s="2" t="s">
+        <v>1362</v>
+      </c>
+      <c r="B457" s="4" t="s">
+        <v>1363</v>
+      </c>
+      <c r="D457" s="3" t="s">
+        <v>1364</v>
+      </c>
+    </row>
+    <row r="458" spans="1:4" ht="30">
+      <c r="A458" s="2" t="s">
+        <v>1359</v>
+      </c>
+      <c r="B458" s="4" t="s">
+        <v>1360</v>
+      </c>
+      <c r="D458" s="3" t="s">
+        <v>1361</v>
+      </c>
+    </row>
+    <row r="459" spans="1:4">
+      <c r="A459" s="2" t="s">
+        <v>1358</v>
+      </c>
+      <c r="B459" s="3" t="s">
+        <v>1357</v>
+      </c>
+      <c r="D459" s="3" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="460" spans="1:4" ht="45">
+      <c r="A460" s="2" t="s">
+        <v>1354</v>
+      </c>
+      <c r="B460" s="4" t="s">
+        <v>1355</v>
+      </c>
+      <c r="D460" s="3" t="s">
+        <v>1356</v>
+      </c>
+    </row>
+    <row r="461" spans="1:4" ht="45">
+      <c r="A461" s="2" t="s">
+        <v>1352</v>
+      </c>
+      <c r="B461" s="4" t="s">
+        <v>1353</v>
+      </c>
+      <c r="D461" s="3" t="s">
+        <v>1386</v>
+      </c>
+    </row>
+    <row r="462" spans="1:4" ht="75">
+      <c r="A462" s="2" t="s">
+        <v>1387</v>
+      </c>
+      <c r="B462" s="4" t="s">
+        <v>1388</v>
+      </c>
+      <c r="D462" s="3" t="s">
+        <v>1389</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
live fast die young
</commit_message>
<xml_diff>
--- a/abkuerzungen.xlsx
+++ b/abkuerzungen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\ストレージ\MarkDown\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42721FF5-4ADB-475B-9BB2-2BBC665902A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{381C6E8D-90C3-4227-A57C-803145CE5435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2310" yWindow="105" windowWidth="24225" windowHeight="15495" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2332" uniqueCount="1540">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2334" uniqueCount="1541">
   <si>
     <t>NAS</t>
   </si>
@@ -5172,6 +5172,9 @@
   </si>
   <si>
     <t>SSL</t>
+  </si>
+  <si>
+    <t>**** est un protocole réseau basé sur la suite de protocoles Internet pour la diffusion et la découverte de services de réseau et d'informations de présence. Il accomplit cette tâche sans l'aide de mécanismes de configuration basés sur le serveur, tels que le protocole DHCP (Dynamic Host Configuration Protocol) ou le DNS (Domain Name System), et sans configuration statique particulière d'un hôte de réseau.</t>
   </si>
 </sst>
 </file>
@@ -5371,7 +5374,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -5420,14 +5423,6 @@
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5821,8 +5816,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:XFD493"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A486" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A492" sqref="A492"/>
+    <sheetView tabSelected="1" topLeftCell="A463" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A469" sqref="A469"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="28.5"/>
@@ -12642,15 +12637,19 @@
       </c>
       <c r="F391" s="3"/>
     </row>
-    <row r="392" spans="1:6">
+    <row r="392" spans="1:6" ht="45">
       <c r="A392" s="18" t="s">
         <v>1051</v>
       </c>
       <c r="B392" s="17" t="s">
         <v>1052</v>
       </c>
-      <c r="C392" s="3"/>
-      <c r="D392" s="20"/>
+      <c r="C392" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="D392" s="20" t="s">
+        <v>1540</v>
+      </c>
       <c r="F392" s="3"/>
     </row>
     <row r="393" spans="1:6">
@@ -14239,98 +14238,92 @@
       <c r="F487" s="3"/>
     </row>
     <row r="488" spans="1:6" ht="30">
-      <c r="A488" s="25" t="s">
+      <c r="A488" s="17" t="s">
         <v>1525</v>
       </c>
-      <c r="B488" s="25" t="s">
+      <c r="B488" s="17" t="s">
         <v>1522</v>
       </c>
-      <c r="C488" s="26" t="s">
+      <c r="C488" s="3" t="s">
         <v>316</v>
       </c>
-      <c r="D488" s="27" t="s">
+      <c r="D488" s="20" t="s">
         <v>1523</v>
       </c>
-      <c r="E488" s="26"/>
-      <c r="F488" s="26"/>
+      <c r="F488" s="3"/>
     </row>
     <row r="489" spans="1:6" ht="33.75">
-      <c r="A489" s="24" t="s">
+      <c r="A489" s="18" t="s">
         <v>1524</v>
       </c>
-      <c r="B489" s="25" t="s">
+      <c r="B489" s="17" t="s">
         <v>1526</v>
       </c>
-      <c r="C489" s="26" t="s">
+      <c r="C489" s="3" t="s">
         <v>316</v>
       </c>
-      <c r="D489" s="27" t="s">
+      <c r="D489" s="20" t="s">
         <v>1527</v>
       </c>
-      <c r="E489" s="26"/>
-      <c r="F489" s="26"/>
+      <c r="F489" s="3"/>
     </row>
     <row r="490" spans="1:6">
-      <c r="A490" s="24" t="s">
+      <c r="A490" s="18" t="s">
         <v>1528</v>
       </c>
-      <c r="B490" s="25" t="s">
+      <c r="B490" s="17" t="s">
         <v>1533</v>
       </c>
-      <c r="C490" s="26" t="s">
+      <c r="C490" s="3" t="s">
         <v>316</v>
       </c>
-      <c r="D490" s="27" t="s">
+      <c r="D490" s="20" t="s">
         <v>1530</v>
       </c>
-      <c r="E490" s="26"/>
-      <c r="F490" s="26"/>
+      <c r="F490" s="3"/>
     </row>
     <row r="491" spans="1:6" ht="33.75">
-      <c r="A491" s="24" t="s">
+      <c r="A491" s="18" t="s">
         <v>1529</v>
       </c>
-      <c r="B491" s="25" t="s">
+      <c r="B491" s="17" t="s">
         <v>1532</v>
       </c>
-      <c r="C491" s="26" t="s">
+      <c r="C491" s="3" t="s">
         <v>316</v>
       </c>
-      <c r="D491" s="27" t="s">
+      <c r="D491" s="20" t="s">
         <v>1531</v>
       </c>
-      <c r="E491" s="26"/>
-      <c r="F491" s="26"/>
+      <c r="F491" s="3"/>
     </row>
     <row r="492" spans="1:6" ht="33.75">
-      <c r="A492" s="24" t="s">
+      <c r="A492" s="18" t="s">
         <v>1535</v>
       </c>
-      <c r="B492" s="25" t="s">
+      <c r="B492" s="17" t="s">
         <v>1536</v>
       </c>
-      <c r="C492" s="26" t="s">
+      <c r="C492" s="3" t="s">
         <v>316</v>
       </c>
-      <c r="D492" s="27" t="s">
+      <c r="D492" s="20" t="s">
         <v>1534</v>
       </c>
-      <c r="E492" s="26"/>
-      <c r="F492" s="26"/>
+      <c r="F492" s="3"/>
     </row>
     <row r="493" spans="1:6">
-      <c r="A493" s="24" t="s">
+      <c r="A493" s="18" t="s">
         <v>1539</v>
       </c>
-      <c r="B493" s="25" t="s">
+      <c r="B493" s="17" t="s">
         <v>1537</v>
       </c>
-      <c r="C493" s="26"/>
-      <c r="D493" s="27" t="s">
+      <c r="C493" s="3"/>
+      <c r="D493" s="20" t="s">
         <v>1538</v>
       </c>
-      <c r="E493" s="26"/>
-      <c r="F493" s="26"/>
+      <c r="F493" s="3"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:D276">

</xml_diff>

<commit_message>
6 000 000 ways to die
</commit_message>
<xml_diff>
--- a/abkuerzungen.xlsx
+++ b/abkuerzungen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10514"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\ストレージ\MarkDown\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gregorio/Sites/markdown/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EBE266E-2ED5-4289-9C7B-C22098AB8FD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D0EC618-6994-6542-B57F-245C57AF4EC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2310" yWindow="105" windowWidth="24225" windowHeight="15495" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="52280" yWindow="500" windowWidth="29460" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2379" uniqueCount="1570">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2402" uniqueCount="1589">
   <si>
     <t>NAS</t>
   </si>
@@ -5259,12 +5259,70 @@
   <si>
     <t>port translation protocol</t>
   </si>
+  <si>
+    <t xml:space="preserve">avr </t>
+  </si>
+  <si>
+    <t>Automatic voltage regulator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">if avr immer VI  for usv
+A voltage regulator is a system designed to automatically maintain a constant voltage. A voltage regulator may use a simple feed-forward design or may include negative feedback. </t>
+  </si>
+  <si>
+    <t>CIFS</t>
+  </si>
+  <si>
+    <t>Common Internet File System</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XXXX  a protocol that gained popularity around the year 2000, as vendors worked to establish an Internet Protocol-based file-sharing protocol. </t>
+  </si>
+  <si>
+    <t>NFS</t>
+  </si>
+  <si>
+    <t>Network File System</t>
+  </si>
+  <si>
+    <t>***  is a distributed file system protocol originally developed by Sun Microsystems in 1984, allowing a user on a client computer to access files over a computer network much like local storage is accessed.</t>
+  </si>
+  <si>
+    <t>FC</t>
+  </si>
+  <si>
+    <t>Fibre Channel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bs </t>
+  </si>
+  <si>
+    <t>** is a high-speed data transfer protocol providing in-order, lossless delivery of raw block data. Fibre Channel is primarily used to connect computer data storage to servers in storage area networks in commercial data centers.</t>
+  </si>
+  <si>
+    <t>iSCSI</t>
+  </si>
+  <si>
+    <t>Internet Small Computer System Interface</t>
+  </si>
+  <si>
+    <t>***** an Internet Protocol-based storage networking standard for linking data storage facilities. iSCSI provides block-level access to storage devices by carrying SCSI commands over a TCP/IP network.</t>
+  </si>
+  <si>
+    <t>SAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> () hard drive is a type of hard disk drive that uses the SAS interface to connect to a computer system. SAS is a high-speed data transfer protocol that is designed for demanding enterprise storage environments.</t>
+  </si>
+  <si>
+    <t>Serial Attached SCSI</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="26">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5430,6 +5488,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1" tint="4.9989318521683403E-2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -5457,7 +5522,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -5506,6 +5571,9 @@
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -5514,9 +5582,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5628,8 +5694,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00096219-7411-470E-8817-26E819582D2F}" name="Table1" displayName="Table1" ref="A1:F507" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6" dataCellStyle="Normal">
-  <autoFilter ref="A1:F507" xr:uid="{00096219-7411-470E-8817-26E819582D2F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00096219-7411-470E-8817-26E819582D2F}" name="Table1" displayName="Table1" ref="A1:F513" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6" dataCellStyle="Normal">
+  <autoFilter ref="A1:F513" xr:uid="{00096219-7411-470E-8817-26E819582D2F}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F475">
     <sortCondition ref="A1:A475"/>
   </sortState>
@@ -5908,23 +5974,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:XFD507"/>
+  <dimension ref="A1:XFD513"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A497" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D507" sqref="D507"/>
+    <sheetView tabSelected="1" topLeftCell="A498" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D512" sqref="D512"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="28.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="29" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.42578125" style="13" customWidth="1"/>
-    <col min="2" max="2" width="31.42578125" style="14" customWidth="1"/>
-    <col min="3" max="3" width="8.28515625" style="15" customWidth="1"/>
-    <col min="4" max="4" width="78.140625" style="16" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" style="3"/>
-    <col min="6" max="6" width="58.85546875" style="12" customWidth="1"/>
+    <col min="1" max="1" width="23.5" style="13" customWidth="1"/>
+    <col min="2" max="2" width="31.5" style="14" customWidth="1"/>
+    <col min="3" max="3" width="8.33203125" style="15" customWidth="1"/>
+    <col min="4" max="4" width="78.1640625" style="16" customWidth="1"/>
+    <col min="5" max="5" width="11.5" style="3"/>
+    <col min="6" max="6" width="58.83203125" style="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="27.75">
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>39</v>
       </c>
@@ -5944,7 +6010,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="2" customFormat="1">
+    <row r="2" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
         <v>1099</v>
       </c>
@@ -5958,7 +6024,7 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:6" s="2" customFormat="1">
+    <row r="3" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="18" t="s">
         <v>1099</v>
       </c>
@@ -5972,7 +6038,7 @@
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="18" t="s">
         <v>1099</v>
       </c>
@@ -5985,7 +6051,7 @@
       </c>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="1:6" s="2" customFormat="1">
+    <row r="5" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="18" t="s">
         <v>1098</v>
       </c>
@@ -5999,7 +6065,7 @@
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
     </row>
-    <row r="6" spans="1:6" s="2" customFormat="1">
+    <row r="6" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="18" t="s">
         <v>1102</v>
       </c>
@@ -6013,7 +6079,7 @@
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" spans="1:6" s="2" customFormat="1">
+    <row r="7" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="18" t="s">
         <v>1104</v>
       </c>
@@ -6027,7 +6093,7 @@
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
     </row>
-    <row r="8" spans="1:6" s="2" customFormat="1">
+    <row r="8" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="18" t="s">
         <v>1105</v>
       </c>
@@ -6041,7 +6107,7 @@
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
     </row>
-    <row r="9" spans="1:6" s="2" customFormat="1">
+    <row r="9" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="18" t="s">
         <v>1110</v>
       </c>
@@ -6055,7 +6121,7 @@
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
     </row>
-    <row r="10" spans="1:6" s="2" customFormat="1">
+    <row r="10" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="18" t="s">
         <v>1113</v>
       </c>
@@ -6069,7 +6135,7 @@
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
     </row>
-    <row r="11" spans="1:6" s="2" customFormat="1">
+    <row r="11" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="18" t="s">
         <v>1117</v>
       </c>
@@ -6083,7 +6149,7 @@
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
     </row>
-    <row r="12" spans="1:6" s="2" customFormat="1">
+    <row r="12" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="18" t="s">
         <v>1119</v>
       </c>
@@ -6097,7 +6163,7 @@
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
     </row>
-    <row r="13" spans="1:6" s="2" customFormat="1">
+    <row r="13" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="18" t="s">
         <v>1122</v>
       </c>
@@ -6111,7 +6177,7 @@
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
     </row>
-    <row r="14" spans="1:6" s="2" customFormat="1">
+    <row r="14" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="18" t="s">
         <v>1123</v>
       </c>
@@ -6125,7 +6191,7 @@
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
     </row>
-    <row r="15" spans="1:6" s="2" customFormat="1">
+    <row r="15" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="18" t="s">
         <v>1130</v>
       </c>
@@ -6139,7 +6205,7 @@
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
     </row>
-    <row r="16" spans="1:6" s="2" customFormat="1">
+    <row r="16" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="18" t="s">
         <v>1129</v>
       </c>
@@ -6153,7 +6219,7 @@
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
     </row>
-    <row r="17" spans="1:6" s="2" customFormat="1" ht="33.75">
+    <row r="17" spans="1:6" s="2" customFormat="1" ht="36" x14ac:dyDescent="0.35">
       <c r="A17" s="18" t="s">
         <v>264</v>
       </c>
@@ -6171,7 +6237,7 @@
       </c>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="1:6" s="2" customFormat="1">
+    <row r="18" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="18" t="s">
         <v>265</v>
       </c>
@@ -6187,7 +6253,7 @@
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
     </row>
-    <row r="19" spans="1:6" s="2" customFormat="1">
+    <row r="19" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="18" t="s">
         <v>263</v>
       </c>
@@ -6203,7 +6269,7 @@
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
     </row>
-    <row r="20" spans="1:6" s="3" customFormat="1">
+    <row r="20" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="18" t="s">
         <v>274</v>
       </c>
@@ -6213,7 +6279,7 @@
       </c>
       <c r="D20" s="20"/>
     </row>
-    <row r="21" spans="1:6" s="2" customFormat="1" ht="33">
+    <row r="21" spans="1:6" s="2" customFormat="1" ht="35" x14ac:dyDescent="0.35">
       <c r="A21" s="18" t="s">
         <v>1335</v>
       </c>
@@ -6231,7 +6297,7 @@
       </c>
       <c r="F21" s="3"/>
     </row>
-    <row r="22" spans="1:6" s="2" customFormat="1">
+    <row r="22" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="18" t="s">
         <v>1277</v>
       </c>
@@ -6247,7 +6313,7 @@
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
     </row>
-    <row r="23" spans="1:6" s="2" customFormat="1">
+    <row r="23" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="18" t="s">
         <v>879</v>
       </c>
@@ -6267,7 +6333,7 @@
         <v>884</v>
       </c>
     </row>
-    <row r="24" spans="1:6" s="2" customFormat="1" ht="33">
+    <row r="24" spans="1:6" s="2" customFormat="1" ht="35" x14ac:dyDescent="0.35">
       <c r="A24" s="18" t="s">
         <v>398</v>
       </c>
@@ -6287,7 +6353,7 @@
         <v>928</v>
       </c>
     </row>
-    <row r="25" spans="1:6" s="2" customFormat="1" ht="33">
+    <row r="25" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" s="18" t="s">
         <v>80</v>
       </c>
@@ -6305,7 +6371,7 @@
         <v>929</v>
       </c>
     </row>
-    <row r="26" spans="1:6" s="2" customFormat="1">
+    <row r="26" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="18" t="s">
         <v>272</v>
       </c>
@@ -6319,7 +6385,7 @@
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
     </row>
-    <row r="27" spans="1:6" s="2" customFormat="1">
+    <row r="27" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A27" s="18" t="s">
         <v>1243</v>
       </c>
@@ -6339,7 +6405,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="28" spans="1:6" s="2" customFormat="1">
+    <row r="28" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A28" s="18" t="s">
         <v>1313</v>
       </c>
@@ -6357,7 +6423,7 @@
       </c>
       <c r="F28" s="3"/>
     </row>
-    <row r="29" spans="1:6" s="2" customFormat="1">
+    <row r="29" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A29" s="18" t="s">
         <v>853</v>
       </c>
@@ -6377,7 +6443,7 @@
         <v>892</v>
       </c>
     </row>
-    <row r="30" spans="1:6" s="2" customFormat="1" ht="33">
+    <row r="30" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A30" s="18" t="s">
         <v>392</v>
       </c>
@@ -6397,7 +6463,7 @@
         <v>931</v>
       </c>
     </row>
-    <row r="31" spans="1:6" s="2" customFormat="1">
+    <row r="31" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A31" s="18" t="s">
         <v>1192</v>
       </c>
@@ -6415,7 +6481,7 @@
       </c>
       <c r="F31" s="3"/>
     </row>
-    <row r="32" spans="1:6" s="2" customFormat="1">
+    <row r="32" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A32" s="18" t="s">
         <v>1089</v>
       </c>
@@ -6431,7 +6497,7 @@
       </c>
       <c r="F32" s="3"/>
     </row>
-    <row r="33" spans="1:6" s="4" customFormat="1">
+    <row r="33" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A33" s="18" t="s">
         <v>107</v>
       </c>
@@ -6451,7 +6517,7 @@
         <v>932</v>
       </c>
     </row>
-    <row r="34" spans="1:6" s="2" customFormat="1">
+    <row r="34" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A34" s="18" t="s">
         <v>1344</v>
       </c>
@@ -6471,7 +6537,7 @@
         <v>933</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" s="18" t="s">
         <v>187</v>
       </c>
@@ -6489,7 +6555,7 @@
         <v>934</v>
       </c>
     </row>
-    <row r="36" spans="1:6" s="2" customFormat="1" ht="33">
+    <row r="36" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A36" s="18" t="s">
         <v>346</v>
       </c>
@@ -6509,7 +6575,7 @@
         <v>935</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="18" t="s">
         <v>255</v>
       </c>
@@ -6529,7 +6595,7 @@
         <v>936</v>
       </c>
     </row>
-    <row r="38" spans="1:6" s="2" customFormat="1" ht="56.25">
+    <row r="38" spans="1:6" s="2" customFormat="1" ht="48" x14ac:dyDescent="0.35">
       <c r="A38" s="18" t="s">
         <v>224</v>
       </c>
@@ -6549,7 +6615,7 @@
         <v>937</v>
       </c>
     </row>
-    <row r="39" spans="1:6" s="2" customFormat="1" ht="33.75">
+    <row r="39" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A39" s="18" t="s">
         <v>1053</v>
       </c>
@@ -6567,7 +6633,7 @@
       </c>
       <c r="F39" s="3"/>
     </row>
-    <row r="40" spans="1:6" s="2" customFormat="1">
+    <row r="40" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A40" s="18" t="s">
         <v>534</v>
       </c>
@@ -6587,7 +6653,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="41" spans="1:6" s="2" customFormat="1">
+    <row r="41" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A41" s="18" t="s">
         <v>482</v>
       </c>
@@ -6607,7 +6673,7 @@
         <v>940</v>
       </c>
     </row>
-    <row r="42" spans="1:6" s="2" customFormat="1">
+    <row r="42" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A42" s="18" t="s">
         <v>25</v>
       </c>
@@ -6623,7 +6689,7 @@
         <v>941</v>
       </c>
     </row>
-    <row r="43" spans="1:6" s="2" customFormat="1" ht="33">
+    <row r="43" spans="1:6" s="2" customFormat="1" ht="35" x14ac:dyDescent="0.35">
       <c r="A43" s="18" t="s">
         <v>22</v>
       </c>
@@ -6643,7 +6709,7 @@
         <v>938</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="33">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44" s="18" t="s">
         <v>470</v>
       </c>
@@ -6663,7 +6729,7 @@
         <v>942</v>
       </c>
     </row>
-    <row r="45" spans="1:6" s="2" customFormat="1">
+    <row r="45" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A45" s="18" t="s">
         <v>53</v>
       </c>
@@ -6683,7 +6749,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="46" spans="1:6" s="2" customFormat="1">
+    <row r="46" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A46" s="18" t="s">
         <v>552</v>
       </c>
@@ -6703,7 +6769,7 @@
         <v>944</v>
       </c>
     </row>
-    <row r="47" spans="1:6" s="2" customFormat="1">
+    <row r="47" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A47" s="18" t="s">
         <v>764</v>
       </c>
@@ -6721,7 +6787,7 @@
       </c>
       <c r="F47" s="3"/>
     </row>
-    <row r="48" spans="1:6" s="2" customFormat="1">
+    <row r="48" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A48" s="18" t="s">
         <v>765</v>
       </c>
@@ -6739,7 +6805,7 @@
       </c>
       <c r="F48" s="3"/>
     </row>
-    <row r="49" spans="1:6" s="2" customFormat="1">
+    <row r="49" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A49" s="18" t="s">
         <v>393</v>
       </c>
@@ -6759,7 +6825,7 @@
         <v>945</v>
       </c>
     </row>
-    <row r="50" spans="1:6" s="2" customFormat="1">
+    <row r="50" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A50" s="18" t="s">
         <v>1347</v>
       </c>
@@ -6779,7 +6845,7 @@
         <v>946</v>
       </c>
     </row>
-    <row r="51" spans="1:6" s="2" customFormat="1" ht="33.75">
+    <row r="51" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A51" s="18" t="s">
         <v>1238</v>
       </c>
@@ -6795,7 +6861,7 @@
       <c r="E51" s="3"/>
       <c r="F51" s="3"/>
     </row>
-    <row r="52" spans="1:6" s="2" customFormat="1">
+    <row r="52" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A52" s="18" t="s">
         <v>1179</v>
       </c>
@@ -6811,7 +6877,7 @@
       </c>
       <c r="F52" s="3"/>
     </row>
-    <row r="53" spans="1:6" s="2" customFormat="1">
+    <row r="53" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A53" s="18" t="s">
         <v>1195</v>
       </c>
@@ -6827,7 +6893,7 @@
       <c r="E53" s="3"/>
       <c r="F53" s="3"/>
     </row>
-    <row r="54" spans="1:6" s="2" customFormat="1">
+    <row r="54" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A54" s="18" t="s">
         <v>549</v>
       </c>
@@ -6847,7 +6913,7 @@
         <v>947</v>
       </c>
     </row>
-    <row r="55" spans="1:6" s="2" customFormat="1">
+    <row r="55" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A55" s="18" t="s">
         <v>1348</v>
       </c>
@@ -6867,7 +6933,7 @@
         <v>948</v>
       </c>
     </row>
-    <row r="56" spans="1:6" s="2" customFormat="1" ht="33.75">
+    <row r="56" spans="1:6" s="2" customFormat="1" ht="36" x14ac:dyDescent="0.35">
       <c r="A56" s="18" t="s">
         <v>369</v>
       </c>
@@ -6887,7 +6953,7 @@
         <v>948</v>
       </c>
     </row>
-    <row r="57" spans="1:6" s="2" customFormat="1" ht="33.75">
+    <row r="57" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A57" s="18" t="s">
         <v>1158</v>
       </c>
@@ -6905,7 +6971,7 @@
       </c>
       <c r="F57" s="3"/>
     </row>
-    <row r="58" spans="1:6" s="2" customFormat="1">
+    <row r="58" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A58" s="18" t="s">
         <v>410</v>
       </c>
@@ -6923,7 +6989,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="59" spans="1:6" s="2" customFormat="1" ht="33">
+    <row r="59" spans="1:6" s="2" customFormat="1" ht="35" x14ac:dyDescent="0.35">
       <c r="A59" s="18" t="s">
         <v>1190</v>
       </c>
@@ -6939,7 +7005,7 @@
       </c>
       <c r="F59" s="3"/>
     </row>
-    <row r="60" spans="1:6" s="2" customFormat="1" ht="48">
+    <row r="60" spans="1:6" s="2" customFormat="1" ht="35" x14ac:dyDescent="0.35">
       <c r="A60" s="18" t="s">
         <v>1184</v>
       </c>
@@ -6953,7 +7019,7 @@
       </c>
       <c r="F60" s="3"/>
     </row>
-    <row r="61" spans="1:6" s="2" customFormat="1" ht="33.75">
+    <row r="61" spans="1:6" s="2" customFormat="1" ht="35" x14ac:dyDescent="0.35">
       <c r="A61" s="18" t="s">
         <v>1072</v>
       </c>
@@ -6969,7 +7035,7 @@
       </c>
       <c r="F61" s="3"/>
     </row>
-    <row r="62" spans="1:6" s="2" customFormat="1">
+    <row r="62" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A62" s="18" t="s">
         <v>555</v>
       </c>
@@ -6989,7 +7055,7 @@
         <v>949</v>
       </c>
     </row>
-    <row r="63" spans="1:6" s="2" customFormat="1" ht="45">
+    <row r="63" spans="1:6" s="2" customFormat="1" ht="48" x14ac:dyDescent="0.35">
       <c r="A63" s="18" t="s">
         <v>359</v>
       </c>
@@ -7009,7 +7075,7 @@
         <v>951</v>
       </c>
     </row>
-    <row r="64" spans="1:6" s="2" customFormat="1" ht="33.75">
+    <row r="64" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A64" s="18" t="s">
         <v>539</v>
       </c>
@@ -7029,7 +7095,7 @@
         <v>952</v>
       </c>
     </row>
-    <row r="65" spans="1:6" s="2" customFormat="1">
+    <row r="65" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A65" s="18" t="s">
         <v>1288</v>
       </c>
@@ -7047,7 +7113,7 @@
       </c>
       <c r="F65" s="3"/>
     </row>
-    <row r="66" spans="1:6" s="2" customFormat="1">
+    <row r="66" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A66" s="18" t="s">
         <v>1019</v>
       </c>
@@ -7063,7 +7129,7 @@
       <c r="E66" s="3"/>
       <c r="F66" s="3"/>
     </row>
-    <row r="67" spans="1:6" s="2" customFormat="1">
+    <row r="67" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A67" s="18" t="s">
         <v>796</v>
       </c>
@@ -7081,7 +7147,7 @@
       </c>
       <c r="F67" s="3"/>
     </row>
-    <row r="68" spans="1:6" s="2" customFormat="1">
+    <row r="68" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A68" s="18" t="s">
         <v>246</v>
       </c>
@@ -7101,7 +7167,7 @@
         <v>953</v>
       </c>
     </row>
-    <row r="69" spans="1:6">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A69" s="18" t="s">
         <v>1289</v>
       </c>
@@ -7116,7 +7182,7 @@
       </c>
       <c r="F69" s="3"/>
     </row>
-    <row r="70" spans="1:6" s="2" customFormat="1" ht="33.75">
+    <row r="70" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A70" s="18" t="s">
         <v>109</v>
       </c>
@@ -7136,7 +7202,7 @@
         <v>954</v>
       </c>
     </row>
-    <row r="71" spans="1:6" s="2" customFormat="1">
+    <row r="71" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A71" s="18" t="s">
         <v>565</v>
       </c>
@@ -7156,7 +7222,7 @@
         <v>952</v>
       </c>
     </row>
-    <row r="72" spans="1:6" s="2" customFormat="1">
+    <row r="72" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A72" s="18" t="s">
         <v>828</v>
       </c>
@@ -7172,7 +7238,7 @@
       </c>
       <c r="F72" s="3"/>
     </row>
-    <row r="73" spans="1:6" s="2" customFormat="1" ht="33.75">
+    <row r="73" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A73" s="18" t="s">
         <v>1226</v>
       </c>
@@ -7190,7 +7256,7 @@
       </c>
       <c r="F73" s="3"/>
     </row>
-    <row r="74" spans="1:6" s="2" customFormat="1" ht="33.75">
+    <row r="74" spans="1:6" s="2" customFormat="1" ht="35" x14ac:dyDescent="0.35">
       <c r="A74" s="18" t="s">
         <v>1378</v>
       </c>
@@ -7210,7 +7276,7 @@
         <v>955</v>
       </c>
     </row>
-    <row r="75" spans="1:6" s="2" customFormat="1" ht="33.75">
+    <row r="75" spans="1:6" s="2" customFormat="1" ht="36" x14ac:dyDescent="0.35">
       <c r="A75" s="18" t="s">
         <v>1042</v>
       </c>
@@ -7226,7 +7292,7 @@
       </c>
       <c r="F75" s="3"/>
     </row>
-    <row r="76" spans="1:6" s="2" customFormat="1">
+    <row r="76" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A76" s="18" t="s">
         <v>456</v>
       </c>
@@ -7246,7 +7312,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="77" spans="1:6" s="2" customFormat="1" ht="45">
+    <row r="77" spans="1:6" s="2" customFormat="1" ht="48" x14ac:dyDescent="0.35">
       <c r="A77" s="18" t="s">
         <v>811</v>
       </c>
@@ -7262,7 +7328,7 @@
       </c>
       <c r="F77" s="3"/>
     </row>
-    <row r="78" spans="1:6" s="2" customFormat="1">
+    <row r="78" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A78" s="18" t="s">
         <v>441</v>
       </c>
@@ -7280,7 +7346,7 @@
       </c>
       <c r="F78" s="3"/>
     </row>
-    <row r="79" spans="1:6">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A79" s="18" t="s">
         <v>396</v>
       </c>
@@ -7297,7 +7363,7 @@
         <v>957</v>
       </c>
     </row>
-    <row r="80" spans="1:6" s="2" customFormat="1" ht="33.75">
+    <row r="80" spans="1:6" s="2" customFormat="1" ht="35" x14ac:dyDescent="0.35">
       <c r="A80" s="18" t="s">
         <v>101</v>
       </c>
@@ -7317,7 +7383,7 @@
         <v>958</v>
       </c>
     </row>
-    <row r="81" spans="1:6" ht="33.75">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A81" s="18" t="s">
         <v>755</v>
       </c>
@@ -7335,7 +7401,7 @@
       </c>
       <c r="F81" s="3"/>
     </row>
-    <row r="82" spans="1:6" s="2" customFormat="1">
+    <row r="82" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A82" s="18" t="s">
         <v>357</v>
       </c>
@@ -7353,7 +7419,7 @@
         <v>959</v>
       </c>
     </row>
-    <row r="83" spans="1:6">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A83" s="18" t="s">
         <v>1169</v>
       </c>
@@ -7369,7 +7435,7 @@
       </c>
       <c r="F83" s="3"/>
     </row>
-    <row r="84" spans="1:6" s="2" customFormat="1" ht="33.75">
+    <row r="84" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A84" s="18" t="s">
         <v>381</v>
       </c>
@@ -7389,7 +7455,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="85" spans="1:6" ht="33">
+    <row r="85" spans="1:6" ht="35" x14ac:dyDescent="0.35">
       <c r="A85" s="18" t="s">
         <v>1352</v>
       </c>
@@ -7409,7 +7475,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="86" spans="1:6" s="2" customFormat="1" ht="33">
+    <row r="86" spans="1:6" s="2" customFormat="1" ht="35" x14ac:dyDescent="0.35">
       <c r="A86" s="18" t="s">
         <v>383</v>
       </c>
@@ -7429,7 +7495,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="87" spans="1:6" s="2" customFormat="1">
+    <row r="87" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A87" s="18" t="s">
         <v>105</v>
       </c>
@@ -7449,7 +7515,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="88" spans="1:6" s="2" customFormat="1">
+    <row r="88" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A88" s="18" t="s">
         <v>75</v>
       </c>
@@ -7469,7 +7535,7 @@
         <v>962</v>
       </c>
     </row>
-    <row r="89" spans="1:6" s="2" customFormat="1">
+    <row r="89" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A89" s="18" t="s">
         <v>881</v>
       </c>
@@ -7489,7 +7555,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="90" spans="1:6" s="2" customFormat="1" ht="33.75">
+    <row r="90" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A90" s="18" t="s">
         <v>337</v>
       </c>
@@ -7509,7 +7575,7 @@
         <v>963</v>
       </c>
     </row>
-    <row r="91" spans="1:6" s="2" customFormat="1">
+    <row r="91" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A91" s="18" t="s">
         <v>1217</v>
       </c>
@@ -7527,7 +7593,7 @@
       </c>
       <c r="F91" s="3"/>
     </row>
-    <row r="92" spans="1:6" s="2" customFormat="1">
+    <row r="92" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A92" s="18" t="s">
         <v>210</v>
       </c>
@@ -7545,7 +7611,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="93" spans="1:6" s="2" customFormat="1">
+    <row r="93" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A93" s="18" t="s">
         <v>327</v>
       </c>
@@ -7565,7 +7631,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="94" spans="1:6" s="2" customFormat="1">
+    <row r="94" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A94" s="18" t="s">
         <v>1214</v>
       </c>
@@ -7583,7 +7649,7 @@
       </c>
       <c r="F94" s="3"/>
     </row>
-    <row r="95" spans="1:6" s="2" customFormat="1">
+    <row r="95" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A95" s="18" t="s">
         <v>1353</v>
       </c>
@@ -7603,7 +7669,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="96" spans="1:6" s="2" customFormat="1">
+    <row r="96" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A96" s="18" t="s">
         <v>90</v>
       </c>
@@ -7623,7 +7689,7 @@
         <v>967</v>
       </c>
     </row>
-    <row r="97" spans="1:6" s="2" customFormat="1">
+    <row r="97" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A97" s="18" t="s">
         <v>493</v>
       </c>
@@ -7643,7 +7709,7 @@
         <v>968</v>
       </c>
     </row>
-    <row r="98" spans="1:6" s="2" customFormat="1" ht="33">
+    <row r="98" spans="1:6" s="2" customFormat="1" ht="35" x14ac:dyDescent="0.35">
       <c r="A98" s="18" t="s">
         <v>485</v>
       </c>
@@ -7663,7 +7729,7 @@
         <v>970</v>
       </c>
     </row>
-    <row r="99" spans="1:6" s="2" customFormat="1">
+    <row r="99" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A99" s="18" t="s">
         <v>1212</v>
       </c>
@@ -7681,7 +7747,7 @@
       </c>
       <c r="F99" s="3"/>
     </row>
-    <row r="100" spans="1:6" s="2" customFormat="1" ht="33.75">
+    <row r="100" spans="1:6" s="2" customFormat="1" ht="35" x14ac:dyDescent="0.35">
       <c r="A100" s="18" t="s">
         <v>232</v>
       </c>
@@ -7701,7 +7767,7 @@
         <v>971</v>
       </c>
     </row>
-    <row r="101" spans="1:6" s="2" customFormat="1" ht="48">
+    <row r="101" spans="1:6" s="2" customFormat="1" ht="35" x14ac:dyDescent="0.35">
       <c r="A101" s="18" t="s">
         <v>2</v>
       </c>
@@ -7721,7 +7787,7 @@
         <v>972</v>
       </c>
     </row>
-    <row r="102" spans="1:6" s="2" customFormat="1" ht="48">
+    <row r="102" spans="1:6" s="2" customFormat="1" ht="35" x14ac:dyDescent="0.35">
       <c r="A102" s="18" t="s">
         <v>1408</v>
       </c>
@@ -7739,7 +7805,7 @@
       </c>
       <c r="F102" s="3"/>
     </row>
-    <row r="103" spans="1:6" s="2" customFormat="1" ht="33.75">
+    <row r="103" spans="1:6" s="2" customFormat="1" ht="36" x14ac:dyDescent="0.35">
       <c r="A103" s="18" t="s">
         <v>1407</v>
       </c>
@@ -7755,7 +7821,7 @@
       <c r="E103" s="3"/>
       <c r="F103" s="3"/>
     </row>
-    <row r="104" spans="1:6" s="2" customFormat="1">
+    <row r="104" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A104" s="18" t="s">
         <v>1409</v>
       </c>
@@ -7769,7 +7835,7 @@
       <c r="E104" s="3"/>
       <c r="F104" s="3"/>
     </row>
-    <row r="105" spans="1:6" s="2" customFormat="1">
+    <row r="105" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A105" s="18" t="s">
         <v>476</v>
       </c>
@@ -7789,7 +7855,7 @@
         <v>973</v>
       </c>
     </row>
-    <row r="106" spans="1:6" s="2" customFormat="1">
+    <row r="106" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A106" s="18" t="s">
         <v>543</v>
       </c>
@@ -7809,7 +7875,7 @@
         <v>975</v>
       </c>
     </row>
-    <row r="107" spans="1:6" s="2" customFormat="1" ht="33">
+    <row r="107" spans="1:6" s="2" customFormat="1" ht="35" x14ac:dyDescent="0.35">
       <c r="A107" s="18" t="s">
         <v>1355</v>
       </c>
@@ -7829,7 +7895,7 @@
         <v>977</v>
       </c>
     </row>
-    <row r="108" spans="1:6" s="2" customFormat="1" ht="33">
+    <row r="108" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A108" s="18" t="s">
         <v>340</v>
       </c>
@@ -7849,7 +7915,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="109" spans="1:6">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A109" s="18" t="s">
         <v>1206</v>
       </c>
@@ -7867,7 +7933,7 @@
       </c>
       <c r="F109" s="3"/>
     </row>
-    <row r="110" spans="1:6" s="2" customFormat="1">
+    <row r="110" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A110" s="18" t="s">
         <v>275</v>
       </c>
@@ -7885,7 +7951,7 @@
       </c>
       <c r="F110" s="3"/>
     </row>
-    <row r="111" spans="1:6" ht="33.75">
+    <row r="111" spans="1:6" ht="36" x14ac:dyDescent="0.35">
       <c r="A111" s="18" t="s">
         <v>1066</v>
       </c>
@@ -7901,7 +7967,7 @@
       </c>
       <c r="F111" s="3"/>
     </row>
-    <row r="112" spans="1:6">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A112" s="18" t="s">
         <v>373</v>
       </c>
@@ -7921,7 +7987,7 @@
         <v>980</v>
       </c>
     </row>
-    <row r="113" spans="1:6">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A113" s="18" t="s">
         <v>92</v>
       </c>
@@ -7941,7 +8007,7 @@
         <v>981</v>
       </c>
     </row>
-    <row r="114" spans="1:6">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A114" s="18" t="s">
         <v>173</v>
       </c>
@@ -7961,7 +8027,7 @@
         <v>983</v>
       </c>
     </row>
-    <row r="115" spans="1:6" ht="33.75">
+    <row r="115" spans="1:6" ht="36" x14ac:dyDescent="0.35">
       <c r="A115" s="18" t="s">
         <v>807</v>
       </c>
@@ -7979,7 +8045,7 @@
       </c>
       <c r="F115" s="3"/>
     </row>
-    <row r="116" spans="1:6" ht="45">
+    <row r="116" spans="1:6" ht="48" x14ac:dyDescent="0.35">
       <c r="A116" s="18" t="s">
         <v>21</v>
       </c>
@@ -7999,7 +8065,7 @@
         <v>985</v>
       </c>
     </row>
-    <row r="117" spans="1:6" ht="33">
+    <row r="117" spans="1:6" ht="35" x14ac:dyDescent="0.35">
       <c r="A117" s="18" t="s">
         <v>249</v>
       </c>
@@ -8019,7 +8085,7 @@
         <v>986</v>
       </c>
     </row>
-    <row r="118" spans="1:6">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A118" s="18" t="s">
         <v>475</v>
       </c>
@@ -8039,7 +8105,7 @@
         <v>987</v>
       </c>
     </row>
-    <row r="119" spans="1:6">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A119" s="18" t="s">
         <v>94</v>
       </c>
@@ -8059,7 +8125,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="120" spans="1:6" ht="33.75">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A120" s="18" t="s">
         <v>379</v>
       </c>
@@ -8079,7 +8145,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="121" spans="1:6" ht="33.75">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A121" s="18" t="s">
         <v>320</v>
       </c>
@@ -8099,7 +8165,7 @@
         <v>991</v>
       </c>
     </row>
-    <row r="122" spans="1:6">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A122" s="18" t="s">
         <v>1028</v>
       </c>
@@ -8117,7 +8183,7 @@
       </c>
       <c r="F122" s="3"/>
     </row>
-    <row r="123" spans="1:6">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A123" s="18" t="s">
         <v>54</v>
       </c>
@@ -8137,7 +8203,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="124" spans="1:6">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A124" s="18" t="s">
         <v>78</v>
       </c>
@@ -8157,7 +8223,7 @@
         <v>993</v>
       </c>
     </row>
-    <row r="125" spans="1:6" ht="33.75">
+    <row r="125" spans="1:6" ht="35" x14ac:dyDescent="0.35">
       <c r="A125" s="18" t="s">
         <v>71</v>
       </c>
@@ -8177,7 +8243,7 @@
         <v>994</v>
       </c>
     </row>
-    <row r="126" spans="1:6" ht="33.75">
+    <row r="126" spans="1:6" ht="36" x14ac:dyDescent="0.35">
       <c r="A126" s="18" t="s">
         <v>1231</v>
       </c>
@@ -8192,7 +8258,7 @@
       </c>
       <c r="F126" s="3"/>
     </row>
-    <row r="127" spans="1:6">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A127" s="18" t="s">
         <v>871</v>
       </c>
@@ -8212,7 +8278,7 @@
         <v>876</v>
       </c>
     </row>
-    <row r="128" spans="1:6" ht="45">
+    <row r="128" spans="1:6" ht="48" x14ac:dyDescent="0.35">
       <c r="A128" s="18" t="s">
         <v>1050</v>
       </c>
@@ -8225,7 +8291,7 @@
       </c>
       <c r="F128" s="3"/>
     </row>
-    <row r="129" spans="1:6">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A129" s="18" t="s">
         <v>209</v>
       </c>
@@ -8238,7 +8304,7 @@
       <c r="D129" s="20"/>
       <c r="F129" s="3"/>
     </row>
-    <row r="130" spans="1:6" ht="33.75">
+    <row r="130" spans="1:6" ht="36" x14ac:dyDescent="0.35">
       <c r="A130" s="18" t="s">
         <v>153</v>
       </c>
@@ -8258,7 +8324,7 @@
         <v>995</v>
       </c>
     </row>
-    <row r="131" spans="1:6">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A131" s="18" t="s">
         <v>1065</v>
       </c>
@@ -8271,7 +8337,7 @@
       </c>
       <c r="F131" s="3"/>
     </row>
-    <row r="132" spans="1:6" ht="33.75">
+    <row r="132" spans="1:6" ht="36" x14ac:dyDescent="0.35">
       <c r="A132" s="18" t="s">
         <v>749</v>
       </c>
@@ -8289,7 +8355,7 @@
       </c>
       <c r="F132" s="3"/>
     </row>
-    <row r="133" spans="1:6" ht="33.75">
+    <row r="133" spans="1:6" ht="35" x14ac:dyDescent="0.35">
       <c r="A133" s="18" t="s">
         <v>491</v>
       </c>
@@ -8309,7 +8375,7 @@
         <v>996</v>
       </c>
     </row>
-    <row r="134" spans="1:6">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A134" s="18" t="s">
         <v>68</v>
       </c>
@@ -8329,7 +8395,7 @@
         <v>997</v>
       </c>
     </row>
-    <row r="135" spans="1:6">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A135" s="18" t="s">
         <v>62</v>
       </c>
@@ -8349,7 +8415,7 @@
         <v>998</v>
       </c>
     </row>
-    <row r="136" spans="1:6" ht="48">
+    <row r="136" spans="1:6" ht="36" x14ac:dyDescent="0.35">
       <c r="A136" s="18" t="s">
         <v>391</v>
       </c>
@@ -8369,7 +8435,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="137" spans="1:6" ht="33.75">
+    <row r="137" spans="1:6" ht="36" x14ac:dyDescent="0.35">
       <c r="A137" s="18" t="s">
         <v>600</v>
       </c>
@@ -8389,7 +8455,7 @@
         <v>1002</v>
       </c>
     </row>
-    <row r="138" spans="1:6" ht="48">
+    <row r="138" spans="1:6" ht="51" x14ac:dyDescent="0.35">
       <c r="A138" s="18" t="s">
         <v>344</v>
       </c>
@@ -8409,7 +8475,7 @@
         <v>1003</v>
       </c>
     </row>
-    <row r="139" spans="1:6" ht="33">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A139" s="18" t="s">
         <v>330</v>
       </c>
@@ -8429,7 +8495,7 @@
         <v>1004</v>
       </c>
     </row>
-    <row r="140" spans="1:6">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A140" s="18" t="s">
         <v>763</v>
       </c>
@@ -8447,7 +8513,7 @@
       </c>
       <c r="F140" s="3"/>
     </row>
-    <row r="141" spans="1:6">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A141" s="18" t="s">
         <v>183</v>
       </c>
@@ -8467,7 +8533,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="142" spans="1:6" ht="33">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A142" s="18" t="s">
         <v>349</v>
       </c>
@@ -8487,7 +8553,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="143" spans="1:6" ht="112.5">
+    <row r="143" spans="1:6" ht="108" x14ac:dyDescent="0.35">
       <c r="A143" s="18" t="s">
         <v>418</v>
       </c>
@@ -8507,7 +8573,7 @@
         <v>1006</v>
       </c>
     </row>
-    <row r="144" spans="1:6" ht="45">
+    <row r="144" spans="1:6" ht="48" x14ac:dyDescent="0.35">
       <c r="A144" s="18" t="s">
         <v>1049</v>
       </c>
@@ -8522,7 +8588,7 @@
       </c>
       <c r="F144" s="3"/>
     </row>
-    <row r="145" spans="1:6" ht="33.75">
+    <row r="145" spans="1:6" ht="35" x14ac:dyDescent="0.35">
       <c r="A145" s="18" t="s">
         <v>467</v>
       </c>
@@ -8542,7 +8608,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="146" spans="1:6">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A146" s="18" t="s">
         <v>1175</v>
       </c>
@@ -8555,7 +8621,7 @@
       </c>
       <c r="F146" s="3"/>
     </row>
-    <row r="147" spans="1:6" ht="33.75">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A147" s="18" t="s">
         <v>413</v>
       </c>
@@ -8575,7 +8641,7 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="148" spans="1:6" ht="33.75">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A148" s="18" t="s">
         <v>414</v>
       </c>
@@ -8592,7 +8658,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="149" spans="1:6" ht="45">
+    <row r="149" spans="1:6" ht="48" x14ac:dyDescent="0.35">
       <c r="A149" s="18" t="s">
         <v>331</v>
       </c>
@@ -8612,7 +8678,7 @@
         <v>1004</v>
       </c>
     </row>
-    <row r="150" spans="1:6" ht="33.75">
+    <row r="150" spans="1:6" ht="35" x14ac:dyDescent="0.35">
       <c r="A150" s="18" t="s">
         <v>1040</v>
       </c>
@@ -8625,7 +8691,7 @@
       </c>
       <c r="F150" s="3"/>
     </row>
-    <row r="151" spans="1:6">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A151" s="18" t="s">
         <v>426</v>
       </c>
@@ -8645,7 +8711,7 @@
         <v>1002</v>
       </c>
     </row>
-    <row r="152" spans="1:6" ht="33">
+    <row r="152" spans="1:6" ht="35" x14ac:dyDescent="0.35">
       <c r="A152" s="18" t="s">
         <v>261</v>
       </c>
@@ -8665,7 +8731,7 @@
         <v>1011</v>
       </c>
     </row>
-    <row r="153" spans="1:6" ht="33">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A153" s="18" t="s">
         <v>98</v>
       </c>
@@ -8685,7 +8751,7 @@
         <v>1012</v>
       </c>
     </row>
-    <row r="154" spans="1:6" ht="33.75">
+    <row r="154" spans="1:6" ht="36" x14ac:dyDescent="0.35">
       <c r="A154" s="18" t="s">
         <v>251</v>
       </c>
@@ -8705,7 +8771,7 @@
         <v>1013</v>
       </c>
     </row>
-    <row r="155" spans="1:6">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A155" s="18" t="s">
         <v>1069</v>
       </c>
@@ -8718,7 +8784,7 @@
       </c>
       <c r="F155" s="3"/>
     </row>
-    <row r="156" spans="1:6">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A156" s="18" t="s">
         <v>1070</v>
       </c>
@@ -8731,7 +8797,7 @@
       </c>
       <c r="F156" s="3"/>
     </row>
-    <row r="157" spans="1:6" ht="33.75">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A157" s="18" t="s">
         <v>1071</v>
       </c>
@@ -8744,7 +8810,7 @@
       </c>
       <c r="F157" s="3"/>
     </row>
-    <row r="158" spans="1:6">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A158" s="18" t="s">
         <v>317</v>
       </c>
@@ -8764,7 +8830,7 @@
         <v>1014</v>
       </c>
     </row>
-    <row r="159" spans="1:6">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A159" s="18" t="s">
         <v>52</v>
       </c>
@@ -8784,7 +8850,7 @@
         <v>1015</v>
       </c>
     </row>
-    <row r="160" spans="1:6">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A160" s="18" t="s">
         <v>1282</v>
       </c>
@@ -8799,7 +8865,7 @@
       </c>
       <c r="F160" s="3"/>
     </row>
-    <row r="161" spans="1:6">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A161" s="18" t="s">
         <v>1091</v>
       </c>
@@ -8812,7 +8878,7 @@
       </c>
       <c r="F161" s="3"/>
     </row>
-    <row r="162" spans="1:6">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A162" s="18" t="s">
         <v>478</v>
       </c>
@@ -8832,7 +8898,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="163" spans="1:6">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A163" s="18" t="s">
         <v>483</v>
       </c>
@@ -8850,7 +8916,7 @@
       </c>
       <c r="F163" s="3"/>
     </row>
-    <row r="164" spans="1:6" ht="33">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A164" s="18" t="s">
         <v>480</v>
       </c>
@@ -8868,7 +8934,7 @@
       </c>
       <c r="F164" s="3"/>
     </row>
-    <row r="165" spans="1:6">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A165" s="18" t="s">
         <v>844</v>
       </c>
@@ -8884,7 +8950,7 @@
       </c>
       <c r="F165" s="3"/>
     </row>
-    <row r="166" spans="1:6">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A166" s="18" t="s">
         <v>766</v>
       </c>
@@ -8902,7 +8968,7 @@
       </c>
       <c r="F166" s="3"/>
     </row>
-    <row r="167" spans="1:6" ht="33.75">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A167" s="18" t="s">
         <v>822</v>
       </c>
@@ -8915,7 +8981,7 @@
       </c>
       <c r="F167" s="3"/>
     </row>
-    <row r="168" spans="1:6">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A168" s="18" t="s">
         <v>433</v>
       </c>
@@ -8933,7 +8999,7 @@
       </c>
       <c r="F168" s="3"/>
     </row>
-    <row r="169" spans="1:6">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A169" s="18" t="s">
         <v>1170</v>
       </c>
@@ -8946,7 +9012,7 @@
       </c>
       <c r="F169" s="3"/>
     </row>
-    <row r="170" spans="1:6" ht="37.5">
+    <row r="170" spans="1:6" ht="40" x14ac:dyDescent="0.25">
       <c r="A170" s="21" t="s">
         <v>1461</v>
       </c>
@@ -8964,7 +9030,7 @@
       </c>
       <c r="F170" s="3"/>
     </row>
-    <row r="171" spans="1:6" ht="33.75">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A171" s="18" t="s">
         <v>435</v>
       </c>
@@ -8982,7 +9048,7 @@
       </c>
       <c r="F171" s="3"/>
     </row>
-    <row r="172" spans="1:6" ht="33.75">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A172" s="18" t="s">
         <v>33</v>
       </c>
@@ -9000,7 +9066,7 @@
       </c>
       <c r="F172" s="3"/>
     </row>
-    <row r="173" spans="1:6">
+    <row r="173" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A173" s="18" t="s">
         <v>145</v>
       </c>
@@ -9018,7 +9084,7 @@
       </c>
       <c r="F173" s="3"/>
     </row>
-    <row r="174" spans="1:6">
+    <row r="174" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A174" s="18" t="s">
         <v>143</v>
       </c>
@@ -9036,7 +9102,7 @@
       </c>
       <c r="F174" s="3"/>
     </row>
-    <row r="175" spans="1:6">
+    <row r="175" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A175" s="18" t="s">
         <v>147</v>
       </c>
@@ -9054,7 +9120,7 @@
       </c>
       <c r="F175" s="3"/>
     </row>
-    <row r="176" spans="1:6">
+    <row r="176" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A176" s="18" t="s">
         <v>84</v>
       </c>
@@ -9072,7 +9138,7 @@
       </c>
       <c r="F176" s="3"/>
     </row>
-    <row r="177" spans="1:6">
+    <row r="177" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A177" s="18" t="s">
         <v>141</v>
       </c>
@@ -9090,7 +9156,7 @@
       </c>
       <c r="F177" s="3"/>
     </row>
-    <row r="178" spans="1:6">
+    <row r="178" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A178" s="18" t="s">
         <v>8</v>
       </c>
@@ -9108,7 +9174,7 @@
       </c>
       <c r="F178" s="3"/>
     </row>
-    <row r="179" spans="1:6">
+    <row r="179" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A179" s="18" t="s">
         <v>278</v>
       </c>
@@ -9123,7 +9189,7 @@
       </c>
       <c r="F179" s="3"/>
     </row>
-    <row r="180" spans="1:6" ht="45">
+    <row r="180" spans="1:6" ht="36" x14ac:dyDescent="0.35">
       <c r="A180" s="18" t="s">
         <v>814</v>
       </c>
@@ -9139,7 +9205,7 @@
       </c>
       <c r="F180" s="3"/>
     </row>
-    <row r="181" spans="1:6">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A181" s="18" t="s">
         <v>497</v>
       </c>
@@ -9157,7 +9223,7 @@
       </c>
       <c r="F181" s="3"/>
     </row>
-    <row r="182" spans="1:6">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A182" s="18" t="s">
         <v>1168</v>
       </c>
@@ -9168,7 +9234,7 @@
       </c>
       <c r="F182" s="3"/>
     </row>
-    <row r="183" spans="1:6" ht="33.75">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A183" s="18" t="s">
         <v>1026</v>
       </c>
@@ -9183,7 +9249,7 @@
       </c>
       <c r="F183" s="3"/>
     </row>
-    <row r="184" spans="1:6">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A184" s="18" t="s">
         <v>800</v>
       </c>
@@ -9201,7 +9267,7 @@
       </c>
       <c r="F184" s="3"/>
     </row>
-    <row r="185" spans="1:6" ht="33.75">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A185" s="18" t="s">
         <v>354</v>
       </c>
@@ -9219,7 +9285,7 @@
       </c>
       <c r="F185" s="3"/>
     </row>
-    <row r="186" spans="1:6" ht="33.75">
+    <row r="186" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A186" s="18" t="s">
         <v>1139</v>
       </c>
@@ -9234,7 +9300,7 @@
       </c>
       <c r="F186" s="3"/>
     </row>
-    <row r="187" spans="1:6" ht="33">
+    <row r="187" spans="1:6" ht="35" x14ac:dyDescent="0.35">
       <c r="A187" s="18" t="s">
         <v>1030</v>
       </c>
@@ -9249,7 +9315,7 @@
       </c>
       <c r="F187" s="3"/>
     </row>
-    <row r="188" spans="1:6" ht="33.75">
+    <row r="188" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A188" s="18" t="s">
         <v>858</v>
       </c>
@@ -9269,7 +9335,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="189" spans="1:6">
+    <row r="189" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A189" s="18" t="s">
         <v>195</v>
       </c>
@@ -9282,7 +9348,7 @@
       </c>
       <c r="F189" s="3"/>
     </row>
-    <row r="190" spans="1:6" ht="33.75">
+    <row r="190" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A190" s="18" t="s">
         <v>167</v>
       </c>
@@ -9300,7 +9366,7 @@
       </c>
       <c r="F190" s="3"/>
     </row>
-    <row r="191" spans="1:6">
+    <row r="191" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A191" s="18" t="s">
         <v>472</v>
       </c>
@@ -9318,7 +9384,7 @@
       </c>
       <c r="F191" s="3"/>
     </row>
-    <row r="192" spans="1:6" ht="33.75">
+    <row r="192" spans="1:6" ht="36" x14ac:dyDescent="0.35">
       <c r="A192" s="18" t="s">
         <v>161</v>
       </c>
@@ -9336,7 +9402,7 @@
       </c>
       <c r="F192" s="3"/>
     </row>
-    <row r="193" spans="1:6">
+    <row r="193" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A193" s="18" t="s">
         <v>118</v>
       </c>
@@ -9351,7 +9417,7 @@
       </c>
       <c r="F193" s="3"/>
     </row>
-    <row r="194" spans="1:6">
+    <row r="194" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A194" s="18" t="s">
         <v>163</v>
       </c>
@@ -9369,7 +9435,7 @@
       </c>
       <c r="F194" s="3"/>
     </row>
-    <row r="195" spans="1:6">
+    <row r="195" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A195" s="18" t="s">
         <v>177</v>
       </c>
@@ -9387,7 +9453,7 @@
       </c>
       <c r="F195" s="3"/>
     </row>
-    <row r="196" spans="1:6" ht="33.75">
+    <row r="196" spans="1:6" ht="36" x14ac:dyDescent="0.35">
       <c r="A196" s="18" t="s">
         <v>1137</v>
       </c>
@@ -9402,7 +9468,7 @@
       </c>
       <c r="F196" s="3"/>
     </row>
-    <row r="197" spans="1:6" ht="33.75">
+    <row r="197" spans="1:6" ht="36" x14ac:dyDescent="0.35">
       <c r="A197" s="18" t="s">
         <v>20</v>
       </c>
@@ -9417,7 +9483,7 @@
       </c>
       <c r="F197" s="3"/>
     </row>
-    <row r="198" spans="1:6">
+    <row r="198" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A198" s="18" t="s">
         <v>1379</v>
       </c>
@@ -9435,7 +9501,7 @@
       </c>
       <c r="F198" s="3"/>
     </row>
-    <row r="199" spans="1:6" ht="33">
+    <row r="199" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A199" s="18" t="s">
         <v>1234</v>
       </c>
@@ -9450,7 +9516,7 @@
       </c>
       <c r="F199" s="3"/>
     </row>
-    <row r="200" spans="1:6" ht="33.75">
+    <row r="200" spans="1:6" ht="36" x14ac:dyDescent="0.35">
       <c r="A200" s="18" t="s">
         <v>874</v>
       </c>
@@ -9470,7 +9536,7 @@
         <v>878</v>
       </c>
     </row>
-    <row r="201" spans="1:6">
+    <row r="201" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A201" s="18" t="s">
         <v>563</v>
       </c>
@@ -9485,7 +9551,7 @@
       </c>
       <c r="F201" s="3"/>
     </row>
-    <row r="202" spans="1:6" ht="33.75">
+    <row r="202" spans="1:6" ht="36" x14ac:dyDescent="0.35">
       <c r="A202" s="18" t="s">
         <v>228</v>
       </c>
@@ -9503,7 +9569,7 @@
       </c>
       <c r="F202" s="3"/>
     </row>
-    <row r="203" spans="1:6" ht="33">
+    <row r="203" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A203" s="18" t="s">
         <v>132</v>
       </c>
@@ -9521,7 +9587,7 @@
       </c>
       <c r="F203" s="3"/>
     </row>
-    <row r="204" spans="1:6">
+    <row r="204" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A204" s="18" t="s">
         <v>136</v>
       </c>
@@ -9539,7 +9605,7 @@
       </c>
       <c r="F204" s="3"/>
     </row>
-    <row r="205" spans="1:6">
+    <row r="205" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A205" s="18" t="s">
         <v>134</v>
       </c>
@@ -9557,7 +9623,7 @@
       </c>
       <c r="F205" s="3"/>
     </row>
-    <row r="206" spans="1:6" ht="33.75">
+    <row r="206" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A206" s="18" t="s">
         <v>440</v>
       </c>
@@ -9575,7 +9641,7 @@
       </c>
       <c r="F206" s="3"/>
     </row>
-    <row r="207" spans="1:6">
+    <row r="207" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A207" s="18" t="s">
         <v>11</v>
       </c>
@@ -9593,7 +9659,7 @@
       </c>
       <c r="F207" s="3"/>
     </row>
-    <row r="208" spans="1:6">
+    <row r="208" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A208" s="18" t="s">
         <v>280</v>
       </c>
@@ -9608,7 +9674,7 @@
       </c>
       <c r="F208" s="3"/>
     </row>
-    <row r="209" spans="1:6">
+    <row r="209" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A209" s="18" t="s">
         <v>253</v>
       </c>
@@ -9621,7 +9687,7 @@
       <c r="D209" s="20"/>
       <c r="F209" s="3"/>
     </row>
-    <row r="210" spans="1:6">
+    <row r="210" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A210" s="18" t="s">
         <v>540</v>
       </c>
@@ -9639,7 +9705,7 @@
       </c>
       <c r="F210" s="3"/>
     </row>
-    <row r="211" spans="1:6" ht="33.75">
+    <row r="211" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A211" s="18" t="s">
         <v>17</v>
       </c>
@@ -9657,7 +9723,7 @@
       </c>
       <c r="F211" s="3"/>
     </row>
-    <row r="212" spans="1:6">
+    <row r="212" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A212" s="18" t="s">
         <v>408</v>
       </c>
@@ -9675,7 +9741,7 @@
       </c>
       <c r="F212" s="3"/>
     </row>
-    <row r="213" spans="1:6" ht="33">
+    <row r="213" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A213" s="18" t="s">
         <v>428</v>
       </c>
@@ -9693,7 +9759,7 @@
       </c>
       <c r="F213" s="3"/>
     </row>
-    <row r="214" spans="1:6">
+    <row r="214" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A214" s="18" t="s">
         <v>26</v>
       </c>
@@ -9711,7 +9777,7 @@
       </c>
       <c r="F214" s="3"/>
     </row>
-    <row r="215" spans="1:6" ht="33">
+    <row r="215" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A215" s="18" t="s">
         <v>238</v>
       </c>
@@ -9729,7 +9795,7 @@
       </c>
       <c r="F215" s="3"/>
     </row>
-    <row r="216" spans="1:6" ht="33.75">
+    <row r="216" spans="1:6" ht="35" x14ac:dyDescent="0.35">
       <c r="A216" s="18" t="s">
         <v>220</v>
       </c>
@@ -9747,7 +9813,7 @@
       </c>
       <c r="F216" s="3"/>
     </row>
-    <row r="217" spans="1:6">
+    <row r="217" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A217" s="18" t="s">
         <v>69</v>
       </c>
@@ -9765,7 +9831,7 @@
       </c>
       <c r="F217" s="3"/>
     </row>
-    <row r="218" spans="1:6" ht="45">
+    <row r="218" spans="1:6" ht="36" x14ac:dyDescent="0.25">
       <c r="A218" s="22" t="s">
         <v>1360</v>
       </c>
@@ -9783,7 +9849,7 @@
       </c>
       <c r="F218" s="3"/>
     </row>
-    <row r="219" spans="1:6" ht="33">
+    <row r="219" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A219" s="18" t="s">
         <v>465</v>
       </c>
@@ -9801,7 +9867,7 @@
       </c>
       <c r="F219" s="3"/>
     </row>
-    <row r="220" spans="1:6">
+    <row r="220" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A220" s="18" t="s">
         <v>1488</v>
       </c>
@@ -9816,7 +9882,7 @@
       </c>
       <c r="F220" s="3"/>
     </row>
-    <row r="221" spans="1:6">
+    <row r="221" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A221" s="18" t="s">
         <v>1057</v>
       </c>
@@ -9831,7 +9897,7 @@
       </c>
       <c r="F221" s="3"/>
     </row>
-    <row r="222" spans="1:6" ht="45">
+    <row r="222" spans="1:6" ht="48" x14ac:dyDescent="0.35">
       <c r="A222" s="18" t="s">
         <v>458</v>
       </c>
@@ -9849,7 +9915,7 @@
       </c>
       <c r="F222" s="3"/>
     </row>
-    <row r="223" spans="1:6" ht="33.75">
+    <row r="223" spans="1:6" ht="36" x14ac:dyDescent="0.35">
       <c r="A223" s="18" t="s">
         <v>430</v>
       </c>
@@ -9867,7 +9933,7 @@
       </c>
       <c r="F223" s="3"/>
     </row>
-    <row r="224" spans="1:6" ht="33.75">
+    <row r="224" spans="1:6" ht="36" x14ac:dyDescent="0.3">
       <c r="A224" s="23" t="s">
         <v>194</v>
       </c>
@@ -9885,7 +9951,7 @@
       </c>
       <c r="F224" s="3"/>
     </row>
-    <row r="225" spans="1:6">
+    <row r="225" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A225" s="18" t="s">
         <v>188</v>
       </c>
@@ -9903,7 +9969,7 @@
       </c>
       <c r="F225" s="3"/>
     </row>
-    <row r="226" spans="1:6">
+    <row r="226" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A226" s="18" t="s">
         <v>12</v>
       </c>
@@ -9918,7 +9984,7 @@
       </c>
       <c r="F226" s="3"/>
     </row>
-    <row r="227" spans="1:6" ht="33.75">
+    <row r="227" spans="1:6" ht="36" x14ac:dyDescent="0.35">
       <c r="A227" s="18" t="s">
         <v>351</v>
       </c>
@@ -9936,7 +10002,7 @@
       </c>
       <c r="F227" s="3"/>
     </row>
-    <row r="228" spans="1:6">
+    <row r="228" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A228" s="18" t="s">
         <v>99</v>
       </c>
@@ -9954,7 +10020,7 @@
       </c>
       <c r="F228" s="3"/>
     </row>
-    <row r="229" spans="1:6" ht="33.75">
+    <row r="229" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A229" s="18" t="s">
         <v>151</v>
       </c>
@@ -9972,7 +10038,7 @@
       </c>
       <c r="F229" s="3"/>
     </row>
-    <row r="230" spans="1:6" ht="33.75">
+    <row r="230" spans="1:6" ht="36" x14ac:dyDescent="0.35">
       <c r="A230" s="18" t="s">
         <v>577</v>
       </c>
@@ -9992,7 +10058,7 @@
         <v>925</v>
       </c>
     </row>
-    <row r="231" spans="1:6" ht="33.75">
+    <row r="231" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A231" s="18" t="s">
         <v>471</v>
       </c>
@@ -10010,7 +10076,7 @@
       </c>
       <c r="F231" s="3"/>
     </row>
-    <row r="232" spans="1:6" ht="33.75">
+    <row r="232" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A232" s="18" t="s">
         <v>1181</v>
       </c>
@@ -10023,7 +10089,7 @@
       </c>
       <c r="F232" s="3"/>
     </row>
-    <row r="233" spans="1:6" ht="33">
+    <row r="233" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A233" s="18" t="s">
         <v>55</v>
       </c>
@@ -10041,7 +10107,7 @@
       </c>
       <c r="F233" s="3"/>
     </row>
-    <row r="234" spans="1:6" ht="33.75">
+    <row r="234" spans="1:6" ht="35" x14ac:dyDescent="0.35">
       <c r="A234" s="18" t="s">
         <v>1186</v>
       </c>
@@ -10054,7 +10120,7 @@
       </c>
       <c r="F234" s="3"/>
     </row>
-    <row r="235" spans="1:6" ht="63">
+    <row r="235" spans="1:6" ht="67" x14ac:dyDescent="0.35">
       <c r="A235" s="18" t="s">
         <v>97</v>
       </c>
@@ -10072,7 +10138,7 @@
       </c>
       <c r="F235" s="3"/>
     </row>
-    <row r="236" spans="1:6">
+    <row r="236" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A236" s="18" t="s">
         <v>15</v>
       </c>
@@ -10090,7 +10156,7 @@
       </c>
       <c r="F236" s="3"/>
     </row>
-    <row r="237" spans="1:6">
+    <row r="237" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A237" s="18" t="s">
         <v>1182</v>
       </c>
@@ -10101,7 +10167,7 @@
       <c r="D237" s="20"/>
       <c r="F237" s="3"/>
     </row>
-    <row r="238" spans="1:6" ht="33">
+    <row r="238" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A238" s="18" t="s">
         <v>557</v>
       </c>
@@ -10119,7 +10185,7 @@
       </c>
       <c r="F238" s="3"/>
     </row>
-    <row r="239" spans="1:6">
+    <row r="239" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A239" s="18" t="s">
         <v>1311</v>
       </c>
@@ -10134,7 +10200,7 @@
       </c>
       <c r="F239" s="3"/>
     </row>
-    <row r="240" spans="1:6" ht="33.75">
+    <row r="240" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A240" s="18" t="s">
         <v>127</v>
       </c>
@@ -10152,7 +10218,7 @@
       </c>
       <c r="F240" s="3"/>
     </row>
-    <row r="241" spans="1:6" ht="33">
+    <row r="241" spans="1:6" ht="35" x14ac:dyDescent="0.35">
       <c r="A241" s="18" t="s">
         <v>770</v>
       </c>
@@ -10170,7 +10236,7 @@
       </c>
       <c r="F241" s="3"/>
     </row>
-    <row r="242" spans="1:6">
+    <row r="242" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A242" s="18" t="s">
         <v>1073</v>
       </c>
@@ -10183,7 +10249,7 @@
       </c>
       <c r="F242" s="3"/>
     </row>
-    <row r="243" spans="1:6">
+    <row r="243" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A243" s="18" t="s">
         <v>125</v>
       </c>
@@ -10201,7 +10267,7 @@
       </c>
       <c r="F243" s="3"/>
     </row>
-    <row r="244" spans="1:6" ht="33.75">
+    <row r="244" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A244" s="18" t="s">
         <v>896</v>
       </c>
@@ -10221,7 +10287,7 @@
         <v>921</v>
       </c>
     </row>
-    <row r="245" spans="1:6" ht="33.75">
+    <row r="245" spans="1:6" ht="36" x14ac:dyDescent="0.35">
       <c r="A245" s="18" t="s">
         <v>1068</v>
       </c>
@@ -10234,7 +10300,7 @@
       </c>
       <c r="F245" s="3"/>
     </row>
-    <row r="246" spans="1:6" ht="45">
+    <row r="246" spans="1:6" ht="48" x14ac:dyDescent="0.35">
       <c r="A246" s="18" t="s">
         <v>808</v>
       </c>
@@ -10252,7 +10318,7 @@
       </c>
       <c r="F246" s="3"/>
     </row>
-    <row r="247" spans="1:6">
+    <row r="247" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A247" s="18" t="s">
         <v>283</v>
       </c>
@@ -10270,7 +10336,7 @@
       </c>
       <c r="F247" s="3"/>
     </row>
-    <row r="248" spans="1:6">
+    <row r="248" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A248" s="18" t="s">
         <v>3</v>
       </c>
@@ -10288,7 +10354,7 @@
       </c>
       <c r="F248" s="3"/>
     </row>
-    <row r="249" spans="1:6">
+    <row r="249" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A249" s="18" t="s">
         <v>419</v>
       </c>
@@ -10306,7 +10372,7 @@
       </c>
       <c r="F249" s="3"/>
     </row>
-    <row r="250" spans="1:6" ht="33.75">
+    <row r="250" spans="1:6" ht="36" x14ac:dyDescent="0.35">
       <c r="A250" s="18" t="s">
         <v>370</v>
       </c>
@@ -10324,7 +10390,7 @@
       </c>
       <c r="F250" s="3"/>
     </row>
-    <row r="251" spans="1:6">
+    <row r="251" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A251" s="18" t="s">
         <v>286</v>
       </c>
@@ -10342,7 +10408,7 @@
       </c>
       <c r="F251" s="3"/>
     </row>
-    <row r="252" spans="1:6">
+    <row r="252" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A252" s="18" t="s">
         <v>207</v>
       </c>
@@ -10360,7 +10426,7 @@
       </c>
       <c r="F252" s="3"/>
     </row>
-    <row r="253" spans="1:6">
+    <row r="253" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A253" s="18" t="s">
         <v>73</v>
       </c>
@@ -10378,7 +10444,7 @@
       </c>
       <c r="F253" s="3"/>
     </row>
-    <row r="254" spans="1:6">
+    <row r="254" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A254" s="18" t="s">
         <v>1193</v>
       </c>
@@ -10393,7 +10459,7 @@
       </c>
       <c r="F254" s="3"/>
     </row>
-    <row r="255" spans="1:6">
+    <row r="255" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A255" s="18" t="s">
         <v>1203</v>
       </c>
@@ -10408,7 +10474,7 @@
       </c>
       <c r="F255" s="3"/>
     </row>
-    <row r="256" spans="1:6">
+    <row r="256" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A256" s="18" t="s">
         <v>122</v>
       </c>
@@ -10426,7 +10492,7 @@
       </c>
       <c r="F256" s="3"/>
     </row>
-    <row r="257" spans="1:6">
+    <row r="257" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A257" s="18" t="s">
         <v>880</v>
       </c>
@@ -10446,7 +10512,7 @@
         <v>886</v>
       </c>
     </row>
-    <row r="258" spans="1:6" ht="33.75">
+    <row r="258" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A258" s="18" t="s">
         <v>199</v>
       </c>
@@ -10464,7 +10530,7 @@
       </c>
       <c r="F258" s="3"/>
     </row>
-    <row r="259" spans="1:6" ht="33">
+    <row r="259" spans="1:6" ht="35" x14ac:dyDescent="0.35">
       <c r="A259" s="18" t="s">
         <v>1138</v>
       </c>
@@ -10479,7 +10545,7 @@
       </c>
       <c r="F259" s="3"/>
     </row>
-    <row r="260" spans="1:6">
+    <row r="260" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A260" s="18" t="s">
         <v>6</v>
       </c>
@@ -10493,7 +10559,7 @@
       </c>
       <c r="F260" s="3"/>
     </row>
-    <row r="261" spans="1:6">
+    <row r="261" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A261" s="18" t="s">
         <v>165</v>
       </c>
@@ -10511,7 +10577,7 @@
       </c>
       <c r="F261" s="3"/>
     </row>
-    <row r="262" spans="1:6" ht="56.25">
+    <row r="262" spans="1:6" ht="60" x14ac:dyDescent="0.35">
       <c r="A262" s="18" t="s">
         <v>459</v>
       </c>
@@ -10529,7 +10595,7 @@
       </c>
       <c r="F262" s="3"/>
     </row>
-    <row r="263" spans="1:6" ht="56.25">
+    <row r="263" spans="1:6" ht="60" x14ac:dyDescent="0.35">
       <c r="A263" s="18" t="s">
         <v>461</v>
       </c>
@@ -10547,7 +10613,7 @@
       </c>
       <c r="F263" s="3"/>
     </row>
-    <row r="264" spans="1:6">
+    <row r="264" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A264" s="18" t="s">
         <v>463</v>
       </c>
@@ -10565,7 +10631,7 @@
       </c>
       <c r="F264" s="3"/>
     </row>
-    <row r="265" spans="1:6">
+    <row r="265" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A265" s="18" t="s">
         <v>411</v>
       </c>
@@ -10583,7 +10649,7 @@
       </c>
       <c r="F265" s="3"/>
     </row>
-    <row r="266" spans="1:6" ht="33">
+    <row r="266" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A266" s="18" t="s">
         <v>241</v>
       </c>
@@ -10601,7 +10667,7 @@
       </c>
       <c r="F266" s="3"/>
     </row>
-    <row r="267" spans="1:6">
+    <row r="267" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A267" s="18" t="s">
         <v>474</v>
       </c>
@@ -10619,7 +10685,7 @@
       </c>
       <c r="F267" s="3"/>
     </row>
-    <row r="268" spans="1:6" s="6" customFormat="1">
+    <row r="268" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A268" s="18" t="s">
         <v>1283</v>
       </c>
@@ -10635,7 +10701,7 @@
       <c r="E268" s="3"/>
       <c r="F268" s="3"/>
     </row>
-    <row r="269" spans="1:6">
+    <row r="269" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A269" s="18" t="s">
         <v>406</v>
       </c>
@@ -10653,7 +10719,7 @@
       </c>
       <c r="F269" s="3"/>
     </row>
-    <row r="270" spans="1:6" ht="48">
+    <row r="270" spans="1:6" ht="51" x14ac:dyDescent="0.35">
       <c r="A270" s="18" t="s">
         <v>756</v>
       </c>
@@ -10671,7 +10737,7 @@
       </c>
       <c r="F270" s="3"/>
     </row>
-    <row r="271" spans="1:6" ht="33.75">
+    <row r="271" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A271" s="18" t="s">
         <v>1250</v>
       </c>
@@ -10686,7 +10752,7 @@
       </c>
       <c r="F271" s="3"/>
     </row>
-    <row r="272" spans="1:6" ht="33.75">
+    <row r="272" spans="1:6" ht="35" x14ac:dyDescent="0.35">
       <c r="A272" s="18" t="s">
         <v>464</v>
       </c>
@@ -10704,7 +10770,7 @@
       </c>
       <c r="F272" s="3"/>
     </row>
-    <row r="273" spans="1:6" ht="33">
+    <row r="273" spans="1:6" ht="35" x14ac:dyDescent="0.35">
       <c r="A273" s="18" t="s">
         <v>449</v>
       </c>
@@ -10722,7 +10788,7 @@
       </c>
       <c r="F273" s="3"/>
     </row>
-    <row r="274" spans="1:6">
+    <row r="274" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A274" s="18" t="s">
         <v>445</v>
       </c>
@@ -10737,7 +10803,7 @@
       </c>
       <c r="F274" s="3"/>
     </row>
-    <row r="275" spans="1:6">
+    <row r="275" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A275" s="18" t="s">
         <v>1199</v>
       </c>
@@ -10752,7 +10818,7 @@
       </c>
       <c r="F275" s="3"/>
     </row>
-    <row r="276" spans="1:6">
+    <row r="276" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A276" s="18" t="s">
         <v>115</v>
       </c>
@@ -10770,7 +10836,7 @@
       </c>
       <c r="F276" s="3"/>
     </row>
-    <row r="277" spans="1:6">
+    <row r="277" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A277" s="18" t="s">
         <v>388</v>
       </c>
@@ -10788,7 +10854,7 @@
       </c>
       <c r="F277" s="3"/>
     </row>
-    <row r="278" spans="1:6">
+    <row r="278" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A278" s="18" t="s">
         <v>1152</v>
       </c>
@@ -10801,7 +10867,7 @@
       <c r="D278" s="20"/>
       <c r="F278" s="3"/>
     </row>
-    <row r="279" spans="1:6" ht="33.75">
+    <row r="279" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A279" s="18" t="s">
         <v>243</v>
       </c>
@@ -10819,7 +10885,7 @@
       </c>
       <c r="F279" s="3"/>
     </row>
-    <row r="280" spans="1:6">
+    <row r="280" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A280" s="18" t="s">
         <v>0</v>
       </c>
@@ -10837,7 +10903,7 @@
       </c>
       <c r="F280" s="3"/>
     </row>
-    <row r="281" spans="1:6">
+    <row r="281" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A281" s="18" t="s">
         <v>197</v>
       </c>
@@ -10853,7 +10919,7 @@
       </c>
       <c r="F281" s="3"/>
     </row>
-    <row r="282" spans="1:6">
+    <row r="282" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A282" s="18" t="s">
         <v>1145</v>
       </c>
@@ -10864,7 +10930,7 @@
       <c r="D282" s="20"/>
       <c r="F282" s="3"/>
     </row>
-    <row r="283" spans="1:6" ht="56.25">
+    <row r="283" spans="1:6" ht="48" x14ac:dyDescent="0.35">
       <c r="A283" s="18" t="s">
         <v>1362</v>
       </c>
@@ -10884,7 +10950,7 @@
         <v>912</v>
       </c>
     </row>
-    <row r="284" spans="1:6" ht="33">
+    <row r="284" spans="1:6" ht="35" x14ac:dyDescent="0.35">
       <c r="A284" s="18" t="s">
         <v>235</v>
       </c>
@@ -10902,7 +10968,7 @@
       </c>
       <c r="F284" s="3"/>
     </row>
-    <row r="285" spans="1:6" ht="33.75">
+    <row r="285" spans="1:6" ht="36" x14ac:dyDescent="0.35">
       <c r="A285" s="18" t="s">
         <v>149</v>
       </c>
@@ -10920,7 +10986,7 @@
       </c>
       <c r="F285" s="3"/>
     </row>
-    <row r="286" spans="1:6">
+    <row r="286" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A286" s="18" t="s">
         <v>222</v>
       </c>
@@ -10938,7 +11004,7 @@
       </c>
       <c r="F286" s="3"/>
     </row>
-    <row r="287" spans="1:6" ht="33.75">
+    <row r="287" spans="1:6" ht="36" x14ac:dyDescent="0.35">
       <c r="A287" s="18" t="s">
         <v>1143</v>
       </c>
@@ -10953,7 +11019,7 @@
       </c>
       <c r="F287" s="3"/>
     </row>
-    <row r="288" spans="1:6">
+    <row r="288" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A288" s="18" t="s">
         <v>234</v>
       </c>
@@ -10969,7 +11035,7 @@
       </c>
       <c r="F288" s="3"/>
     </row>
-    <row r="289" spans="1:6">
+    <row r="289" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A289" s="18" t="s">
         <v>211</v>
       </c>
@@ -10987,7 +11053,7 @@
       </c>
       <c r="F289" s="3"/>
     </row>
-    <row r="290" spans="1:6" ht="33">
+    <row r="290" spans="1:6" ht="35" x14ac:dyDescent="0.35">
       <c r="A290" s="18" t="s">
         <v>231</v>
       </c>
@@ -11005,7 +11071,7 @@
       </c>
       <c r="F290" s="3"/>
     </row>
-    <row r="291" spans="1:6" ht="33">
+    <row r="291" spans="1:6" ht="35" x14ac:dyDescent="0.35">
       <c r="A291" s="18" t="s">
         <v>290</v>
       </c>
@@ -11023,7 +11089,7 @@
       </c>
       <c r="F291" s="3"/>
     </row>
-    <row r="292" spans="1:6">
+    <row r="292" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A292" s="18" t="s">
         <v>158</v>
       </c>
@@ -11041,7 +11107,7 @@
       </c>
       <c r="F292" s="3"/>
     </row>
-    <row r="293" spans="1:6">
+    <row r="293" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A293" s="18" t="s">
         <v>45</v>
       </c>
@@ -11059,7 +11125,7 @@
       </c>
       <c r="F293" s="3"/>
     </row>
-    <row r="294" spans="1:6" ht="33">
+    <row r="294" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A294" s="18" t="s">
         <v>490</v>
       </c>
@@ -11077,7 +11143,7 @@
       </c>
       <c r="F294" s="3"/>
     </row>
-    <row r="295" spans="1:6">
+    <row r="295" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A295" s="18" t="s">
         <v>1275</v>
       </c>
@@ -11092,7 +11158,7 @@
       </c>
       <c r="F295" s="3"/>
     </row>
-    <row r="296" spans="1:6">
+    <row r="296" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A296" s="18" t="s">
         <v>1364</v>
       </c>
@@ -11110,7 +11176,7 @@
       </c>
       <c r="F296" s="3"/>
     </row>
-    <row r="297" spans="1:6" ht="33.75">
+    <row r="297" spans="1:6" ht="36" x14ac:dyDescent="0.35">
       <c r="A297" s="18" t="s">
         <v>1365</v>
       </c>
@@ -11128,7 +11194,7 @@
       </c>
       <c r="F297" s="3"/>
     </row>
-    <row r="298" spans="1:6" ht="33.75">
+    <row r="298" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A298" s="18" t="s">
         <v>239</v>
       </c>
@@ -11146,7 +11212,7 @@
       </c>
       <c r="F298" s="3"/>
     </row>
-    <row r="299" spans="1:6">
+    <row r="299" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A299" s="18" t="s">
         <v>1022</v>
       </c>
@@ -11161,7 +11227,7 @@
       </c>
       <c r="F299" s="3"/>
     </row>
-    <row r="300" spans="1:6">
+    <row r="300" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A300" s="18" t="s">
         <v>466</v>
       </c>
@@ -11179,7 +11245,7 @@
       </c>
       <c r="F300" s="3"/>
     </row>
-    <row r="301" spans="1:6" ht="33.75">
+    <row r="301" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A301" s="18" t="s">
         <v>1259</v>
       </c>
@@ -11194,7 +11260,7 @@
       </c>
       <c r="F301" s="3"/>
     </row>
-    <row r="302" spans="1:6" ht="33.75">
+    <row r="302" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A302" s="18" t="s">
         <v>1252</v>
       </c>
@@ -11209,7 +11275,7 @@
       </c>
       <c r="F302" s="3"/>
     </row>
-    <row r="303" spans="1:6">
+    <row r="303" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A303" s="18" t="s">
         <v>171</v>
       </c>
@@ -11227,7 +11293,7 @@
       </c>
       <c r="F303" s="3"/>
     </row>
-    <row r="304" spans="1:6">
+    <row r="304" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A304" s="18" t="s">
         <v>1331</v>
       </c>
@@ -11242,7 +11308,7 @@
       </c>
       <c r="F304" s="3"/>
     </row>
-    <row r="305" spans="1:6">
+    <row r="305" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A305" s="18" t="s">
         <v>292</v>
       </c>
@@ -11253,7 +11319,7 @@
       <c r="D305" s="20"/>
       <c r="F305" s="3"/>
     </row>
-    <row r="306" spans="1:6">
+    <row r="306" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A306" s="18" t="s">
         <v>1263</v>
       </c>
@@ -11268,7 +11334,7 @@
       </c>
       <c r="F306" s="3"/>
     </row>
-    <row r="307" spans="1:6" ht="33">
+    <row r="307" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A307" s="18" t="s">
         <v>385</v>
       </c>
@@ -11288,7 +11354,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="308" spans="1:6">
+    <row r="308" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A308" s="18" t="s">
         <v>489</v>
       </c>
@@ -11306,7 +11372,7 @@
       </c>
       <c r="F308" s="3"/>
     </row>
-    <row r="309" spans="1:6">
+    <row r="309" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A309" s="18" t="s">
         <v>1272</v>
       </c>
@@ -11321,7 +11387,7 @@
       </c>
       <c r="F309" s="3"/>
     </row>
-    <row r="310" spans="1:6" ht="33">
+    <row r="310" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A310" s="18" t="s">
         <v>394</v>
       </c>
@@ -11339,7 +11405,7 @@
       </c>
       <c r="F310" s="3"/>
     </row>
-    <row r="311" spans="1:6" ht="33">
+    <row r="311" spans="1:6" ht="35" x14ac:dyDescent="0.35">
       <c r="A311" s="18" t="s">
         <v>1166</v>
       </c>
@@ -11352,7 +11418,7 @@
       </c>
       <c r="F311" s="3"/>
     </row>
-    <row r="312" spans="1:6">
+    <row r="312" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A312" s="18" t="s">
         <v>487</v>
       </c>
@@ -11370,7 +11436,7 @@
       </c>
       <c r="F312" s="3"/>
     </row>
-    <row r="313" spans="1:6" ht="33">
+    <row r="313" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A313" s="18" t="s">
         <v>488</v>
       </c>
@@ -11388,7 +11454,7 @@
       </c>
       <c r="F313" s="3"/>
     </row>
-    <row r="314" spans="1:6">
+    <row r="314" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A314" s="18" t="s">
         <v>293</v>
       </c>
@@ -11406,7 +11472,7 @@
       </c>
       <c r="F314" s="3"/>
     </row>
-    <row r="315" spans="1:6" ht="33.75">
+    <row r="315" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A315" s="18" t="s">
         <v>1258</v>
       </c>
@@ -11421,7 +11487,7 @@
       </c>
       <c r="F315" s="3"/>
     </row>
-    <row r="316" spans="1:6">
+    <row r="316" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A316" s="18" t="s">
         <v>479</v>
       </c>
@@ -11439,7 +11505,7 @@
       </c>
       <c r="F316" s="3"/>
     </row>
-    <row r="317" spans="1:6">
+    <row r="317" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A317" s="18" t="s">
         <v>1366</v>
       </c>
@@ -11457,7 +11523,7 @@
       </c>
       <c r="F317" s="3"/>
     </row>
-    <row r="318" spans="1:6" ht="33.75">
+    <row r="318" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A318" s="18" t="s">
         <v>1149</v>
       </c>
@@ -11472,7 +11538,7 @@
       </c>
       <c r="F318" s="3"/>
     </row>
-    <row r="319" spans="1:6" ht="33.75">
+    <row r="319" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A319" s="18" t="s">
         <v>1290</v>
       </c>
@@ -11487,7 +11553,7 @@
       </c>
       <c r="F319" s="3"/>
     </row>
-    <row r="320" spans="1:6" ht="112.5">
+    <row r="320" spans="1:6" ht="96" x14ac:dyDescent="0.35">
       <c r="A320" s="18" t="s">
         <v>417</v>
       </c>
@@ -11505,7 +11571,7 @@
       </c>
       <c r="F320" s="3"/>
     </row>
-    <row r="321" spans="1:6 16384:16384" ht="33">
+    <row r="321" spans="1:6 16384:16384" ht="35" x14ac:dyDescent="0.35">
       <c r="A321" s="18" t="s">
         <v>802</v>
       </c>
@@ -11523,7 +11589,7 @@
       </c>
       <c r="F321" s="3"/>
     </row>
-    <row r="322" spans="1:6 16384:16384">
+    <row r="322" spans="1:6 16384:16384" x14ac:dyDescent="0.35">
       <c r="A322" s="18" t="s">
         <v>1060</v>
       </c>
@@ -11534,7 +11600,7 @@
       </c>
       <c r="F322" s="3"/>
     </row>
-    <row r="323" spans="1:6 16384:16384" ht="78.75">
+    <row r="323" spans="1:6 16384:16384" ht="84" x14ac:dyDescent="0.35">
       <c r="A323" s="18" t="s">
         <v>1059</v>
       </c>
@@ -11547,7 +11613,7 @@
       </c>
       <c r="F323" s="3"/>
     </row>
-    <row r="324" spans="1:6 16384:16384">
+    <row r="324" spans="1:6 16384:16384" x14ac:dyDescent="0.35">
       <c r="A324" s="18" t="s">
         <v>31</v>
       </c>
@@ -11565,7 +11631,7 @@
       </c>
       <c r="F324" s="3"/>
     </row>
-    <row r="325" spans="1:6 16384:16384">
+    <row r="325" spans="1:6 16384:16384" x14ac:dyDescent="0.35">
       <c r="A325" s="18" t="s">
         <v>376</v>
       </c>
@@ -11583,7 +11649,7 @@
       </c>
       <c r="F325" s="3"/>
     </row>
-    <row r="326" spans="1:6 16384:16384">
+    <row r="326" spans="1:6 16384:16384" x14ac:dyDescent="0.35">
       <c r="A326" s="18" t="s">
         <v>213</v>
       </c>
@@ -11601,7 +11667,7 @@
       </c>
       <c r="F326" s="3"/>
     </row>
-    <row r="327" spans="1:6 16384:16384">
+    <row r="327" spans="1:6 16384:16384" x14ac:dyDescent="0.35">
       <c r="A327" s="18" t="s">
         <v>51</v>
       </c>
@@ -11619,7 +11685,7 @@
       </c>
       <c r="F327" s="3"/>
     </row>
-    <row r="328" spans="1:6 16384:16384" ht="33">
+    <row r="328" spans="1:6 16384:16384" x14ac:dyDescent="0.35">
       <c r="A328" s="18" t="s">
         <v>446</v>
       </c>
@@ -11637,7 +11703,7 @@
       </c>
       <c r="F328" s="3"/>
     </row>
-    <row r="329" spans="1:6 16384:16384" ht="33">
+    <row r="329" spans="1:6 16384:16384" x14ac:dyDescent="0.35">
       <c r="A329" s="18" t="s">
         <v>190</v>
       </c>
@@ -11655,7 +11721,7 @@
       </c>
       <c r="F329" s="3"/>
     </row>
-    <row r="330" spans="1:6 16384:16384">
+    <row r="330" spans="1:6 16384:16384" x14ac:dyDescent="0.35">
       <c r="A330" s="18" t="s">
         <v>294</v>
       </c>
@@ -11673,7 +11739,7 @@
       </c>
       <c r="F330" s="3"/>
     </row>
-    <row r="331" spans="1:6 16384:16384">
+    <row r="331" spans="1:6 16384:16384" x14ac:dyDescent="0.35">
       <c r="A331" s="18" t="s">
         <v>1278</v>
       </c>
@@ -11688,7 +11754,7 @@
       </c>
       <c r="F331" s="3"/>
     </row>
-    <row r="332" spans="1:6 16384:16384">
+    <row r="332" spans="1:6 16384:16384" x14ac:dyDescent="0.35">
       <c r="A332" s="18" t="s">
         <v>1220</v>
       </c>
@@ -11703,7 +11769,7 @@
       </c>
       <c r="F332" s="3"/>
     </row>
-    <row r="333" spans="1:6 16384:16384" ht="33.75">
+    <row r="333" spans="1:6 16384:16384" x14ac:dyDescent="0.35">
       <c r="A333" s="18" t="s">
         <v>1367</v>
       </c>
@@ -11721,7 +11787,7 @@
       </c>
       <c r="F333" s="3"/>
     </row>
-    <row r="334" spans="1:6 16384:16384" ht="48">
+    <row r="334" spans="1:6 16384:16384" ht="51" x14ac:dyDescent="0.35">
       <c r="A334" s="18" t="s">
         <v>399</v>
       </c>
@@ -11739,7 +11805,7 @@
       </c>
       <c r="F334" s="3"/>
     </row>
-    <row r="335" spans="1:6 16384:16384">
+    <row r="335" spans="1:6 16384:16384" x14ac:dyDescent="0.35">
       <c r="A335" s="18" t="s">
         <v>64</v>
       </c>
@@ -11757,7 +11823,7 @@
       </c>
       <c r="F335" s="3"/>
     </row>
-    <row r="336" spans="1:6 16384:16384" ht="33.75">
+    <row r="336" spans="1:6 16384:16384" ht="36" x14ac:dyDescent="0.35">
       <c r="A336" s="18" t="s">
         <v>855</v>
       </c>
@@ -11778,7 +11844,7 @@
       </c>
       <c r="XFD336" s="5"/>
     </row>
-    <row r="337" spans="1:6">
+    <row r="337" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A337" s="18" t="s">
         <v>492</v>
       </c>
@@ -11796,7 +11862,7 @@
       </c>
       <c r="F337" s="3"/>
     </row>
-    <row r="338" spans="1:6">
+    <row r="338" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A338" s="18" t="s">
         <v>882</v>
       </c>
@@ -11816,7 +11882,7 @@
         <v>890</v>
       </c>
     </row>
-    <row r="339" spans="1:6">
+    <row r="339" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A339" s="18" t="s">
         <v>494</v>
       </c>
@@ -11834,7 +11900,7 @@
       </c>
       <c r="F339" s="3"/>
     </row>
-    <row r="340" spans="1:6">
+    <row r="340" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A340" s="18" t="s">
         <v>1056</v>
       </c>
@@ -11845,7 +11911,7 @@
       <c r="D340" s="20"/>
       <c r="F340" s="3"/>
     </row>
-    <row r="341" spans="1:6">
+    <row r="341" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A341" s="18" t="s">
         <v>185</v>
       </c>
@@ -11863,7 +11929,7 @@
       </c>
       <c r="F341" s="3"/>
     </row>
-    <row r="342" spans="1:6">
+    <row r="342" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A342" s="18" t="s">
         <v>495</v>
       </c>
@@ -11881,7 +11947,7 @@
       </c>
       <c r="F342" s="3"/>
     </row>
-    <row r="343" spans="1:6" ht="33.75">
+    <row r="343" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A343" s="18" t="s">
         <v>1329</v>
       </c>
@@ -11896,7 +11962,7 @@
       </c>
       <c r="F343" s="3"/>
     </row>
-    <row r="344" spans="1:6" ht="33">
+    <row r="344" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A344" s="18" t="s">
         <v>111</v>
       </c>
@@ -11914,7 +11980,7 @@
       </c>
       <c r="F344" s="3"/>
     </row>
-    <row r="345" spans="1:6">
+    <row r="345" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A345" s="18" t="s">
         <v>342</v>
       </c>
@@ -11932,7 +11998,7 @@
       </c>
       <c r="F345" s="3"/>
     </row>
-    <row r="346" spans="1:6">
+    <row r="346" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A346" s="18" t="s">
         <v>66</v>
       </c>
@@ -11950,7 +12016,7 @@
       </c>
       <c r="F346" s="3"/>
     </row>
-    <row r="347" spans="1:6" ht="33">
+    <row r="347" spans="1:6" ht="35" x14ac:dyDescent="0.35">
       <c r="A347" s="18" t="s">
         <v>864</v>
       </c>
@@ -11970,7 +12036,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="348" spans="1:6">
+    <row r="348" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A348" s="18" t="s">
         <v>56</v>
       </c>
@@ -11988,7 +12054,7 @@
       </c>
       <c r="F348" s="3"/>
     </row>
-    <row r="349" spans="1:6">
+    <row r="349" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A349" s="18" t="s">
         <v>815</v>
       </c>
@@ -12004,7 +12070,7 @@
       </c>
       <c r="F349" s="3"/>
     </row>
-    <row r="350" spans="1:6" ht="33.75">
+    <row r="350" spans="1:6" ht="36" x14ac:dyDescent="0.35">
       <c r="A350" s="18" t="s">
         <v>560</v>
       </c>
@@ -12022,7 +12088,7 @@
       </c>
       <c r="F350" s="3"/>
     </row>
-    <row r="351" spans="1:6" ht="33">
+    <row r="351" spans="1:6" ht="35" x14ac:dyDescent="0.35">
       <c r="A351" s="18" t="s">
         <v>1155</v>
       </c>
@@ -12037,7 +12103,7 @@
       </c>
       <c r="F351" s="3"/>
     </row>
-    <row r="352" spans="1:6">
+    <row r="352" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A352" s="18" t="s">
         <v>821</v>
       </c>
@@ -12055,7 +12121,7 @@
       </c>
       <c r="F352" s="3"/>
     </row>
-    <row r="353" spans="1:6">
+    <row r="353" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A353" s="18" t="s">
         <v>336</v>
       </c>
@@ -12073,7 +12139,7 @@
       </c>
       <c r="F353" s="3"/>
     </row>
-    <row r="354" spans="1:6">
+    <row r="354" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A354" s="18" t="s">
         <v>300</v>
       </c>
@@ -12089,7 +12155,7 @@
       </c>
       <c r="F354" s="3"/>
     </row>
-    <row r="355" spans="1:6">
+    <row r="355" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A355" s="18" t="s">
         <v>573</v>
       </c>
@@ -12107,7 +12173,7 @@
       </c>
       <c r="F355" s="3"/>
     </row>
-    <row r="356" spans="1:6" ht="33">
+    <row r="356" spans="1:6" ht="35" x14ac:dyDescent="0.35">
       <c r="A356" s="18" t="s">
         <v>468</v>
       </c>
@@ -12125,7 +12191,7 @@
       </c>
       <c r="F356" s="3"/>
     </row>
-    <row r="357" spans="1:6">
+    <row r="357" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A357" s="18" t="s">
         <v>1265</v>
       </c>
@@ -12140,7 +12206,7 @@
       </c>
       <c r="F357" s="3"/>
     </row>
-    <row r="358" spans="1:6" ht="33.75">
+    <row r="358" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A358" s="18" t="s">
         <v>226</v>
       </c>
@@ -12158,7 +12224,7 @@
       </c>
       <c r="F358" s="3"/>
     </row>
-    <row r="359" spans="1:6" ht="33">
+    <row r="359" spans="1:6" ht="35" x14ac:dyDescent="0.35">
       <c r="A359" s="18" t="s">
         <v>486</v>
       </c>
@@ -12174,7 +12240,7 @@
       </c>
       <c r="F359" s="3"/>
     </row>
-    <row r="360" spans="1:6" ht="33">
+    <row r="360" spans="1:6" ht="35" x14ac:dyDescent="0.35">
       <c r="A360" s="18" t="s">
         <v>1369</v>
       </c>
@@ -12192,7 +12258,7 @@
       </c>
       <c r="F360" s="3"/>
     </row>
-    <row r="361" spans="1:6" ht="33.75">
+    <row r="361" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A361" s="18" t="s">
         <v>301</v>
       </c>
@@ -12210,7 +12276,7 @@
       </c>
       <c r="F361" s="3"/>
     </row>
-    <row r="362" spans="1:6">
+    <row r="362" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A362" s="18" t="s">
         <v>314</v>
       </c>
@@ -12228,7 +12294,7 @@
       </c>
       <c r="F362" s="3"/>
     </row>
-    <row r="363" spans="1:6">
+    <row r="363" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A363" s="18" t="s">
         <v>203</v>
       </c>
@@ -12246,7 +12312,7 @@
       </c>
       <c r="F363" s="3"/>
     </row>
-    <row r="364" spans="1:6">
+    <row r="364" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A364" s="18" t="s">
         <v>1083</v>
       </c>
@@ -12259,7 +12325,7 @@
       </c>
       <c r="F364" s="3"/>
     </row>
-    <row r="365" spans="1:6">
+    <row r="365" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A365" s="18" t="s">
         <v>404</v>
       </c>
@@ -12277,7 +12343,7 @@
       </c>
       <c r="F365" s="3"/>
     </row>
-    <row r="366" spans="1:6" ht="33.75">
+    <row r="366" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A366" s="18" t="s">
         <v>708</v>
       </c>
@@ -12295,7 +12361,7 @@
       </c>
       <c r="F366" s="3"/>
     </row>
-    <row r="367" spans="1:6">
+    <row r="367" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A367" s="18" t="s">
         <v>477</v>
       </c>
@@ -12313,7 +12379,7 @@
       </c>
       <c r="F367" s="3"/>
     </row>
-    <row r="368" spans="1:6">
+    <row r="368" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A368" s="18" t="s">
         <v>139</v>
       </c>
@@ -12331,7 +12397,7 @@
       </c>
       <c r="F368" s="3"/>
     </row>
-    <row r="369" spans="1:6" ht="33.75">
+    <row r="369" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A369" s="18" t="s">
         <v>1285</v>
       </c>
@@ -12346,7 +12412,7 @@
       </c>
       <c r="F369" s="3"/>
     </row>
-    <row r="370" spans="1:6">
+    <row r="370" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A370" s="18" t="s">
         <v>861</v>
       </c>
@@ -12366,7 +12432,7 @@
         <v>904</v>
       </c>
     </row>
-    <row r="371" spans="1:6">
+    <row r="371" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A371" s="18" t="s">
         <v>1209</v>
       </c>
@@ -12381,7 +12447,7 @@
       </c>
       <c r="F371" s="3"/>
     </row>
-    <row r="372" spans="1:6" ht="33.75">
+    <row r="372" spans="1:6" ht="35" x14ac:dyDescent="0.35">
       <c r="A372" s="18" t="s">
         <v>898</v>
       </c>
@@ -12401,7 +12467,7 @@
         <v>923</v>
       </c>
     </row>
-    <row r="373" spans="1:6" ht="33">
+    <row r="373" spans="1:6" ht="35" x14ac:dyDescent="0.35">
       <c r="A373" s="18" t="s">
         <v>898</v>
       </c>
@@ -12414,7 +12480,7 @@
       </c>
       <c r="F373" s="3"/>
     </row>
-    <row r="374" spans="1:6" ht="33.75">
+    <row r="374" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A374" s="18" t="s">
         <v>23</v>
       </c>
@@ -12432,7 +12498,7 @@
       </c>
       <c r="F374" s="3"/>
     </row>
-    <row r="375" spans="1:6">
+    <row r="375" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A375" s="18" t="s">
         <v>713</v>
       </c>
@@ -12450,7 +12516,7 @@
       </c>
       <c r="F375" s="3"/>
     </row>
-    <row r="376" spans="1:6">
+    <row r="376" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A376" s="18" t="s">
         <v>823</v>
       </c>
@@ -12466,7 +12532,7 @@
       </c>
       <c r="F376" s="3"/>
     </row>
-    <row r="377" spans="1:6">
+    <row r="377" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A377" s="18" t="s">
         <v>454</v>
       </c>
@@ -12484,7 +12550,7 @@
       </c>
       <c r="F377" s="3"/>
     </row>
-    <row r="378" spans="1:6">
+    <row r="378" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A378" s="18" t="s">
         <v>1041</v>
       </c>
@@ -12497,7 +12563,7 @@
       </c>
       <c r="F378" s="3"/>
     </row>
-    <row r="379" spans="1:6">
+    <row r="379" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A379" s="18" t="s">
         <v>453</v>
       </c>
@@ -12515,7 +12581,7 @@
       </c>
       <c r="F379" s="3"/>
     </row>
-    <row r="380" spans="1:6">
+    <row r="380" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A380" s="18" t="s">
         <v>29</v>
       </c>
@@ -12533,7 +12599,7 @@
       </c>
       <c r="F380" s="3"/>
     </row>
-    <row r="381" spans="1:6" ht="33.75">
+    <row r="381" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A381" s="18" t="s">
         <v>315</v>
       </c>
@@ -12551,7 +12617,7 @@
       </c>
       <c r="F381" s="3"/>
     </row>
-    <row r="382" spans="1:6" ht="33">
+    <row r="382" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A382" s="18" t="s">
         <v>43</v>
       </c>
@@ -12569,7 +12635,7 @@
       </c>
       <c r="F382" s="3"/>
     </row>
-    <row r="383" spans="1:6">
+    <row r="383" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A383" s="18" t="s">
         <v>733</v>
       </c>
@@ -12587,7 +12653,7 @@
       </c>
       <c r="F383" s="3"/>
     </row>
-    <row r="384" spans="1:6" ht="33">
+    <row r="384" spans="1:6" ht="35" x14ac:dyDescent="0.35">
       <c r="A384" s="18" t="s">
         <v>484</v>
       </c>
@@ -12605,7 +12671,7 @@
       </c>
       <c r="F384" s="3"/>
     </row>
-    <row r="385" spans="1:6">
+    <row r="385" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A385" s="18" t="s">
         <v>546</v>
       </c>
@@ -12623,7 +12689,7 @@
       </c>
       <c r="F385" s="3"/>
     </row>
-    <row r="386" spans="1:6" ht="33.75">
+    <row r="386" spans="1:6" ht="36" x14ac:dyDescent="0.35">
       <c r="A386" s="18" t="s">
         <v>442</v>
       </c>
@@ -12641,7 +12707,7 @@
       </c>
       <c r="F386" s="3"/>
     </row>
-    <row r="387" spans="1:6" ht="45">
+    <row r="387" spans="1:6" ht="48" x14ac:dyDescent="0.35">
       <c r="A387" s="18" t="s">
         <v>88</v>
       </c>
@@ -12659,7 +12725,7 @@
       </c>
       <c r="F387" s="3"/>
     </row>
-    <row r="388" spans="1:6" ht="33.75">
+    <row r="388" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A388" s="18" t="s">
         <v>1374</v>
       </c>
@@ -12677,7 +12743,7 @@
       </c>
       <c r="F388" s="3"/>
     </row>
-    <row r="389" spans="1:6">
+    <row r="389" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A389" s="18" t="s">
         <v>720</v>
       </c>
@@ -12695,7 +12761,7 @@
       </c>
       <c r="F389" s="3"/>
     </row>
-    <row r="390" spans="1:6">
+    <row r="390" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A390" s="18" t="s">
         <v>319</v>
       </c>
@@ -12713,7 +12779,7 @@
       </c>
       <c r="F390" s="3"/>
     </row>
-    <row r="391" spans="1:6">
+    <row r="391" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A391" s="18" t="s">
         <v>237</v>
       </c>
@@ -12731,7 +12797,7 @@
       </c>
       <c r="F391" s="3"/>
     </row>
-    <row r="392" spans="1:6" ht="45">
+    <row r="392" spans="1:6" ht="48" x14ac:dyDescent="0.35">
       <c r="A392" s="18" t="s">
         <v>1051</v>
       </c>
@@ -12746,7 +12812,7 @@
       </c>
       <c r="F392" s="3"/>
     </row>
-    <row r="393" spans="1:6">
+    <row r="393" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A393" s="18" t="s">
         <v>757</v>
       </c>
@@ -12764,7 +12830,7 @@
       </c>
       <c r="F393" s="3"/>
     </row>
-    <row r="394" spans="1:6">
+    <row r="394" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A394" s="18" t="s">
         <v>758</v>
       </c>
@@ -12782,7 +12848,7 @@
       </c>
       <c r="F394" s="3"/>
     </row>
-    <row r="395" spans="1:6">
+    <row r="395" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A395" s="18" t="s">
         <v>759</v>
       </c>
@@ -12800,7 +12866,7 @@
       </c>
       <c r="F395" s="3"/>
     </row>
-    <row r="396" spans="1:6">
+    <row r="396" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A396" s="18" t="s">
         <v>761</v>
       </c>
@@ -12818,7 +12884,7 @@
       </c>
       <c r="F396" s="3"/>
     </row>
-    <row r="397" spans="1:6">
+    <row r="397" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A397" s="18" t="s">
         <v>762</v>
       </c>
@@ -12836,7 +12902,7 @@
       </c>
       <c r="F397" s="3"/>
     </row>
-    <row r="398" spans="1:6" ht="45">
+    <row r="398" spans="1:6" ht="48" x14ac:dyDescent="0.35">
       <c r="A398" s="18" t="s">
         <v>817</v>
       </c>
@@ -12852,7 +12918,7 @@
       </c>
       <c r="F398" s="3"/>
     </row>
-    <row r="399" spans="1:6" ht="33.75">
+    <row r="399" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A399" s="18" t="s">
         <v>1308</v>
       </c>
@@ -12867,7 +12933,7 @@
       </c>
       <c r="F399" s="3"/>
     </row>
-    <row r="400" spans="1:6">
+    <row r="400" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A400" s="18" t="s">
         <v>304</v>
       </c>
@@ -12885,7 +12951,7 @@
       </c>
       <c r="F400" s="3"/>
     </row>
-    <row r="401" spans="1:6" ht="33">
+    <row r="401" spans="1:6" ht="35" x14ac:dyDescent="0.35">
       <c r="A401" s="18" t="s">
         <v>760</v>
       </c>
@@ -12903,7 +12969,7 @@
       </c>
       <c r="F401" s="3"/>
     </row>
-    <row r="402" spans="1:6">
+    <row r="402" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A402" s="18" t="s">
         <v>179</v>
       </c>
@@ -12921,7 +12987,7 @@
       </c>
       <c r="F402" s="3"/>
     </row>
-    <row r="403" spans="1:6" ht="33.75">
+    <row r="403" spans="1:6" ht="36" x14ac:dyDescent="0.35">
       <c r="A403" s="18" t="s">
         <v>271</v>
       </c>
@@ -12939,7 +13005,7 @@
       </c>
       <c r="F403" s="3"/>
     </row>
-    <row r="404" spans="1:6">
+    <row r="404" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A404" s="18" t="s">
         <v>47</v>
       </c>
@@ -12957,7 +13023,7 @@
       </c>
       <c r="F404" s="3"/>
     </row>
-    <row r="405" spans="1:6">
+    <row r="405" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A405" s="18" t="s">
         <v>437</v>
       </c>
@@ -12975,7 +13041,7 @@
       </c>
       <c r="F405" s="3"/>
     </row>
-    <row r="406" spans="1:6">
+    <row r="406" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A406" s="18" t="s">
         <v>212</v>
       </c>
@@ -12988,7 +13054,7 @@
       <c r="D406" s="20"/>
       <c r="F406" s="3"/>
     </row>
-    <row r="407" spans="1:6" ht="45">
+    <row r="407" spans="1:6" ht="48" x14ac:dyDescent="0.35">
       <c r="A407" s="18" t="s">
         <v>35</v>
       </c>
@@ -13006,7 +13072,7 @@
       </c>
       <c r="F407" s="3"/>
     </row>
-    <row r="408" spans="1:6">
+    <row r="408" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A408" s="18" t="s">
         <v>1326</v>
       </c>
@@ -13021,7 +13087,7 @@
       </c>
       <c r="F408" s="3"/>
     </row>
-    <row r="409" spans="1:6">
+    <row r="409" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A409" s="18" t="s">
         <v>36</v>
       </c>
@@ -13039,7 +13105,7 @@
       </c>
       <c r="F409" s="3"/>
     </row>
-    <row r="410" spans="1:6">
+    <row r="410" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A410" s="18" t="s">
         <v>247</v>
       </c>
@@ -13054,7 +13120,7 @@
       </c>
       <c r="F410" s="3"/>
     </row>
-    <row r="411" spans="1:6">
+    <row r="411" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A411" s="18" t="s">
         <v>325</v>
       </c>
@@ -13072,7 +13138,7 @@
       </c>
       <c r="F411" s="3"/>
     </row>
-    <row r="412" spans="1:6">
+    <row r="412" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A412" s="18" t="s">
         <v>1172</v>
       </c>
@@ -13083,7 +13149,7 @@
       <c r="D412" s="20"/>
       <c r="F412" s="3"/>
     </row>
-    <row r="413" spans="1:6">
+    <row r="413" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A413" s="18" t="s">
         <v>1177</v>
       </c>
@@ -13094,7 +13160,7 @@
       <c r="D413" s="20"/>
       <c r="F413" s="3"/>
     </row>
-    <row r="414" spans="1:6" ht="33.75">
+    <row r="414" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A414" s="18" t="s">
         <v>863</v>
       </c>
@@ -13114,7 +13180,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="415" spans="1:6">
+    <row r="415" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A415" s="18" t="s">
         <v>481</v>
       </c>
@@ -13132,7 +13198,7 @@
       </c>
       <c r="F415" s="3"/>
     </row>
-    <row r="416" spans="1:6">
+    <row r="416" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A416" s="18" t="s">
         <v>1154</v>
       </c>
@@ -13145,7 +13211,7 @@
       <c r="D416" s="20"/>
       <c r="F416" s="3"/>
     </row>
-    <row r="417" spans="1:6">
+    <row r="417" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A417" s="18" t="s">
         <v>160</v>
       </c>
@@ -13163,7 +13229,7 @@
       </c>
       <c r="F417" s="3"/>
     </row>
-    <row r="418" spans="1:6" ht="33.75">
+    <row r="418" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A418" s="18" t="s">
         <v>469</v>
       </c>
@@ -13181,7 +13247,7 @@
       </c>
       <c r="F418" s="3"/>
     </row>
-    <row r="419" spans="1:6">
+    <row r="419" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A419" s="18" t="s">
         <v>568</v>
       </c>
@@ -13199,7 +13265,7 @@
       </c>
       <c r="F419" s="3"/>
     </row>
-    <row r="420" spans="1:6">
+    <row r="420" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A420" s="18" t="s">
         <v>566</v>
       </c>
@@ -13217,7 +13283,7 @@
       </c>
       <c r="F420" s="3"/>
     </row>
-    <row r="421" spans="1:6">
+    <row r="421" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A421" s="18" t="s">
         <v>754</v>
       </c>
@@ -13235,7 +13301,7 @@
       </c>
       <c r="F421" s="3"/>
     </row>
-    <row r="422" spans="1:6">
+    <row r="422" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A422" s="18" t="s">
         <v>567</v>
       </c>
@@ -13253,7 +13319,7 @@
       </c>
       <c r="F422" s="3"/>
     </row>
-    <row r="423" spans="1:6">
+    <row r="423" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A423" s="18" t="s">
         <v>1150</v>
       </c>
@@ -13268,7 +13334,7 @@
       </c>
       <c r="F423" s="3"/>
     </row>
-    <row r="424" spans="1:6">
+    <row r="424" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A424" s="18" t="s">
         <v>548</v>
       </c>
@@ -13286,7 +13352,7 @@
       </c>
       <c r="F424" s="3"/>
     </row>
-    <row r="425" spans="1:6" ht="33">
+    <row r="425" spans="1:6" ht="35" x14ac:dyDescent="0.35">
       <c r="A425" s="18" t="s">
         <v>767</v>
       </c>
@@ -13304,7 +13370,7 @@
       </c>
       <c r="F425" s="3"/>
     </row>
-    <row r="426" spans="1:6" ht="33.75">
+    <row r="426" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A426" s="18" t="s">
         <v>120</v>
       </c>
@@ -13322,7 +13388,7 @@
       </c>
       <c r="F426" s="3"/>
     </row>
-    <row r="427" spans="1:6">
+    <row r="427" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A427" s="18" t="s">
         <v>402</v>
       </c>
@@ -13340,7 +13406,7 @@
       </c>
       <c r="F427" s="3"/>
     </row>
-    <row r="428" spans="1:6">
+    <row r="428" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A428" s="18" t="s">
         <v>298</v>
       </c>
@@ -13358,7 +13424,7 @@
       </c>
       <c r="F428" s="3"/>
     </row>
-    <row r="429" spans="1:6">
+    <row r="429" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A429" s="18" t="s">
         <v>1229</v>
       </c>
@@ -13373,7 +13439,7 @@
       </c>
       <c r="F429" s="3"/>
     </row>
-    <row r="430" spans="1:6">
+    <row r="430" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A430" s="18" t="s">
         <v>48</v>
       </c>
@@ -13391,7 +13457,7 @@
       </c>
       <c r="F430" s="3"/>
     </row>
-    <row r="431" spans="1:6" ht="33">
+    <row r="431" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A431" s="18" t="s">
         <v>169</v>
       </c>
@@ -13409,7 +13475,7 @@
       </c>
       <c r="F431" s="3"/>
     </row>
-    <row r="432" spans="1:6">
+    <row r="432" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A432" s="18" t="s">
         <v>1032</v>
       </c>
@@ -13424,7 +13490,7 @@
       </c>
       <c r="F432" s="3"/>
     </row>
-    <row r="433" spans="1:6" ht="33">
+    <row r="433" spans="1:6" ht="35" x14ac:dyDescent="0.35">
       <c r="A433" s="18" t="s">
         <v>129</v>
       </c>
@@ -13442,7 +13508,7 @@
       </c>
       <c r="F433" s="3"/>
     </row>
-    <row r="434" spans="1:6">
+    <row r="434" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A434" s="18" t="s">
         <v>1035</v>
       </c>
@@ -13457,7 +13523,7 @@
       </c>
       <c r="F434" s="3"/>
     </row>
-    <row r="435" spans="1:6">
+    <row r="435" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A435" s="18" t="s">
         <v>257</v>
       </c>
@@ -13473,7 +13539,7 @@
       </c>
       <c r="F435" s="3"/>
     </row>
-    <row r="436" spans="1:6">
+    <row r="436" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A436" s="18" t="s">
         <v>1377</v>
       </c>
@@ -13491,7 +13557,7 @@
       </c>
       <c r="F436" s="3"/>
     </row>
-    <row r="437" spans="1:6">
+    <row r="437" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A437" s="18" t="s">
         <v>102</v>
       </c>
@@ -13509,7 +13575,7 @@
       </c>
       <c r="F437" s="3"/>
     </row>
-    <row r="438" spans="1:6" ht="33">
+    <row r="438" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A438" s="18" t="s">
         <v>155</v>
       </c>
@@ -13527,7 +13593,7 @@
       </c>
       <c r="F438" s="3"/>
     </row>
-    <row r="439" spans="1:6" ht="45">
+    <row r="439" spans="1:6" ht="36" x14ac:dyDescent="0.35">
       <c r="A439" s="18" t="s">
         <v>775</v>
       </c>
@@ -13545,7 +13611,7 @@
       </c>
       <c r="F439" s="3"/>
     </row>
-    <row r="440" spans="1:6">
+    <row r="440" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A440" s="18" t="s">
         <v>181</v>
       </c>
@@ -13563,7 +13629,7 @@
       </c>
       <c r="F440" s="3"/>
     </row>
-    <row r="441" spans="1:6">
+    <row r="441" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A441" s="18" t="s">
         <v>205</v>
       </c>
@@ -13581,7 +13647,7 @@
       </c>
       <c r="F441" s="3"/>
     </row>
-    <row r="442" spans="1:6">
+    <row r="442" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A442" s="18" t="s">
         <v>1270</v>
       </c>
@@ -13596,7 +13662,7 @@
       </c>
       <c r="F442" s="3"/>
     </row>
-    <row r="443" spans="1:6">
+    <row r="443" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A443" s="18" t="s">
         <v>1047</v>
       </c>
@@ -13611,7 +13677,7 @@
       </c>
       <c r="F443" s="3"/>
     </row>
-    <row r="444" spans="1:6">
+    <row r="444" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A444" s="18" t="s">
         <v>1255</v>
       </c>
@@ -13626,7 +13692,7 @@
       </c>
       <c r="F444" s="3"/>
     </row>
-    <row r="445" spans="1:6" ht="33">
+    <row r="445" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A445" s="18" t="s">
         <v>82</v>
       </c>
@@ -13644,7 +13710,7 @@
       </c>
       <c r="F445" s="3"/>
     </row>
-    <row r="446" spans="1:6" ht="33">
+    <row r="446" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A446" s="18" t="s">
         <v>851</v>
       </c>
@@ -13664,7 +13730,7 @@
         <v>891</v>
       </c>
     </row>
-    <row r="447" spans="1:6" ht="33">
+    <row r="447" spans="1:6" ht="35" x14ac:dyDescent="0.35">
       <c r="A447" s="18" t="s">
         <v>1322</v>
       </c>
@@ -13679,7 +13745,7 @@
       </c>
       <c r="F447" s="3"/>
     </row>
-    <row r="448" spans="1:6" ht="33">
+    <row r="448" spans="1:6" ht="35" x14ac:dyDescent="0.35">
       <c r="A448" s="18" t="s">
         <v>1318</v>
       </c>
@@ -13694,7 +13760,7 @@
       </c>
       <c r="F448" s="3"/>
     </row>
-    <row r="449" spans="1:6">
+    <row r="449" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A449" s="18" t="s">
         <v>870</v>
       </c>
@@ -13714,7 +13780,7 @@
         <v>875</v>
       </c>
     </row>
-    <row r="450" spans="1:6" ht="33">
+    <row r="450" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A450" s="18" t="s">
         <v>365</v>
       </c>
@@ -13732,7 +13798,7 @@
       </c>
       <c r="F450" s="3"/>
     </row>
-    <row r="451" spans="1:6">
+    <row r="451" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A451" s="18" t="s">
         <v>591</v>
       </c>
@@ -13750,7 +13816,7 @@
       </c>
       <c r="F451" s="3"/>
     </row>
-    <row r="452" spans="1:6" ht="33.75">
+    <row r="452" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A452" s="18" t="s">
         <v>794</v>
       </c>
@@ -13768,7 +13834,7 @@
       </c>
       <c r="F452" s="3"/>
     </row>
-    <row r="453" spans="1:6" ht="33">
+    <row r="453" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A453" s="18" t="s">
         <v>1320</v>
       </c>
@@ -13783,7 +13849,7 @@
       </c>
       <c r="F453" s="3"/>
     </row>
-    <row r="454" spans="1:6">
+    <row r="454" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A454" s="18" t="s">
         <v>175</v>
       </c>
@@ -13801,7 +13867,7 @@
       </c>
       <c r="F454" s="3"/>
     </row>
-    <row r="455" spans="1:6">
+    <row r="455" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A455" s="18" t="s">
         <v>496</v>
       </c>
@@ -13819,7 +13885,7 @@
       </c>
       <c r="F455" s="3"/>
     </row>
-    <row r="456" spans="1:6" ht="33.75">
+    <row r="456" spans="1:6" ht="36" x14ac:dyDescent="0.35">
       <c r="A456" s="18" t="s">
         <v>192</v>
       </c>
@@ -13837,7 +13903,7 @@
       </c>
       <c r="F456" s="3"/>
     </row>
-    <row r="457" spans="1:6" ht="33.75">
+    <row r="457" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A457" s="18" t="s">
         <v>860</v>
       </c>
@@ -13857,7 +13923,7 @@
         <v>869</v>
       </c>
     </row>
-    <row r="458" spans="1:6" ht="33">
+    <row r="458" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A458" s="18" t="s">
         <v>1188</v>
       </c>
@@ -13870,7 +13936,7 @@
       </c>
       <c r="F458" s="3"/>
     </row>
-    <row r="459" spans="1:6" ht="78.75">
+    <row r="459" spans="1:6" ht="72" x14ac:dyDescent="0.35">
       <c r="A459" s="18" t="s">
         <v>363</v>
       </c>
@@ -13888,7 +13954,7 @@
       </c>
       <c r="F459" s="3"/>
     </row>
-    <row r="460" spans="1:6">
+    <row r="460" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A460" s="18" t="s">
         <v>1200</v>
       </c>
@@ -13903,7 +13969,7 @@
       </c>
       <c r="F460" s="3"/>
     </row>
-    <row r="461" spans="1:6">
+    <row r="461" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A461" s="18" t="s">
         <v>7</v>
       </c>
@@ -13921,7 +13987,7 @@
       </c>
       <c r="F461" s="3"/>
     </row>
-    <row r="462" spans="1:6">
+    <row r="462" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A462" s="18" t="s">
         <v>306</v>
       </c>
@@ -13939,7 +14005,7 @@
       </c>
       <c r="F462" s="3"/>
     </row>
-    <row r="463" spans="1:6">
+    <row r="463" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A463" s="18" t="s">
         <v>311</v>
       </c>
@@ -13957,7 +14023,7 @@
       </c>
       <c r="F463" s="3"/>
     </row>
-    <row r="464" spans="1:6">
+    <row r="464" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A464" s="18" t="s">
         <v>322</v>
       </c>
@@ -13975,7 +14041,7 @@
       </c>
       <c r="F464" s="3"/>
     </row>
-    <row r="465" spans="1:6" ht="33">
+    <row r="465" spans="1:6" ht="35" x14ac:dyDescent="0.35">
       <c r="A465" s="18" t="s">
         <v>137</v>
       </c>
@@ -13993,7 +14059,7 @@
       </c>
       <c r="F465" s="3"/>
     </row>
-    <row r="466" spans="1:6" ht="48">
+    <row r="466" spans="1:6" ht="35" x14ac:dyDescent="0.35">
       <c r="A466" s="18" t="s">
         <v>341</v>
       </c>
@@ -14011,7 +14077,7 @@
       </c>
       <c r="F466" s="3"/>
     </row>
-    <row r="467" spans="1:6">
+    <row r="467" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A467" s="18" t="s">
         <v>310</v>
       </c>
@@ -14029,7 +14095,7 @@
       </c>
       <c r="F467" s="3"/>
     </row>
-    <row r="468" spans="1:6" ht="33.75">
+    <row r="468" spans="1:6" ht="36" x14ac:dyDescent="0.35">
       <c r="A468" s="18" t="s">
         <v>1240</v>
       </c>
@@ -14044,7 +14110,7 @@
       </c>
       <c r="F468" s="3"/>
     </row>
-    <row r="469" spans="1:6">
+    <row r="469" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A469" s="18" t="s">
         <v>245</v>
       </c>
@@ -14062,7 +14128,7 @@
       </c>
       <c r="F469" s="3"/>
     </row>
-    <row r="470" spans="1:6">
+    <row r="470" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A470" s="18" t="s">
         <v>473</v>
       </c>
@@ -14080,7 +14146,7 @@
       </c>
       <c r="F470" s="3"/>
     </row>
-    <row r="471" spans="1:6">
+    <row r="471" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A471" s="18" t="s">
         <v>86</v>
       </c>
@@ -14098,7 +14164,7 @@
       </c>
       <c r="F471" s="3"/>
     </row>
-    <row r="472" spans="1:6">
+    <row r="472" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A472" s="18" t="s">
         <v>1074</v>
       </c>
@@ -14111,7 +14177,7 @@
       </c>
       <c r="F472" s="3"/>
     </row>
-    <row r="473" spans="1:6">
+    <row r="473" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A473" s="18" t="s">
         <v>893</v>
       </c>
@@ -14131,7 +14197,7 @@
         <v>922</v>
       </c>
     </row>
-    <row r="474" spans="1:6">
+    <row r="474" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A474" s="18" t="s">
         <v>1017</v>
       </c>
@@ -14146,7 +14212,7 @@
       </c>
       <c r="F474" s="3"/>
     </row>
-    <row r="475" spans="1:6">
+    <row r="475" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A475" s="18" t="s">
         <v>1305</v>
       </c>
@@ -14161,7 +14227,7 @@
       </c>
       <c r="F475" s="3"/>
     </row>
-    <row r="476" spans="1:6" ht="33.75">
+    <row r="476" spans="1:6" ht="36" x14ac:dyDescent="0.35">
       <c r="A476" s="18" t="s">
         <v>1421</v>
       </c>
@@ -14176,7 +14242,7 @@
       </c>
       <c r="F476" s="3"/>
     </row>
-    <row r="477" spans="1:6">
+    <row r="477" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A477" s="18" t="s">
         <v>1424</v>
       </c>
@@ -14189,7 +14255,7 @@
       </c>
       <c r="F477" s="3"/>
     </row>
-    <row r="478" spans="1:6">
+    <row r="478" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A478" s="18" t="s">
         <v>1491</v>
       </c>
@@ -14204,7 +14270,7 @@
       </c>
       <c r="F478" s="3"/>
     </row>
-    <row r="479" spans="1:6">
+    <row r="479" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A479" s="18" t="s">
         <v>1493</v>
       </c>
@@ -14219,7 +14285,7 @@
       </c>
       <c r="F479" s="3"/>
     </row>
-    <row r="480" spans="1:6">
+    <row r="480" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A480" s="18" t="s">
         <v>1488</v>
       </c>
@@ -14234,7 +14300,7 @@
       </c>
       <c r="F480" s="3"/>
     </row>
-    <row r="481" spans="1:6" ht="33.75">
+    <row r="481" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A481" s="18" t="s">
         <v>1496</v>
       </c>
@@ -14249,7 +14315,7 @@
       </c>
       <c r="F481" s="3"/>
     </row>
-    <row r="482" spans="1:6" ht="33">
+    <row r="482" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A482" s="18" t="s">
         <v>1026</v>
       </c>
@@ -14262,7 +14328,7 @@
       </c>
       <c r="F482" s="3"/>
     </row>
-    <row r="483" spans="1:6">
+    <row r="483" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A483" s="18" t="s">
         <v>1502</v>
       </c>
@@ -14275,7 +14341,7 @@
       </c>
       <c r="F483" s="3"/>
     </row>
-    <row r="484" spans="1:6">
+    <row r="484" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A484" s="18" t="s">
         <v>1505</v>
       </c>
@@ -14288,7 +14354,7 @@
       </c>
       <c r="F484" s="3"/>
     </row>
-    <row r="485" spans="1:6">
+    <row r="485" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A485" s="18" t="s">
         <v>1508</v>
       </c>
@@ -14301,7 +14367,7 @@
       </c>
       <c r="F485" s="3"/>
     </row>
-    <row r="486" spans="1:6" ht="33.75">
+    <row r="486" spans="1:6" ht="36" x14ac:dyDescent="0.35">
       <c r="A486" s="18" t="s">
         <v>1516</v>
       </c>
@@ -14316,7 +14382,7 @@
       </c>
       <c r="F486" s="3"/>
     </row>
-    <row r="487" spans="1:6">
+    <row r="487" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A487" s="18" t="s">
         <v>1519</v>
       </c>
@@ -14331,7 +14397,7 @@
       </c>
       <c r="F487" s="3"/>
     </row>
-    <row r="488" spans="1:6" ht="30">
+    <row r="488" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A488" s="17" t="s">
         <v>1525</v>
       </c>
@@ -14346,7 +14412,7 @@
       </c>
       <c r="F488" s="3"/>
     </row>
-    <row r="489" spans="1:6" ht="33.75">
+    <row r="489" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A489" s="18" t="s">
         <v>1524</v>
       </c>
@@ -14361,7 +14427,7 @@
       </c>
       <c r="F489" s="3"/>
     </row>
-    <row r="490" spans="1:6">
+    <row r="490" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A490" s="18" t="s">
         <v>1528</v>
       </c>
@@ -14376,7 +14442,7 @@
       </c>
       <c r="F490" s="3"/>
     </row>
-    <row r="491" spans="1:6" ht="33.75">
+    <row r="491" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A491" s="18" t="s">
         <v>1529</v>
       </c>
@@ -14391,7 +14457,7 @@
       </c>
       <c r="F491" s="3"/>
     </row>
-    <row r="492" spans="1:6" ht="33.75">
+    <row r="492" spans="1:6" ht="36" x14ac:dyDescent="0.35">
       <c r="A492" s="18" t="s">
         <v>1535</v>
       </c>
@@ -14406,7 +14472,7 @@
       </c>
       <c r="F492" s="3"/>
     </row>
-    <row r="493" spans="1:6">
+    <row r="493" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A493" s="18" t="s">
         <v>1539</v>
       </c>
@@ -14421,7 +14487,7 @@
       </c>
       <c r="F493" s="3"/>
     </row>
-    <row r="494" spans="1:6">
+    <row r="494" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A494" s="18" t="s">
         <v>1541</v>
       </c>
@@ -14434,7 +14500,7 @@
       <c r="D494" s="20"/>
       <c r="F494" s="3"/>
     </row>
-    <row r="495" spans="1:6">
+    <row r="495" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A495" s="18" t="s">
         <v>1543</v>
       </c>
@@ -14447,7 +14513,7 @@
       <c r="D495" s="20"/>
       <c r="F495" s="3"/>
     </row>
-    <row r="496" spans="1:6">
+    <row r="496" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A496" s="18" t="s">
         <v>1545</v>
       </c>
@@ -14460,7 +14526,7 @@
       <c r="D496" s="20"/>
       <c r="F496" s="3"/>
     </row>
-    <row r="497" spans="1:6">
+    <row r="497" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A497" s="18" t="s">
         <v>1547</v>
       </c>
@@ -14473,7 +14539,7 @@
       <c r="D497" s="20"/>
       <c r="F497" s="3"/>
     </row>
-    <row r="498" spans="1:6">
+    <row r="498" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A498" s="18" t="s">
         <v>1564</v>
       </c>
@@ -14486,7 +14552,7 @@
       <c r="D498" s="20"/>
       <c r="F498" s="3"/>
     </row>
-    <row r="499" spans="1:6">
+    <row r="499" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A499" s="18" t="s">
         <v>1562</v>
       </c>
@@ -14499,7 +14565,7 @@
       <c r="D499" s="20"/>
       <c r="F499" s="3"/>
     </row>
-    <row r="500" spans="1:6">
+    <row r="500" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A500" s="18" t="s">
         <v>1560</v>
       </c>
@@ -14512,7 +14578,7 @@
       <c r="D500" s="20"/>
       <c r="F500" s="3"/>
     </row>
-    <row r="501" spans="1:6">
+    <row r="501" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A501" s="18" t="s">
         <v>1558</v>
       </c>
@@ -14525,7 +14591,7 @@
       <c r="D501" s="20"/>
       <c r="F501" s="3"/>
     </row>
-    <row r="502" spans="1:6">
+    <row r="502" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A502" s="18" t="s">
         <v>1556</v>
       </c>
@@ -14538,7 +14604,7 @@
       <c r="D502" s="20"/>
       <c r="F502" s="3"/>
     </row>
-    <row r="503" spans="1:6">
+    <row r="503" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A503" s="18" t="s">
         <v>1553</v>
       </c>
@@ -14553,7 +14619,7 @@
       </c>
       <c r="F503" s="3"/>
     </row>
-    <row r="504" spans="1:6" ht="33">
+    <row r="504" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A504" s="18" t="s">
         <v>1551</v>
       </c>
@@ -14566,7 +14632,7 @@
       <c r="D504" s="20"/>
       <c r="F504" s="3"/>
     </row>
-    <row r="505" spans="1:6">
+    <row r="505" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A505" s="18" t="s">
         <v>1549</v>
       </c>
@@ -14581,33 +14647,125 @@
       </c>
       <c r="F505" s="3"/>
     </row>
-    <row r="506" spans="1:6" ht="33">
-      <c r="A506" s="24" t="s">
+    <row r="506" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A506" s="18" t="s">
         <v>1566</v>
       </c>
-      <c r="B506" s="25" t="s">
+      <c r="B506" s="17" t="s">
         <v>1567</v>
       </c>
-      <c r="C506" s="26" t="s">
+      <c r="C506" s="3" t="s">
         <v>316</v>
       </c>
-      <c r="D506" s="27"/>
-      <c r="E506" s="26"/>
-      <c r="F506" s="26"/>
-    </row>
-    <row r="507" spans="1:6" ht="114">
-      <c r="A507" s="28" t="s">
+      <c r="D506" s="20"/>
+      <c r="F506" s="3"/>
+    </row>
+    <row r="507" spans="1:6" ht="120" x14ac:dyDescent="0.35">
+      <c r="A507" s="24" t="s">
         <v>1568</v>
       </c>
-      <c r="B507" s="25" t="s">
+      <c r="B507" s="17" t="s">
         <v>1569</v>
       </c>
-      <c r="C507" s="26" t="s">
+      <c r="C507" s="3" t="s">
         <v>316</v>
       </c>
-      <c r="D507" s="27"/>
-      <c r="E507" s="26"/>
-      <c r="F507" s="26"/>
+      <c r="D507" s="20"/>
+      <c r="F507" s="3"/>
+    </row>
+    <row r="508" spans="1:6" ht="36" x14ac:dyDescent="0.35">
+      <c r="A508" s="25" t="s">
+        <v>1570</v>
+      </c>
+      <c r="B508" s="26" t="s">
+        <v>1571</v>
+      </c>
+      <c r="C508" s="27" t="s">
+        <v>113</v>
+      </c>
+      <c r="D508" s="28" t="s">
+        <v>1572</v>
+      </c>
+      <c r="E508" s="27"/>
+      <c r="F508" s="27"/>
+    </row>
+    <row r="509" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A509" s="25" t="s">
+        <v>1573</v>
+      </c>
+      <c r="B509" s="26" t="s">
+        <v>1574</v>
+      </c>
+      <c r="C509" s="27" t="s">
+        <v>113</v>
+      </c>
+      <c r="D509" s="28" t="s">
+        <v>1575</v>
+      </c>
+      <c r="E509" s="27"/>
+      <c r="F509" s="27"/>
+    </row>
+    <row r="510" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A510" s="25" t="s">
+        <v>1576</v>
+      </c>
+      <c r="B510" s="26" t="s">
+        <v>1577</v>
+      </c>
+      <c r="C510" s="27" t="s">
+        <v>113</v>
+      </c>
+      <c r="D510" s="28" t="s">
+        <v>1578</v>
+      </c>
+      <c r="E510" s="27"/>
+      <c r="F510" s="27"/>
+    </row>
+    <row r="511" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A511" s="25" t="s">
+        <v>1579</v>
+      </c>
+      <c r="B511" s="26" t="s">
+        <v>1580</v>
+      </c>
+      <c r="C511" s="27" t="s">
+        <v>1581</v>
+      </c>
+      <c r="D511" s="28" t="s">
+        <v>1582</v>
+      </c>
+      <c r="E511" s="27"/>
+      <c r="F511" s="27"/>
+    </row>
+    <row r="512" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A512" s="25" t="s">
+        <v>1583</v>
+      </c>
+      <c r="B512" s="29" t="s">
+        <v>1584</v>
+      </c>
+      <c r="C512" s="27" t="s">
+        <v>113</v>
+      </c>
+      <c r="D512" s="28" t="s">
+        <v>1585</v>
+      </c>
+      <c r="E512" s="27"/>
+      <c r="F512" s="27"/>
+    </row>
+    <row r="513" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A513" s="25" t="s">
+        <v>1586</v>
+      </c>
+      <c r="B513" s="26" t="s">
+        <v>1588</v>
+      </c>
+      <c r="C513" s="27"/>
+      <c r="D513" s="28" t="s">
+        <v>1587</v>
+      </c>
+      <c r="E513" s="27"/>
+      <c r="F513" s="27"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:D276">

</xml_diff>

<commit_message>
all work and no fun
</commit_message>
<xml_diff>
--- a/abkuerzungen.xlsx
+++ b/abkuerzungen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\markdown\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5F62823-6E3E-4257-B02E-4F88CDB4C70E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F9C48A1-E5FD-49DA-9BF3-3C3090663E9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="28800" windowHeight="15495" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="345" yWindow="660" windowWidth="16365" windowHeight="15285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -6793,10 +6793,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:XFD579"/>
+  <dimension ref="A1:XFD577"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A275" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A289" sqref="A289"/>
+    <sheetView tabSelected="1" topLeftCell="A240" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B376" sqref="B376"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="28.5"/>
@@ -12314,7 +12314,7 @@
       <c r="F271" s="25"/>
       <c r="G271" s="25"/>
     </row>
-    <row r="272" spans="1:7" customFormat="1" ht="90">
+    <row r="272" spans="1:7" ht="90">
       <c r="A272" s="23" t="s">
         <v>96</v>
       </c>
@@ -12335,7 +12335,7 @@
       </c>
       <c r="G272" s="25"/>
     </row>
-    <row r="273" spans="1:7" customFormat="1" ht="30">
+    <row r="273" spans="1:7" ht="30">
       <c r="A273" s="23" t="s">
         <v>15</v>
       </c>
@@ -12356,7 +12356,7 @@
       </c>
       <c r="G273" s="25"/>
     </row>
-    <row r="274" spans="1:7" customFormat="1">
+    <row r="274" spans="1:7">
       <c r="A274" s="23" t="s">
         <v>1175</v>
       </c>
@@ -12373,7 +12373,7 @@
       <c r="F274" s="25"/>
       <c r="G274" s="25"/>
     </row>
-    <row r="275" spans="1:7" customFormat="1" ht="30">
+    <row r="275" spans="1:7" ht="30">
       <c r="A275" s="23" t="s">
         <v>553</v>
       </c>
@@ -12392,7 +12392,7 @@
       </c>
       <c r="G275" s="25"/>
     </row>
-    <row r="276" spans="1:7" customFormat="1">
+    <row r="276" spans="1:7">
       <c r="A276" s="23" t="s">
         <v>1304</v>
       </c>
@@ -12411,7 +12411,7 @@
       <c r="F276" s="25"/>
       <c r="G276" s="25"/>
     </row>
-    <row r="277" spans="1:7" customFormat="1">
+    <row r="277" spans="1:7">
       <c r="A277" s="23" t="s">
         <v>126</v>
       </c>
@@ -12432,7 +12432,7 @@
       </c>
       <c r="G277" s="25"/>
     </row>
-    <row r="278" spans="1:7" customFormat="1" ht="30">
+    <row r="278" spans="1:7" ht="30">
       <c r="A278" s="23" t="s">
         <v>765</v>
       </c>
@@ -12451,7 +12451,7 @@
       </c>
       <c r="G278" s="25"/>
     </row>
-    <row r="279" spans="1:7" customFormat="1">
+    <row r="279" spans="1:7">
       <c r="A279" s="23" t="s">
         <v>1067</v>
       </c>
@@ -12470,7 +12470,7 @@
       <c r="F279" s="25"/>
       <c r="G279" s="25"/>
     </row>
-    <row r="280" spans="1:7" customFormat="1" ht="30">
+    <row r="280" spans="1:7" ht="30">
       <c r="A280" s="23" t="s">
         <v>124</v>
       </c>
@@ -12491,7 +12491,7 @@
       </c>
       <c r="G280" s="25"/>
     </row>
-    <row r="281" spans="1:7" customFormat="1" ht="30">
+    <row r="281" spans="1:7" ht="30">
       <c r="A281" s="23" t="s">
         <v>890</v>
       </c>
@@ -12514,7 +12514,7 @@
         <v>915</v>
       </c>
     </row>
-    <row r="282" spans="1:7" customFormat="1" ht="45">
+    <row r="282" spans="1:7" ht="45">
       <c r="A282" s="23" t="s">
         <v>1543</v>
       </c>
@@ -12533,7 +12533,7 @@
       <c r="F282" s="25"/>
       <c r="G282" s="25"/>
     </row>
-    <row r="283" spans="1:7" customFormat="1" ht="45">
+    <row r="283" spans="1:7" ht="45">
       <c r="A283" s="23" t="s">
         <v>1062</v>
       </c>
@@ -12550,7 +12550,7 @@
       <c r="F283" s="25"/>
       <c r="G283" s="25"/>
     </row>
-    <row r="284" spans="1:7" customFormat="1" ht="45">
+    <row r="284" spans="1:7" ht="45">
       <c r="A284" s="23" t="s">
         <v>802</v>
       </c>
@@ -12571,7 +12571,7 @@
       </c>
       <c r="G284" s="25"/>
     </row>
-    <row r="285" spans="1:7" customFormat="1">
+    <row r="285" spans="1:7">
       <c r="A285" s="23" t="s">
         <v>282</v>
       </c>
@@ -12592,7 +12592,7 @@
       </c>
       <c r="G285" s="25"/>
     </row>
-    <row r="286" spans="1:7" customFormat="1">
+    <row r="286" spans="1:7">
       <c r="A286" s="23" t="s">
         <v>3</v>
       </c>
@@ -12613,7 +12613,7 @@
       </c>
       <c r="G286" s="25"/>
     </row>
-    <row r="287" spans="1:7" customFormat="1" ht="45">
+    <row r="287" spans="1:7" ht="45">
       <c r="A287" s="23" t="s">
         <v>416</v>
       </c>
@@ -12634,7 +12634,7 @@
       </c>
       <c r="G287" s="25"/>
     </row>
-    <row r="288" spans="1:7" customFormat="1" ht="33.75">
+    <row r="288" spans="1:7" ht="33.75">
       <c r="A288" s="23" t="s">
         <v>1626</v>
       </c>
@@ -12653,7 +12653,7 @@
       <c r="F288" s="25"/>
       <c r="G288" s="25"/>
     </row>
-    <row r="289" spans="1:7" customFormat="1" ht="33.75">
+    <row r="289" spans="1:7" ht="33.75">
       <c r="A289" s="23" t="s">
         <v>1642</v>
       </c>
@@ -12672,7 +12672,7 @@
       <c r="F289" s="25"/>
       <c r="G289" s="25"/>
     </row>
-    <row r="290" spans="1:7" customFormat="1" ht="33.75">
+    <row r="290" spans="1:7" ht="33.75">
       <c r="A290" s="23" t="s">
         <v>367</v>
       </c>
@@ -12691,7 +12691,7 @@
       </c>
       <c r="G290" s="25"/>
     </row>
-    <row r="291" spans="1:7" customFormat="1">
+    <row r="291" spans="1:7">
       <c r="A291" s="23" t="s">
         <v>285</v>
       </c>
@@ -12712,7 +12712,7 @@
       </c>
       <c r="G291" s="25"/>
     </row>
-    <row r="292" spans="1:7" customFormat="1" ht="30">
+    <row r="292" spans="1:7" ht="30">
       <c r="A292" s="23" t="s">
         <v>206</v>
       </c>
@@ -12733,7 +12733,7 @@
       </c>
       <c r="G292" s="25"/>
     </row>
-    <row r="293" spans="1:7" customFormat="1">
+    <row r="293" spans="1:7">
       <c r="A293" s="23" t="s">
         <v>72</v>
       </c>
@@ -12754,7 +12754,7 @@
       </c>
       <c r="G293" s="25"/>
     </row>
-    <row r="294" spans="1:7" customFormat="1" ht="45">
+    <row r="294" spans="1:7" ht="45">
       <c r="A294" s="23" t="s">
         <v>1186</v>
       </c>
@@ -12773,7 +12773,7 @@
       <c r="F294" s="25"/>
       <c r="G294" s="25"/>
     </row>
-    <row r="295" spans="1:7" customFormat="1" ht="45">
+    <row r="295" spans="1:7" ht="45">
       <c r="A295" s="23" t="s">
         <v>1196</v>
       </c>
@@ -12792,7 +12792,7 @@
       <c r="F295" s="25"/>
       <c r="G295" s="25"/>
     </row>
-    <row r="296" spans="1:7" customFormat="1" ht="30">
+    <row r="296" spans="1:7" ht="30">
       <c r="A296" s="23" t="s">
         <v>121</v>
       </c>
@@ -12813,7 +12813,7 @@
       </c>
       <c r="G296" s="25"/>
     </row>
-    <row r="297" spans="1:7" customFormat="1" ht="30">
+    <row r="297" spans="1:7" ht="30">
       <c r="A297" s="23" t="s">
         <v>874</v>
       </c>
@@ -12836,7 +12836,7 @@
         <v>880</v>
       </c>
     </row>
-    <row r="298" spans="1:7" customFormat="1" ht="33.75">
+    <row r="298" spans="1:7" ht="33.75">
       <c r="A298" s="23" t="s">
         <v>198</v>
       </c>
@@ -12857,7 +12857,7 @@
       </c>
       <c r="G298" s="25"/>
     </row>
-    <row r="299" spans="1:7" customFormat="1" ht="45">
+    <row r="299" spans="1:7" ht="45">
       <c r="A299" s="23" t="s">
         <v>1132</v>
       </c>
@@ -12876,7 +12876,7 @@
       <c r="F299" s="25"/>
       <c r="G299" s="25"/>
     </row>
-    <row r="300" spans="1:7" customFormat="1" ht="30">
+    <row r="300" spans="1:7" ht="30">
       <c r="A300" s="23" t="s">
         <v>6</v>
       </c>
@@ -12895,7 +12895,7 @@
       </c>
       <c r="G300" s="25"/>
     </row>
-    <row r="301" spans="1:7" customFormat="1" ht="45">
+    <row r="301" spans="1:7" ht="45">
       <c r="A301" s="23" t="s">
         <v>164</v>
       </c>
@@ -12916,7 +12916,7 @@
       </c>
       <c r="G301" s="25"/>
     </row>
-    <row r="302" spans="1:7" customFormat="1" ht="56.25">
+    <row r="302" spans="1:7" ht="56.25">
       <c r="A302" s="23" t="s">
         <v>456</v>
       </c>
@@ -12935,7 +12935,7 @@
       </c>
       <c r="G302" s="25"/>
     </row>
-    <row r="303" spans="1:7" customFormat="1" ht="56.25">
+    <row r="303" spans="1:7" ht="56.25">
       <c r="A303" s="23" t="s">
         <v>458</v>
       </c>
@@ -12954,7 +12954,7 @@
       </c>
       <c r="G303" s="25"/>
     </row>
-    <row r="304" spans="1:7" customFormat="1" ht="30">
+    <row r="304" spans="1:7" ht="30">
       <c r="A304" s="23" t="s">
         <v>1697</v>
       </c>
@@ -12973,7 +12973,7 @@
       <c r="F304" s="25"/>
       <c r="G304" s="25"/>
     </row>
-    <row r="305" spans="1:7" customFormat="1" ht="30">
+    <row r="305" spans="1:7" ht="30">
       <c r="A305" s="23" t="s">
         <v>460</v>
       </c>
@@ -12992,7 +12992,7 @@
       </c>
       <c r="G305" s="25"/>
     </row>
-    <row r="306" spans="1:7" customFormat="1" ht="30">
+    <row r="306" spans="1:7" ht="30">
       <c r="A306" s="23" t="s">
         <v>408</v>
       </c>
@@ -13011,7 +13011,7 @@
       </c>
       <c r="G306" s="25"/>
     </row>
-    <row r="307" spans="1:7" customFormat="1" ht="30">
+    <row r="307" spans="1:7" ht="30">
       <c r="A307" s="23" t="s">
         <v>240</v>
       </c>
@@ -13032,7 +13032,7 @@
       </c>
       <c r="G307" s="25"/>
     </row>
-    <row r="308" spans="1:7" customFormat="1">
+    <row r="308" spans="1:7">
       <c r="A308" s="23" t="s">
         <v>1495</v>
       </c>
@@ -13051,7 +13051,7 @@
       <c r="F308" s="25"/>
       <c r="G308" s="25"/>
     </row>
-    <row r="309" spans="1:7" customFormat="1">
+    <row r="309" spans="1:7">
       <c r="A309" s="23" t="s">
         <v>471</v>
       </c>
@@ -13070,7 +13070,7 @@
       </c>
       <c r="G309" s="25"/>
     </row>
-    <row r="310" spans="1:7" customFormat="1">
+    <row r="310" spans="1:7">
       <c r="A310" s="23" t="s">
         <v>1276</v>
       </c>
@@ -13089,7 +13089,7 @@
       <c r="F310" s="25"/>
       <c r="G310" s="25"/>
     </row>
-    <row r="311" spans="1:7" customFormat="1" ht="30">
+    <row r="311" spans="1:7" ht="30">
       <c r="A311" s="23" t="s">
         <v>403</v>
       </c>
@@ -13108,7 +13108,7 @@
       </c>
       <c r="G311" s="25"/>
     </row>
-    <row r="312" spans="1:7" customFormat="1" ht="90">
+    <row r="312" spans="1:7" ht="90">
       <c r="A312" s="23" t="s">
         <v>751</v>
       </c>
@@ -13127,7 +13127,7 @@
       </c>
       <c r="G312" s="25"/>
     </row>
-    <row r="313" spans="1:7" customFormat="1" ht="33.75">
+    <row r="313" spans="1:7" ht="33.75">
       <c r="A313" s="23" t="s">
         <v>1243</v>
       </c>
@@ -13146,7 +13146,7 @@
       <c r="F313" s="25"/>
       <c r="G313" s="25"/>
     </row>
-    <row r="314" spans="1:7" customFormat="1" ht="45">
+    <row r="314" spans="1:7" ht="45">
       <c r="A314" s="23" t="s">
         <v>461</v>
       </c>
@@ -13165,7 +13165,7 @@
       </c>
       <c r="G314" s="25"/>
     </row>
-    <row r="315" spans="1:7" customFormat="1" ht="45">
+    <row r="315" spans="1:7" ht="45">
       <c r="A315" s="23" t="s">
         <v>446</v>
       </c>
@@ -13186,7 +13186,7 @@
       </c>
       <c r="G315" s="25"/>
     </row>
-    <row r="316" spans="1:7" customFormat="1" ht="45">
+    <row r="316" spans="1:7" ht="45">
       <c r="A316" s="23" t="s">
         <v>442</v>
       </c>
@@ -13205,7 +13205,7 @@
       <c r="F316" s="25"/>
       <c r="G316" s="25"/>
     </row>
-    <row r="317" spans="1:7" customFormat="1" ht="45">
+    <row r="317" spans="1:7" ht="45">
       <c r="A317" s="23" t="s">
         <v>1192</v>
       </c>
@@ -13224,7 +13224,7 @@
       <c r="F317" s="25"/>
       <c r="G317" s="25"/>
     </row>
-    <row r="318" spans="1:7" customFormat="1" ht="30">
+    <row r="318" spans="1:7" ht="30">
       <c r="A318" s="23" t="s">
         <v>114</v>
       </c>
@@ -13245,7 +13245,7 @@
       </c>
       <c r="G318" s="25"/>
     </row>
-    <row r="319" spans="1:7" customFormat="1" ht="30">
+    <row r="319" spans="1:7" ht="30">
       <c r="A319" s="23" t="s">
         <v>385</v>
       </c>
@@ -13266,7 +13266,7 @@
       </c>
       <c r="G319" s="25"/>
     </row>
-    <row r="320" spans="1:7" customFormat="1" ht="45">
+    <row r="320" spans="1:7" ht="45">
       <c r="A320" s="29" t="s">
         <v>1539</v>
       </c>
@@ -13285,7 +13285,7 @@
       <c r="F320" s="25"/>
       <c r="G320" s="25"/>
     </row>
-    <row r="321" spans="1:7" customFormat="1" ht="30">
+    <row r="321" spans="1:7" ht="30">
       <c r="A321" s="23" t="s">
         <v>1146</v>
       </c>
@@ -13300,7 +13300,7 @@
       <c r="F321" s="25"/>
       <c r="G321" s="25"/>
     </row>
-    <row r="322" spans="1:7" customFormat="1" ht="33.75">
+    <row r="322" spans="1:7" ht="33.75">
       <c r="A322" s="23" t="s">
         <v>1604</v>
       </c>
@@ -13319,7 +13319,7 @@
       <c r="F322" s="25"/>
       <c r="G322" s="25"/>
     </row>
-    <row r="323" spans="1:7" customFormat="1">
+    <row r="323" spans="1:7">
       <c r="A323" s="23" t="s">
         <v>242</v>
       </c>
@@ -13340,7 +13340,7 @@
       </c>
       <c r="G323" s="25"/>
     </row>
-    <row r="324" spans="1:7" customFormat="1" ht="30">
+    <row r="324" spans="1:7" ht="30">
       <c r="A324" s="23" t="s">
         <v>1632</v>
       </c>
@@ -13359,7 +13359,7 @@
       <c r="F324" s="25"/>
       <c r="G324" s="25"/>
     </row>
-    <row r="325" spans="1:7" customFormat="1" ht="30">
+    <row r="325" spans="1:7" ht="30">
       <c r="A325" s="23" t="s">
         <v>0</v>
       </c>
@@ -13380,7 +13380,7 @@
       </c>
       <c r="G325" s="25"/>
     </row>
-    <row r="326" spans="1:7" customFormat="1" ht="30">
+    <row r="326" spans="1:7" ht="30">
       <c r="A326" s="23" t="s">
         <v>196</v>
       </c>
@@ -13401,7 +13401,7 @@
       </c>
       <c r="G326" s="25"/>
     </row>
-    <row r="327" spans="1:7" customFormat="1" ht="69.75">
+    <row r="327" spans="1:7" ht="69.75">
       <c r="A327" s="30" t="s">
         <v>1743</v>
       </c>
@@ -13420,7 +13420,7 @@
       <c r="F327" s="25"/>
       <c r="G327" s="25"/>
     </row>
-    <row r="328" spans="1:7" customFormat="1">
+    <row r="328" spans="1:7">
       <c r="A328" s="23" t="s">
         <v>1139</v>
       </c>
@@ -13433,7 +13433,7 @@
       <c r="F328" s="25"/>
       <c r="G328" s="25"/>
     </row>
-    <row r="329" spans="1:7" customFormat="1" ht="30">
+    <row r="329" spans="1:7" ht="30">
       <c r="A329" s="23" t="s">
         <v>1599</v>
       </c>
@@ -13452,7 +13452,7 @@
       <c r="F329" s="25"/>
       <c r="G329" s="25"/>
     </row>
-    <row r="330" spans="1:7" customFormat="1" ht="33.75">
+    <row r="330" spans="1:7" ht="33.75">
       <c r="A330" s="23" t="s">
         <v>1411</v>
       </c>
@@ -13471,7 +13471,7 @@
       <c r="F330" s="25"/>
       <c r="G330" s="25"/>
     </row>
-    <row r="331" spans="1:7" customFormat="1" ht="56.25">
+    <row r="331" spans="1:7" ht="56.25">
       <c r="A331" s="23" t="s">
         <v>1352</v>
       </c>
@@ -13494,7 +13494,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="332" spans="1:7" customFormat="1" ht="45">
+    <row r="332" spans="1:7" ht="45">
       <c r="A332" s="23" t="s">
         <v>234</v>
       </c>
@@ -13515,7 +13515,7 @@
       </c>
       <c r="G332" s="25"/>
     </row>
-    <row r="333" spans="1:7" customFormat="1">
+    <row r="333" spans="1:7">
       <c r="A333" s="23" t="s">
         <v>1565</v>
       </c>
@@ -13534,7 +13534,7 @@
       <c r="F333" s="25"/>
       <c r="G333" s="25"/>
     </row>
-    <row r="334" spans="1:7" customFormat="1">
+    <row r="334" spans="1:7">
       <c r="A334" s="23" t="s">
         <v>1565</v>
       </c>
@@ -13551,7 +13551,7 @@
       <c r="F334" s="25"/>
       <c r="G334" s="25"/>
     </row>
-    <row r="335" spans="1:7" customFormat="1" ht="33.75">
+    <row r="335" spans="1:7" ht="33.75">
       <c r="A335" s="23" t="s">
         <v>148</v>
       </c>
@@ -13572,7 +13572,7 @@
       </c>
       <c r="G335" s="25"/>
     </row>
-    <row r="336" spans="1:7" customFormat="1" ht="30">
+    <row r="336" spans="1:7" ht="30">
       <c r="A336" s="23" t="s">
         <v>221</v>
       </c>
@@ -13593,7 +13593,7 @@
       </c>
       <c r="G336" s="25"/>
     </row>
-    <row r="337" spans="1:7" customFormat="1" ht="33.75">
+    <row r="337" spans="1:7" ht="33.75">
       <c r="A337" s="23" t="s">
         <v>1137</v>
       </c>
@@ -13612,7 +13612,7 @@
       <c r="F337" s="25"/>
       <c r="G337" s="25"/>
     </row>
-    <row r="338" spans="1:7" customFormat="1" ht="30">
+    <row r="338" spans="1:7" ht="30">
       <c r="A338" s="23" t="s">
         <v>1519</v>
       </c>
@@ -13631,7 +13631,7 @@
       <c r="F338" s="25"/>
       <c r="G338" s="25"/>
     </row>
-    <row r="339" spans="1:7" customFormat="1">
+    <row r="339" spans="1:7">
       <c r="A339" s="23" t="s">
         <v>233</v>
       </c>
@@ -13650,7 +13650,7 @@
       </c>
       <c r="G339" s="25"/>
     </row>
-    <row r="340" spans="1:7" customFormat="1" ht="30">
+    <row r="340" spans="1:7" ht="30">
       <c r="A340" s="23" t="s">
         <v>210</v>
       </c>
@@ -13671,7 +13671,7 @@
       </c>
       <c r="G340" s="25"/>
     </row>
-    <row r="341" spans="1:7" customFormat="1" ht="45">
+    <row r="341" spans="1:7" ht="45">
       <c r="A341" s="23" t="s">
         <v>230</v>
       </c>
@@ -13692,7 +13692,7 @@
       </c>
       <c r="G341" s="25"/>
     </row>
-    <row r="342" spans="1:7" customFormat="1" ht="30">
+    <row r="342" spans="1:7" ht="30">
       <c r="A342" s="23" t="s">
         <v>289</v>
       </c>
@@ -13713,7 +13713,7 @@
       </c>
       <c r="G342" s="25"/>
     </row>
-    <row r="343" spans="1:7" customFormat="1" ht="30">
+    <row r="343" spans="1:7" ht="30">
       <c r="A343" s="23" t="s">
         <v>157</v>
       </c>
@@ -13734,7 +13734,7 @@
       </c>
       <c r="G343" s="25"/>
     </row>
-    <row r="344" spans="1:7" customFormat="1" ht="30">
+    <row r="344" spans="1:7" ht="30">
       <c r="A344" s="23" t="s">
         <v>1531</v>
       </c>
@@ -13751,7 +13751,7 @@
       <c r="F344" s="25"/>
       <c r="G344" s="25"/>
     </row>
-    <row r="345" spans="1:7" customFormat="1">
+    <row r="345" spans="1:7">
       <c r="A345" s="23" t="s">
         <v>44</v>
       </c>
@@ -13772,7 +13772,7 @@
       </c>
       <c r="G345" s="25"/>
     </row>
-    <row r="346" spans="1:7" customFormat="1" ht="45">
+    <row r="346" spans="1:7" ht="45">
       <c r="A346" s="23" t="s">
         <v>487</v>
       </c>
@@ -13793,7 +13793,7 @@
       </c>
       <c r="G346" s="25"/>
     </row>
-    <row r="347" spans="1:7" customFormat="1" ht="30">
+    <row r="347" spans="1:7" ht="30">
       <c r="A347" s="23" t="s">
         <v>1268</v>
       </c>
@@ -13812,7 +13812,7 @@
       <c r="F347" s="25"/>
       <c r="G347" s="25"/>
     </row>
-    <row r="348" spans="1:7" customFormat="1" ht="30">
+    <row r="348" spans="1:7" ht="30">
       <c r="A348" s="23" t="s">
         <v>1354</v>
       </c>
@@ -13833,7 +13833,7 @@
       </c>
       <c r="G348" s="25"/>
     </row>
-    <row r="349" spans="1:7" customFormat="1" ht="30">
+    <row r="349" spans="1:7" ht="30">
       <c r="A349" s="23" t="s">
         <v>1646</v>
       </c>
@@ -13852,7 +13852,7 @@
       <c r="F349" s="25"/>
       <c r="G349" s="25"/>
     </row>
-    <row r="350" spans="1:7" customFormat="1" ht="33.75">
+    <row r="350" spans="1:7" ht="33.75">
       <c r="A350" s="23" t="s">
         <v>1355</v>
       </c>
@@ -13873,7 +13873,7 @@
       </c>
       <c r="G350" s="25"/>
     </row>
-    <row r="351" spans="1:7" customFormat="1" ht="33.75">
+    <row r="351" spans="1:7" ht="33.75">
       <c r="A351" s="23" t="s">
         <v>238</v>
       </c>
@@ -13894,7 +13894,7 @@
       </c>
       <c r="G351" s="25"/>
     </row>
-    <row r="352" spans="1:7" customFormat="1" ht="30">
+    <row r="352" spans="1:7" ht="30">
       <c r="A352" s="23" t="s">
         <v>1016</v>
       </c>
@@ -13913,7 +13913,7 @@
       <c r="F352" s="25"/>
       <c r="G352" s="25"/>
     </row>
-    <row r="353" spans="1:7" customFormat="1" ht="30">
+    <row r="353" spans="1:7" ht="30">
       <c r="A353" s="23" t="s">
         <v>463</v>
       </c>
@@ -13934,7 +13934,7 @@
       </c>
       <c r="G353" s="25"/>
     </row>
-    <row r="354" spans="1:7" customFormat="1" ht="33.75">
+    <row r="354" spans="1:7" ht="33.75">
       <c r="A354" s="23" t="s">
         <v>1252</v>
       </c>
@@ -13953,7 +13953,7 @@
       <c r="F354" s="25"/>
       <c r="G354" s="25"/>
     </row>
-    <row r="355" spans="1:7" customFormat="1">
+    <row r="355" spans="1:7">
       <c r="A355" s="23" t="s">
         <v>1245</v>
       </c>
@@ -13972,7 +13972,7 @@
       <c r="F355" s="25"/>
       <c r="G355" s="25"/>
     </row>
-    <row r="356" spans="1:7" customFormat="1">
+    <row r="356" spans="1:7">
       <c r="A356" s="23" t="s">
         <v>1583</v>
       </c>
@@ -13991,7 +13991,7 @@
       <c r="F356" s="25"/>
       <c r="G356" s="25"/>
     </row>
-    <row r="357" spans="1:7" customFormat="1" ht="30">
+    <row r="357" spans="1:7" ht="30">
       <c r="A357" s="23" t="s">
         <v>170</v>
       </c>
@@ -14012,7 +14012,7 @@
       </c>
       <c r="G357" s="25"/>
     </row>
-    <row r="358" spans="1:7" customFormat="1" ht="30">
+    <row r="358" spans="1:7" ht="30">
       <c r="A358" s="23" t="s">
         <v>1481</v>
       </c>
@@ -14031,7 +14031,7 @@
       <c r="F358" s="25"/>
       <c r="G358" s="25"/>
     </row>
-    <row r="359" spans="1:7" customFormat="1" ht="30">
+    <row r="359" spans="1:7" ht="30">
       <c r="A359" s="23" t="s">
         <v>1321</v>
       </c>
@@ -14050,11 +14050,10 @@
       <c r="F359" s="25"/>
       <c r="G359" s="25"/>
     </row>
-    <row r="360" spans="1:7" customFormat="1">
+    <row r="360" spans="1:7">
       <c r="A360" s="23" t="s">
         <v>291</v>
       </c>
-      <c r="B360" s="12"/>
       <c r="C360" s="24" t="s">
         <v>218</v>
       </c>
@@ -14063,7 +14062,7 @@
       <c r="F360" s="25"/>
       <c r="G360" s="25"/>
     </row>
-    <row r="361" spans="1:7" customFormat="1" ht="30">
+    <row r="361" spans="1:7" ht="30">
       <c r="A361" s="23" t="s">
         <v>1256</v>
       </c>
@@ -14082,7 +14081,7 @@
       <c r="F361" s="25"/>
       <c r="G361" s="25"/>
     </row>
-    <row r="362" spans="1:7" customFormat="1" ht="30">
+    <row r="362" spans="1:7" ht="30">
       <c r="A362" s="23" t="s">
         <v>382</v>
       </c>
@@ -14103,7 +14102,7 @@
         <v>907</v>
       </c>
     </row>
-    <row r="363" spans="1:7" customFormat="1" ht="45">
+    <row r="363" spans="1:7" ht="45">
       <c r="A363" s="23" t="s">
         <v>486</v>
       </c>
@@ -14124,7 +14123,7 @@
       </c>
       <c r="G363" s="25"/>
     </row>
-    <row r="364" spans="1:7" customFormat="1" ht="30">
+    <row r="364" spans="1:7" ht="30">
       <c r="A364" s="23" t="s">
         <v>1265</v>
       </c>
@@ -14143,7 +14142,7 @@
       <c r="F364" s="25"/>
       <c r="G364" s="25"/>
     </row>
-    <row r="365" spans="1:7" customFormat="1" ht="33.75">
+    <row r="365" spans="1:7" ht="33.75">
       <c r="A365" s="23" t="s">
         <v>1622</v>
       </c>
@@ -14162,7 +14161,7 @@
       <c r="F365" s="25"/>
       <c r="G365" s="25"/>
     </row>
-    <row r="366" spans="1:7" customFormat="1" ht="45">
+    <row r="366" spans="1:7" ht="45">
       <c r="A366" s="23" t="s">
         <v>391</v>
       </c>
@@ -14183,7 +14182,7 @@
       </c>
       <c r="G366" s="25"/>
     </row>
-    <row r="367" spans="1:7" customFormat="1" ht="45">
+    <row r="367" spans="1:7" ht="45">
       <c r="A367" s="23" t="s">
         <v>1159</v>
       </c>
@@ -14200,7 +14199,7 @@
       <c r="F367" s="25"/>
       <c r="G367" s="25"/>
     </row>
-    <row r="368" spans="1:7" customFormat="1" ht="45">
+    <row r="368" spans="1:7" ht="45">
       <c r="A368" s="23" t="s">
         <v>484</v>
       </c>
@@ -14221,7 +14220,7 @@
       </c>
       <c r="G368" s="25"/>
     </row>
-    <row r="369" spans="1:7" customFormat="1" ht="45">
+    <row r="369" spans="1:7" ht="45">
       <c r="A369" s="23" t="s">
         <v>485</v>
       </c>
@@ -14242,7 +14241,7 @@
       </c>
       <c r="G369" s="25"/>
     </row>
-    <row r="370" spans="1:7" customFormat="1">
+    <row r="370" spans="1:7">
       <c r="A370" s="23" t="s">
         <v>1594</v>
       </c>
@@ -14261,7 +14260,7 @@
       <c r="F370" s="25"/>
       <c r="G370" s="25"/>
     </row>
-    <row r="371" spans="1:7" customFormat="1">
+    <row r="371" spans="1:7">
       <c r="A371" s="23" t="s">
         <v>292</v>
       </c>
@@ -14282,7 +14281,7 @@
       </c>
       <c r="G371" s="25"/>
     </row>
-    <row r="372" spans="1:7" customFormat="1" ht="45">
+    <row r="372" spans="1:7" ht="45">
       <c r="A372" s="23" t="s">
         <v>1535</v>
       </c>
@@ -14299,7 +14298,7 @@
       <c r="F372" s="25"/>
       <c r="G372" s="25"/>
     </row>
-    <row r="373" spans="1:7" customFormat="1" ht="30">
+    <row r="373" spans="1:7" ht="30">
       <c r="A373" s="23" t="s">
         <v>1251</v>
       </c>
@@ -14318,7 +14317,7 @@
       <c r="F373" s="25"/>
       <c r="G373" s="25"/>
     </row>
-    <row r="374" spans="1:7" customFormat="1">
+    <row r="374" spans="1:7">
       <c r="A374" s="23" t="s">
         <v>1579</v>
       </c>
@@ -14337,7 +14336,7 @@
       <c r="F374" s="25"/>
       <c r="G374" s="25"/>
     </row>
-    <row r="375" spans="1:7" customFormat="1">
+    <row r="375" spans="1:7">
       <c r="A375" s="23" t="s">
         <v>476</v>
       </c>
@@ -14356,7 +14355,7 @@
       </c>
       <c r="G375" s="25"/>
     </row>
-    <row r="376" spans="1:7" customFormat="1">
+    <row r="376" spans="1:7">
       <c r="A376" s="23" t="s">
         <v>1356</v>
       </c>
@@ -14377,7 +14376,7 @@
       </c>
       <c r="G376" s="25"/>
     </row>
-    <row r="377" spans="1:7" customFormat="1" ht="45">
+    <row r="377" spans="1:7" ht="45">
       <c r="A377" s="23" t="s">
         <v>1546</v>
       </c>
@@ -14394,7 +14393,7 @@
       <c r="F377" s="25"/>
       <c r="G377" s="25"/>
     </row>
-    <row r="378" spans="1:7" customFormat="1" ht="33.75">
+    <row r="378" spans="1:7" ht="33.75">
       <c r="A378" s="23" t="s">
         <v>1143</v>
       </c>
@@ -14413,7 +14412,7 @@
       <c r="F378" s="25"/>
       <c r="G378" s="25"/>
     </row>
-    <row r="379" spans="1:7" customFormat="1">
+    <row r="379" spans="1:7">
       <c r="A379" s="23" t="s">
         <v>1283</v>
       </c>
@@ -14432,7 +14431,7 @@
       <c r="F379" s="25"/>
       <c r="G379" s="25"/>
     </row>
-    <row r="380" spans="1:7" customFormat="1">
+    <row r="380" spans="1:7">
       <c r="A380" s="23" t="s">
         <v>1618</v>
       </c>
@@ -14451,7 +14450,7 @@
       <c r="F380" s="25"/>
       <c r="G380" s="25"/>
     </row>
-    <row r="381" spans="1:7" customFormat="1" ht="101.25">
+    <row r="381" spans="1:7" ht="101.25">
       <c r="A381" s="23" t="s">
         <v>414</v>
       </c>
@@ -14472,7 +14471,7 @@
       </c>
       <c r="G381" s="25"/>
     </row>
-    <row r="382" spans="1:7" customFormat="1" ht="45">
+    <row r="382" spans="1:7" ht="45">
       <c r="A382" s="23" t="s">
         <v>796</v>
       </c>
@@ -14493,11 +14492,10 @@
       </c>
       <c r="G382" s="25"/>
     </row>
-    <row r="383" spans="1:7" customFormat="1">
+    <row r="383" spans="1:7">
       <c r="A383" s="23" t="s">
         <v>1054</v>
       </c>
-      <c r="B383" s="12"/>
       <c r="C383" s="24"/>
       <c r="D383" s="42"/>
       <c r="E383" s="15" t="s">
@@ -14506,7 +14504,7 @@
       <c r="F383" s="25"/>
       <c r="G383" s="25"/>
     </row>
-    <row r="384" spans="1:7" customFormat="1" ht="78.75">
+    <row r="384" spans="1:7" ht="78.75">
       <c r="A384" s="23" t="s">
         <v>1053</v>
       </c>
@@ -14525,7 +14523,7 @@
       <c r="F384" s="25"/>
       <c r="G384" s="25"/>
     </row>
-    <row r="385" spans="1:7" customFormat="1">
+    <row r="385" spans="1:7">
       <c r="A385" s="23" t="s">
         <v>31</v>
       </c>
@@ -14546,7 +14544,7 @@
       </c>
       <c r="G385" s="25"/>
     </row>
-    <row r="386" spans="1:7" customFormat="1" ht="45">
+    <row r="386" spans="1:7" ht="45">
       <c r="A386" s="23" t="s">
         <v>373</v>
       </c>
@@ -14567,7 +14565,7 @@
       </c>
       <c r="G386" s="25"/>
     </row>
-    <row r="387" spans="1:7" customFormat="1" ht="30">
+    <row r="387" spans="1:7" ht="30">
       <c r="A387" s="23" t="s">
         <v>212</v>
       </c>
@@ -14588,7 +14586,7 @@
       </c>
       <c r="G387" s="25"/>
     </row>
-    <row r="388" spans="1:7" customFormat="1" ht="30">
+    <row r="388" spans="1:7" ht="30">
       <c r="A388" s="23" t="s">
         <v>50</v>
       </c>
@@ -14609,7 +14607,7 @@
       </c>
       <c r="G388" s="25"/>
     </row>
-    <row r="389" spans="1:7" customFormat="1" ht="45">
+    <row r="389" spans="1:7" ht="45">
       <c r="A389" s="23" t="s">
         <v>443</v>
       </c>
@@ -14630,7 +14628,7 @@
       </c>
       <c r="G389" s="25"/>
     </row>
-    <row r="390" spans="1:7" customFormat="1" ht="30">
+    <row r="390" spans="1:7" ht="30">
       <c r="A390" s="23" t="s">
         <v>1612</v>
       </c>
@@ -14649,7 +14647,7 @@
       <c r="F390" s="25"/>
       <c r="G390" s="25"/>
     </row>
-    <row r="391" spans="1:7" customFormat="1" ht="30">
+    <row r="391" spans="1:7" ht="30">
       <c r="A391" s="23" t="s">
         <v>189</v>
       </c>
@@ -14670,7 +14668,7 @@
       </c>
       <c r="G391" s="25"/>
     </row>
-    <row r="392" spans="1:7" customFormat="1" ht="30">
+    <row r="392" spans="1:7" ht="30">
       <c r="A392" s="23" t="s">
         <v>1634</v>
       </c>
@@ -14689,7 +14687,7 @@
       <c r="F392" s="25"/>
       <c r="G392" s="25"/>
     </row>
-    <row r="393" spans="1:7" customFormat="1">
+    <row r="393" spans="1:7">
       <c r="A393" s="23" t="s">
         <v>293</v>
       </c>
@@ -14710,7 +14708,7 @@
       </c>
       <c r="G393" s="25"/>
     </row>
-    <row r="394" spans="1:7" customFormat="1" ht="30">
+    <row r="394" spans="1:7" ht="30">
       <c r="A394" s="23" t="s">
         <v>1271</v>
       </c>
@@ -14729,7 +14727,7 @@
       <c r="F394" s="25"/>
       <c r="G394" s="25"/>
     </row>
-    <row r="395" spans="1:7" customFormat="1" ht="45">
+    <row r="395" spans="1:7" ht="45">
       <c r="A395" s="23" t="s">
         <v>1213</v>
       </c>
@@ -14748,7 +14746,7 @@
       <c r="F395" s="25"/>
       <c r="G395" s="25"/>
     </row>
-    <row r="396" spans="1:7" customFormat="1" ht="30">
+    <row r="396" spans="1:7" ht="30">
       <c r="A396" s="23" t="s">
         <v>1644</v>
       </c>
@@ -14767,7 +14765,7 @@
       <c r="F396" s="25"/>
       <c r="G396" s="25"/>
     </row>
-    <row r="397" spans="1:7" customFormat="1" ht="30">
+    <row r="397" spans="1:7" ht="30">
       <c r="A397" s="23" t="s">
         <v>1589</v>
       </c>
@@ -14786,7 +14784,7 @@
       <c r="F397" s="25"/>
       <c r="G397" s="25"/>
     </row>
-    <row r="398" spans="1:7" customFormat="1">
+    <row r="398" spans="1:7">
       <c r="A398" s="23" t="s">
         <v>1357</v>
       </c>
@@ -14807,7 +14805,7 @@
       </c>
       <c r="G398" s="25"/>
     </row>
-    <row r="399" spans="1:7" customFormat="1" ht="60">
+    <row r="399" spans="1:7" ht="60">
       <c r="A399" s="23" t="s">
         <v>396</v>
       </c>
@@ -14828,7 +14826,7 @@
       </c>
       <c r="G399" s="25"/>
     </row>
-    <row r="400" spans="1:7" customFormat="1" ht="30">
+    <row r="400" spans="1:7" ht="30">
       <c r="A400" s="23" t="s">
         <v>63</v>
       </c>
@@ -14847,7 +14845,7 @@
       </c>
       <c r="G400" s="25"/>
     </row>
-    <row r="401" spans="1:7" customFormat="1" ht="45">
+    <row r="401" spans="1:7" ht="45">
       <c r="A401" s="23" t="s">
         <v>849</v>
       </c>
@@ -14870,7 +14868,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="402" spans="1:7" customFormat="1" ht="45">
+    <row r="402" spans="1:7" ht="45">
       <c r="A402" s="23" t="s">
         <v>489</v>
       </c>
@@ -14891,7 +14889,7 @@
       </c>
       <c r="G402" s="25"/>
     </row>
-    <row r="403" spans="1:7" customFormat="1" ht="30">
+    <row r="403" spans="1:7" ht="30">
       <c r="A403" s="23" t="s">
         <v>876</v>
       </c>
@@ -14914,7 +14912,7 @@
         <v>884</v>
       </c>
     </row>
-    <row r="404" spans="1:7" customFormat="1" ht="45">
+    <row r="404" spans="1:7" ht="45">
       <c r="A404" s="23" t="s">
         <v>491</v>
       </c>
@@ -14935,7 +14933,7 @@
       </c>
       <c r="G404" s="25"/>
     </row>
-    <row r="405" spans="1:7" customFormat="1" ht="30">
+    <row r="405" spans="1:7" ht="30">
       <c r="A405" s="23" t="s">
         <v>1050</v>
       </c>
@@ -14952,7 +14950,7 @@
       <c r="F405" s="25"/>
       <c r="G405" s="25"/>
     </row>
-    <row r="406" spans="1:7" customFormat="1" ht="30">
+    <row r="406" spans="1:7" ht="30">
       <c r="A406" s="23" t="s">
         <v>184</v>
       </c>
@@ -14973,7 +14971,7 @@
       </c>
       <c r="G406" s="25"/>
     </row>
-    <row r="407" spans="1:7" customFormat="1" ht="45">
+    <row r="407" spans="1:7" ht="45">
       <c r="A407" s="23" t="s">
         <v>492</v>
       </c>
@@ -14994,7 +14992,7 @@
       </c>
       <c r="G407" s="25"/>
     </row>
-    <row r="408" spans="1:7" customFormat="1" ht="30">
+    <row r="408" spans="1:7" ht="30">
       <c r="A408" s="23" t="s">
         <v>1319</v>
       </c>
@@ -15013,7 +15011,7 @@
       <c r="F408" s="25"/>
       <c r="G408" s="25"/>
     </row>
-    <row r="409" spans="1:7" customFormat="1" ht="30">
+    <row r="409" spans="1:7" ht="30">
       <c r="A409" s="23" t="s">
         <v>110</v>
       </c>
@@ -15034,7 +15032,7 @@
       </c>
       <c r="G409" s="25"/>
     </row>
-    <row r="410" spans="1:7" customFormat="1">
+    <row r="410" spans="1:7">
       <c r="A410" s="23" t="s">
         <v>340</v>
       </c>
@@ -15055,7 +15053,7 @@
       </c>
       <c r="G410" s="25"/>
     </row>
-    <row r="411" spans="1:7" customFormat="1" ht="45">
+    <row r="411" spans="1:7" ht="45">
       <c r="A411" s="23" t="s">
         <v>65</v>
       </c>
@@ -15076,7 +15074,7 @@
       </c>
       <c r="G411" s="25"/>
     </row>
-    <row r="412" spans="1:7" customFormat="1" ht="45">
+    <row r="412" spans="1:7" ht="45">
       <c r="A412" s="23" t="s">
         <v>858</v>
       </c>
@@ -15099,7 +15097,7 @@
         <v>861</v>
       </c>
     </row>
-    <row r="413" spans="1:7" customFormat="1" ht="30">
+    <row r="413" spans="1:7" ht="30">
       <c r="A413" s="23" t="s">
         <v>55</v>
       </c>
@@ -15120,7 +15118,7 @@
       </c>
       <c r="G413" s="25"/>
     </row>
-    <row r="414" spans="1:7" customFormat="1" ht="30">
+    <row r="414" spans="1:7" ht="30">
       <c r="A414" s="23" t="s">
         <v>809</v>
       </c>
@@ -15141,7 +15139,7 @@
       </c>
       <c r="G414" s="25"/>
     </row>
-    <row r="415" spans="1:7" customFormat="1" ht="45">
+    <row r="415" spans="1:7" ht="45">
       <c r="A415" s="23" t="s">
         <v>1550</v>
       </c>
@@ -15158,7 +15156,7 @@
       <c r="F415" s="25"/>
       <c r="G415" s="25"/>
     </row>
-    <row r="416" spans="1:7" customFormat="1" ht="33.75">
+    <row r="416" spans="1:7" ht="33.75">
       <c r="A416" s="23" t="s">
         <v>556</v>
       </c>
@@ -15179,7 +15177,7 @@
       </c>
       <c r="G416" s="25"/>
     </row>
-    <row r="417" spans="1:7" customFormat="1" ht="45">
+    <row r="417" spans="1:7" ht="45">
       <c r="A417" s="23" t="s">
         <v>1149</v>
       </c>
@@ -15198,7 +15196,7 @@
       <c r="F417" s="25"/>
       <c r="G417" s="25"/>
     </row>
-    <row r="418" spans="1:7" customFormat="1" ht="30">
+    <row r="418" spans="1:7" ht="30">
       <c r="A418" s="23" t="s">
         <v>815</v>
       </c>
@@ -15219,7 +15217,7 @@
       </c>
       <c r="G418" s="25"/>
     </row>
-    <row r="419" spans="1:7" customFormat="1">
+    <row r="419" spans="1:7">
       <c r="A419" s="23" t="s">
         <v>335</v>
       </c>
@@ -15240,7 +15238,7 @@
       </c>
       <c r="G419" s="25"/>
     </row>
-    <row r="420" spans="1:7" customFormat="1" ht="30">
+    <row r="420" spans="1:7" ht="30">
       <c r="A420" s="23" t="s">
         <v>299</v>
       </c>
@@ -15259,7 +15257,7 @@
       </c>
       <c r="G420" s="25"/>
     </row>
-    <row r="421" spans="1:7" customFormat="1" ht="60">
+    <row r="421" spans="1:7" ht="60">
       <c r="A421" s="23" t="s">
         <v>569</v>
       </c>
@@ -15280,7 +15278,7 @@
       </c>
       <c r="G421" s="25"/>
     </row>
-    <row r="422" spans="1:7" customFormat="1" ht="60">
+    <row r="422" spans="1:7" ht="60">
       <c r="A422" s="23" t="s">
         <v>1575</v>
       </c>
@@ -15299,7 +15297,7 @@
       <c r="F422" s="25"/>
       <c r="G422" s="25"/>
     </row>
-    <row r="423" spans="1:7" customFormat="1" ht="75">
+    <row r="423" spans="1:7" ht="75">
       <c r="A423" s="23" t="s">
         <v>465</v>
       </c>
@@ -15320,7 +15318,7 @@
       </c>
       <c r="G423" s="25"/>
     </row>
-    <row r="424" spans="1:7" customFormat="1" ht="30">
+    <row r="424" spans="1:7" ht="30">
       <c r="A424" s="23" t="s">
         <v>1258</v>
       </c>
@@ -15339,7 +15337,7 @@
       <c r="F424" s="25"/>
       <c r="G424" s="25"/>
     </row>
-    <row r="425" spans="1:7" customFormat="1" ht="60">
+    <row r="425" spans="1:7" ht="60">
       <c r="A425" s="23" t="s">
         <v>225</v>
       </c>
@@ -15360,7 +15358,7 @@
       </c>
       <c r="G425" s="25"/>
     </row>
-    <row r="426" spans="1:7" customFormat="1" ht="33.75">
+    <row r="426" spans="1:7" ht="33.75">
       <c r="A426" s="23" t="s">
         <v>1506</v>
       </c>
@@ -15379,7 +15377,7 @@
       <c r="F426" s="25"/>
       <c r="G426" s="25"/>
     </row>
-    <row r="427" spans="1:7" customFormat="1" ht="60">
+    <row r="427" spans="1:7" ht="60">
       <c r="A427" s="29" t="s">
         <v>483</v>
       </c>
@@ -15398,7 +15396,7 @@
       </c>
       <c r="G427" s="25"/>
     </row>
-    <row r="428" spans="1:7" customFormat="1" ht="45">
+    <row r="428" spans="1:7" ht="45">
       <c r="A428" s="23" t="s">
         <v>1359</v>
       </c>
@@ -15419,7 +15417,7 @@
       </c>
       <c r="G428" s="25"/>
     </row>
-    <row r="429" spans="1:7" customFormat="1" ht="33.75">
+    <row r="429" spans="1:7" ht="33.75">
       <c r="A429" s="23" t="s">
         <v>300</v>
       </c>
@@ -15440,7 +15438,7 @@
       </c>
       <c r="G429" s="25"/>
     </row>
-    <row r="430" spans="1:7" customFormat="1">
+    <row r="430" spans="1:7">
       <c r="A430" s="23" t="s">
         <v>313</v>
       </c>
@@ -15461,7 +15459,7 @@
       </c>
       <c r="G430" s="25"/>
     </row>
-    <row r="431" spans="1:7" customFormat="1" ht="30">
+    <row r="431" spans="1:7" ht="30">
       <c r="A431" s="23" t="s">
         <v>202</v>
       </c>
@@ -15482,7 +15480,7 @@
       </c>
       <c r="G431" s="25"/>
     </row>
-    <row r="432" spans="1:7" customFormat="1">
+    <row r="432" spans="1:7">
       <c r="A432" s="23" t="s">
         <v>1077</v>
       </c>
@@ -15497,7 +15495,7 @@
       <c r="F432" s="25"/>
       <c r="G432" s="25"/>
     </row>
-    <row r="433" spans="1:7" customFormat="1" ht="30">
+    <row r="433" spans="1:7" ht="30">
       <c r="A433" s="23" t="s">
         <v>1700</v>
       </c>
@@ -15516,7 +15514,7 @@
       <c r="F433" s="25"/>
       <c r="G433" s="25"/>
     </row>
-    <row r="434" spans="1:7" customFormat="1">
+    <row r="434" spans="1:7">
       <c r="A434" s="23" t="s">
         <v>401</v>
       </c>
@@ -15535,7 +15533,7 @@
       </c>
       <c r="G434" s="25"/>
     </row>
-    <row r="435" spans="1:7" customFormat="1" ht="30">
+    <row r="435" spans="1:7" ht="30">
       <c r="A435" s="23" t="s">
         <v>703</v>
       </c>
@@ -15554,7 +15552,7 @@
       </c>
       <c r="G435" s="25"/>
     </row>
-    <row r="436" spans="1:7" customFormat="1" ht="30">
+    <row r="436" spans="1:7" ht="30">
       <c r="A436" s="23" t="s">
         <v>474</v>
       </c>
@@ -15573,7 +15571,7 @@
       </c>
       <c r="G436" s="25"/>
     </row>
-    <row r="437" spans="1:7" customFormat="1" ht="30">
+    <row r="437" spans="1:7" ht="30">
       <c r="A437" s="23" t="s">
         <v>138</v>
       </c>
@@ -15594,7 +15592,7 @@
       </c>
       <c r="G437" s="25"/>
     </row>
-    <row r="438" spans="1:7" customFormat="1">
+    <row r="438" spans="1:7">
       <c r="A438" s="23" t="s">
         <v>1278</v>
       </c>
@@ -15613,7 +15611,7 @@
       <c r="F438" s="25"/>
       <c r="G438" s="25"/>
     </row>
-    <row r="439" spans="1:7" customFormat="1" ht="30">
+    <row r="439" spans="1:7" ht="30">
       <c r="A439" s="23" t="s">
         <v>855</v>
       </c>
@@ -15636,7 +15634,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="440" spans="1:7" customFormat="1" ht="45">
+    <row r="440" spans="1:7" ht="45">
       <c r="A440" s="23" t="s">
         <v>1202</v>
       </c>
@@ -15655,7 +15653,7 @@
       <c r="F440" s="25"/>
       <c r="G440" s="25"/>
     </row>
-    <row r="441" spans="1:7" customFormat="1" ht="45">
+    <row r="441" spans="1:7" ht="45">
       <c r="A441" s="23" t="s">
         <v>892</v>
       </c>
@@ -15674,7 +15672,7 @@
       <c r="F441" s="25"/>
       <c r="G441" s="25"/>
     </row>
-    <row r="442" spans="1:7" customFormat="1" ht="45">
+    <row r="442" spans="1:7" ht="45">
       <c r="A442" s="23" t="s">
         <v>892</v>
       </c>
@@ -15697,7 +15695,7 @@
         <v>917</v>
       </c>
     </row>
-    <row r="443" spans="1:7" customFormat="1" ht="33.75">
+    <row r="443" spans="1:7" ht="33.75">
       <c r="A443" s="23" t="s">
         <v>23</v>
       </c>
@@ -15718,7 +15716,7 @@
       </c>
       <c r="G443" s="25"/>
     </row>
-    <row r="444" spans="1:7" customFormat="1" ht="30">
+    <row r="444" spans="1:7" ht="30">
       <c r="A444" s="23" t="s">
         <v>1518</v>
       </c>
@@ -15737,7 +15735,7 @@
       <c r="F444" s="25"/>
       <c r="G444" s="25"/>
     </row>
-    <row r="445" spans="1:7" customFormat="1" ht="45">
+    <row r="445" spans="1:7" ht="45">
       <c r="A445" s="23" t="s">
         <v>708</v>
       </c>
@@ -15758,7 +15756,7 @@
       </c>
       <c r="G445" s="25"/>
     </row>
-    <row r="446" spans="1:7" customFormat="1" ht="30">
+    <row r="446" spans="1:7" ht="30">
       <c r="A446" s="23" t="s">
         <v>817</v>
       </c>
@@ -15775,7 +15773,7 @@
       </c>
       <c r="G446" s="25"/>
     </row>
-    <row r="447" spans="1:7" customFormat="1" ht="30">
+    <row r="447" spans="1:7" ht="30">
       <c r="A447" s="23" t="s">
         <v>451</v>
       </c>
@@ -15796,7 +15794,7 @@
       </c>
       <c r="G447" s="25"/>
     </row>
-    <row r="448" spans="1:7" customFormat="1" ht="30">
+    <row r="448" spans="1:7" ht="30">
       <c r="A448" s="23" t="s">
         <v>1035</v>
       </c>
@@ -15813,7 +15811,7 @@
       <c r="F448" s="25"/>
       <c r="G448" s="25"/>
     </row>
-    <row r="449" spans="1:7" customFormat="1" ht="30">
+    <row r="449" spans="1:7" ht="30">
       <c r="A449" s="23" t="s">
         <v>450</v>
       </c>
@@ -15832,7 +15830,7 @@
       </c>
       <c r="G449" s="25"/>
     </row>
-    <row r="450" spans="1:7" customFormat="1" ht="30">
+    <row r="450" spans="1:7" ht="30">
       <c r="A450" s="23" t="s">
         <v>29</v>
       </c>
@@ -15853,7 +15851,7 @@
       </c>
       <c r="G450" s="25"/>
     </row>
-    <row r="451" spans="1:7" customFormat="1" ht="33.75">
+    <row r="451" spans="1:7" ht="33.75">
       <c r="A451" s="23" t="s">
         <v>314</v>
       </c>
@@ -15874,7 +15872,7 @@
       </c>
       <c r="G451" s="25"/>
     </row>
-    <row r="452" spans="1:7" customFormat="1" ht="30">
+    <row r="452" spans="1:7" ht="30">
       <c r="A452" s="23" t="s">
         <v>42</v>
       </c>
@@ -15895,7 +15893,7 @@
       </c>
       <c r="G452" s="25"/>
     </row>
-    <row r="453" spans="1:7" customFormat="1">
+    <row r="453" spans="1:7">
       <c r="A453" s="23" t="s">
         <v>728</v>
       </c>
@@ -15914,7 +15912,7 @@
       </c>
       <c r="G453" s="25"/>
     </row>
-    <row r="454" spans="1:7" customFormat="1" ht="45">
+    <row r="454" spans="1:7" ht="45">
       <c r="A454" s="23" t="s">
         <v>481</v>
       </c>
@@ -15935,7 +15933,7 @@
       </c>
       <c r="G454" s="25"/>
     </row>
-    <row r="455" spans="1:7" customFormat="1" ht="30">
+    <row r="455" spans="1:7" ht="30">
       <c r="A455" s="23" t="s">
         <v>1610</v>
       </c>
@@ -15952,7 +15950,7 @@
       <c r="F455" s="25"/>
       <c r="G455" s="25"/>
     </row>
-    <row r="456" spans="1:7" customFormat="1">
+    <row r="456" spans="1:7">
       <c r="A456" s="23" t="s">
         <v>542</v>
       </c>
@@ -15971,7 +15969,7 @@
       </c>
       <c r="G456" s="25"/>
     </row>
-    <row r="457" spans="1:7" customFormat="1" ht="45">
+    <row r="457" spans="1:7" ht="45">
       <c r="A457" s="23" t="s">
         <v>439</v>
       </c>
@@ -15992,7 +15990,7 @@
       </c>
       <c r="G457" s="25"/>
     </row>
-    <row r="458" spans="1:7" customFormat="1" ht="30">
+    <row r="458" spans="1:7" ht="30">
       <c r="A458" s="23" t="s">
         <v>1556</v>
       </c>
@@ -16009,7 +16007,7 @@
       <c r="F458" s="25"/>
       <c r="G458" s="25"/>
     </row>
-    <row r="459" spans="1:7" customFormat="1" ht="45">
+    <row r="459" spans="1:7" ht="45">
       <c r="A459" s="23" t="s">
         <v>87</v>
       </c>
@@ -16030,7 +16028,7 @@
       </c>
       <c r="G459" s="25"/>
     </row>
-    <row r="460" spans="1:7" customFormat="1" ht="45">
+    <row r="460" spans="1:7" ht="45">
       <c r="A460" s="23" t="s">
         <v>1364</v>
       </c>
@@ -16051,7 +16049,7 @@
       </c>
       <c r="G460" s="25"/>
     </row>
-    <row r="461" spans="1:7" customFormat="1">
+    <row r="461" spans="1:7">
       <c r="A461" s="23" t="s">
         <v>715</v>
       </c>
@@ -16070,7 +16068,7 @@
       </c>
       <c r="G461" s="25"/>
     </row>
-    <row r="462" spans="1:7" customFormat="1" ht="30">
+    <row r="462" spans="1:7" ht="30">
       <c r="A462" s="23" t="s">
         <v>318</v>
       </c>
@@ -16091,7 +16089,7 @@
       </c>
       <c r="G462" s="25"/>
     </row>
-    <row r="463" spans="1:7" customFormat="1">
+    <row r="463" spans="1:7">
       <c r="A463" s="23" t="s">
         <v>236</v>
       </c>
@@ -16112,7 +16110,7 @@
       </c>
       <c r="G463" s="25"/>
     </row>
-    <row r="464" spans="1:7" customFormat="1" ht="45">
+    <row r="464" spans="1:7" ht="45">
       <c r="A464" s="23" t="s">
         <v>1045</v>
       </c>
@@ -16131,7 +16129,7 @@
       <c r="F464" s="25"/>
       <c r="G464" s="25"/>
     </row>
-    <row r="465" spans="1:7" customFormat="1" ht="30">
+    <row r="465" spans="1:7" ht="30">
       <c r="A465" s="23" t="s">
         <v>752</v>
       </c>
@@ -16150,7 +16148,7 @@
       </c>
       <c r="G465" s="25"/>
     </row>
-    <row r="466" spans="1:7" customFormat="1" ht="30">
+    <row r="466" spans="1:7" ht="30">
       <c r="A466" s="23" t="s">
         <v>753</v>
       </c>
@@ -16169,7 +16167,7 @@
       </c>
       <c r="G466" s="25"/>
     </row>
-    <row r="467" spans="1:7" customFormat="1" ht="30">
+    <row r="467" spans="1:7" ht="30">
       <c r="A467" s="23" t="s">
         <v>754</v>
       </c>
@@ -16188,7 +16186,7 @@
       </c>
       <c r="G467" s="25"/>
     </row>
-    <row r="468" spans="1:7" customFormat="1" ht="30">
+    <row r="468" spans="1:7" ht="30">
       <c r="A468" s="23" t="s">
         <v>756</v>
       </c>
@@ -16207,7 +16205,7 @@
       </c>
       <c r="G468" s="25"/>
     </row>
-    <row r="469" spans="1:7" customFormat="1" ht="30">
+    <row r="469" spans="1:7" ht="30">
       <c r="A469" s="23" t="s">
         <v>757</v>
       </c>
@@ -16226,7 +16224,7 @@
       </c>
       <c r="G469" s="25"/>
     </row>
-    <row r="470" spans="1:7" customFormat="1" ht="45">
+    <row r="470" spans="1:7" ht="45">
       <c r="A470" s="23" t="s">
         <v>811</v>
       </c>
@@ -16243,7 +16241,7 @@
       </c>
       <c r="G470" s="25"/>
     </row>
-    <row r="471" spans="1:7" customFormat="1" ht="33.75">
+    <row r="471" spans="1:7" ht="33.75">
       <c r="A471" s="23" t="s">
         <v>1301</v>
       </c>
@@ -16262,7 +16260,7 @@
       <c r="F471" s="25"/>
       <c r="G471" s="25"/>
     </row>
-    <row r="472" spans="1:7" customFormat="1">
+    <row r="472" spans="1:7">
       <c r="A472" s="23" t="s">
         <v>303</v>
       </c>
@@ -16283,7 +16281,7 @@
       </c>
       <c r="G472" s="25"/>
     </row>
-    <row r="473" spans="1:7" customFormat="1">
+    <row r="473" spans="1:7">
       <c r="A473" s="23" t="s">
         <v>1529</v>
       </c>
@@ -16302,7 +16300,7 @@
       <c r="F473" s="25"/>
       <c r="G473" s="25"/>
     </row>
-    <row r="474" spans="1:7" customFormat="1" ht="45">
+    <row r="474" spans="1:7" ht="45">
       <c r="A474" s="23" t="s">
         <v>755</v>
       </c>
@@ -16321,7 +16319,7 @@
       </c>
       <c r="G474" s="25"/>
     </row>
-    <row r="475" spans="1:7" customFormat="1">
+    <row r="475" spans="1:7">
       <c r="A475" s="23" t="s">
         <v>178</v>
       </c>
@@ -16342,7 +16340,7 @@
       </c>
       <c r="G475" s="25"/>
     </row>
-    <row r="476" spans="1:7" customFormat="1">
+    <row r="476" spans="1:7">
       <c r="A476" s="23" t="s">
         <v>1585</v>
       </c>
@@ -16361,7 +16359,7 @@
       <c r="F476" s="25"/>
       <c r="G476" s="25"/>
     </row>
-    <row r="477" spans="1:7" customFormat="1" ht="33.75">
+    <row r="477" spans="1:7" ht="33.75">
       <c r="A477" s="23" t="s">
         <v>270</v>
       </c>
@@ -16382,7 +16380,7 @@
       </c>
       <c r="G477" s="25"/>
     </row>
-    <row r="478" spans="1:7" customFormat="1" ht="30">
+    <row r="478" spans="1:7" ht="30">
       <c r="A478" s="23" t="s">
         <v>46</v>
       </c>
@@ -16403,7 +16401,7 @@
       </c>
       <c r="G478" s="25"/>
     </row>
-    <row r="479" spans="1:7" customFormat="1">
+    <row r="479" spans="1:7">
       <c r="A479" s="23" t="s">
         <v>434</v>
       </c>
@@ -16424,7 +16422,7 @@
       </c>
       <c r="G479" s="25"/>
     </row>
-    <row r="480" spans="1:7" customFormat="1">
+    <row r="480" spans="1:7">
       <c r="A480" s="23" t="s">
         <v>211</v>
       </c>
@@ -16441,7 +16439,7 @@
       <c r="F480" s="25"/>
       <c r="G480" s="25"/>
     </row>
-    <row r="481" spans="1:7" customFormat="1" ht="45">
+    <row r="481" spans="1:7" ht="45">
       <c r="A481" s="23" t="s">
         <v>35</v>
       </c>
@@ -16462,7 +16460,7 @@
       </c>
       <c r="G481" s="25"/>
     </row>
-    <row r="482" spans="1:7" customFormat="1" ht="30">
+    <row r="482" spans="1:7" ht="30">
       <c r="A482" s="23" t="s">
         <v>1316</v>
       </c>
@@ -16481,7 +16479,7 @@
       <c r="F482" s="25"/>
       <c r="G482" s="25"/>
     </row>
-    <row r="483" spans="1:7" customFormat="1" ht="30">
+    <row r="483" spans="1:7" ht="30">
       <c r="A483" s="23" t="s">
         <v>1628</v>
       </c>
@@ -16500,7 +16498,7 @@
       <c r="F483" s="25"/>
       <c r="G483" s="25"/>
     </row>
-    <row r="484" spans="1:7" customFormat="1" ht="30">
+    <row r="484" spans="1:7" ht="30">
       <c r="A484" s="23" t="s">
         <v>36</v>
       </c>
@@ -16521,7 +16519,7 @@
       </c>
       <c r="G484" s="25"/>
     </row>
-    <row r="485" spans="1:7" customFormat="1" ht="30">
+    <row r="485" spans="1:7" ht="30">
       <c r="A485" s="23" t="s">
         <v>246</v>
       </c>
@@ -16540,7 +16538,7 @@
       <c r="F485" s="25"/>
       <c r="G485" s="25"/>
     </row>
-    <row r="486" spans="1:7" customFormat="1" ht="30">
+    <row r="486" spans="1:7" ht="30">
       <c r="A486" s="23" t="s">
         <v>324</v>
       </c>
@@ -16561,7 +16559,7 @@
       </c>
       <c r="G486" s="25"/>
     </row>
-    <row r="487" spans="1:7" customFormat="1">
+    <row r="487" spans="1:7">
       <c r="A487" s="23" t="s">
         <v>1165</v>
       </c>
@@ -16578,7 +16576,7 @@
       <c r="F487" s="25"/>
       <c r="G487" s="25"/>
     </row>
-    <row r="488" spans="1:7" customFormat="1" ht="33.75">
+    <row r="488" spans="1:7" ht="33.75">
       <c r="A488" s="23" t="s">
         <v>1525</v>
       </c>
@@ -16597,7 +16595,7 @@
       <c r="F488" s="25"/>
       <c r="G488" s="25"/>
     </row>
-    <row r="489" spans="1:7" customFormat="1">
+    <row r="489" spans="1:7">
       <c r="A489" s="23" t="s">
         <v>1170</v>
       </c>
@@ -16614,7 +16612,7 @@
       <c r="F489" s="25"/>
       <c r="G489" s="25"/>
     </row>
-    <row r="490" spans="1:7" customFormat="1" ht="30">
+    <row r="490" spans="1:7" ht="30">
       <c r="A490" s="23" t="s">
         <v>857</v>
       </c>
@@ -16637,7 +16635,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="491" spans="1:7" customFormat="1">
+    <row r="491" spans="1:7">
       <c r="A491" s="23" t="s">
         <v>1630</v>
       </c>
@@ -16656,7 +16654,7 @@
       <c r="F491" s="25"/>
       <c r="G491" s="25"/>
     </row>
-    <row r="492" spans="1:7" customFormat="1" ht="45">
+    <row r="492" spans="1:7" ht="45">
       <c r="A492" s="23" t="s">
         <v>1581</v>
       </c>
@@ -16675,7 +16673,7 @@
       <c r="F492" s="25"/>
       <c r="G492" s="25"/>
     </row>
-    <row r="493" spans="1:7" customFormat="1" ht="30">
+    <row r="493" spans="1:7" ht="30">
       <c r="A493" s="23" t="s">
         <v>478</v>
       </c>
@@ -16694,7 +16692,7 @@
       </c>
       <c r="G493" s="25"/>
     </row>
-    <row r="494" spans="1:7" customFormat="1" ht="30">
+    <row r="494" spans="1:7" ht="30">
       <c r="A494" s="23" t="s">
         <v>1148</v>
       </c>
@@ -16711,7 +16709,7 @@
       <c r="F494" s="25"/>
       <c r="G494" s="25"/>
     </row>
-    <row r="495" spans="1:7" customFormat="1" ht="30">
+    <row r="495" spans="1:7" ht="30">
       <c r="A495" s="23" t="s">
         <v>159</v>
       </c>
@@ -16730,7 +16728,7 @@
       </c>
       <c r="G495" s="25"/>
     </row>
-    <row r="496" spans="1:7" customFormat="1">
+    <row r="496" spans="1:7">
       <c r="A496" s="23" t="s">
         <v>466</v>
       </c>
@@ -16749,7 +16747,7 @@
       </c>
       <c r="G496" s="25"/>
     </row>
-    <row r="497" spans="1:7" customFormat="1">
+    <row r="497" spans="1:7">
       <c r="A497" s="23" t="s">
         <v>564</v>
       </c>
@@ -16768,7 +16766,7 @@
       </c>
       <c r="G497" s="25"/>
     </row>
-    <row r="498" spans="1:7" customFormat="1">
+    <row r="498" spans="1:7">
       <c r="A498" s="23" t="s">
         <v>562</v>
       </c>
@@ -16787,7 +16785,7 @@
       </c>
       <c r="G498" s="25"/>
     </row>
-    <row r="499" spans="1:7" customFormat="1">
+    <row r="499" spans="1:7">
       <c r="A499" s="23" t="s">
         <v>749</v>
       </c>
@@ -16806,7 +16804,7 @@
       </c>
       <c r="G499" s="25"/>
     </row>
-    <row r="500" spans="1:7" customFormat="1">
+    <row r="500" spans="1:7">
       <c r="A500" s="23" t="s">
         <v>563</v>
       </c>
@@ -16825,7 +16823,7 @@
       </c>
       <c r="G500" s="25"/>
     </row>
-    <row r="501" spans="1:7" customFormat="1" ht="30">
+    <row r="501" spans="1:7" ht="30">
       <c r="A501" s="23" t="s">
         <v>1144</v>
       </c>
@@ -16844,7 +16842,7 @@
       <c r="F501" s="25"/>
       <c r="G501" s="25"/>
     </row>
-    <row r="502" spans="1:7" customFormat="1" ht="45">
+    <row r="502" spans="1:7" ht="45">
       <c r="A502" s="23" t="s">
         <v>1552</v>
       </c>
@@ -16861,7 +16859,7 @@
       <c r="F502" s="25"/>
       <c r="G502" s="25"/>
     </row>
-    <row r="503" spans="1:7" customFormat="1" ht="30">
+    <row r="503" spans="1:7" ht="30">
       <c r="A503" s="23" t="s">
         <v>544</v>
       </c>
@@ -16880,7 +16878,7 @@
       </c>
       <c r="G503" s="25"/>
     </row>
-    <row r="504" spans="1:7" customFormat="1" ht="45">
+    <row r="504" spans="1:7" ht="45">
       <c r="A504" s="23" t="s">
         <v>762</v>
       </c>
@@ -16899,7 +16897,7 @@
       </c>
       <c r="G504" s="25"/>
     </row>
-    <row r="505" spans="1:7" customFormat="1" ht="33.75">
+    <row r="505" spans="1:7" ht="33.75">
       <c r="A505" s="23" t="s">
         <v>119</v>
       </c>
@@ -16920,7 +16918,7 @@
       </c>
       <c r="G505" s="25"/>
     </row>
-    <row r="506" spans="1:7" customFormat="1">
+    <row r="506" spans="1:7">
       <c r="A506" s="23" t="s">
         <v>399</v>
       </c>
@@ -16941,7 +16939,7 @@
       </c>
       <c r="G506" s="25"/>
     </row>
-    <row r="507" spans="1:7" customFormat="1" ht="30">
+    <row r="507" spans="1:7" ht="30">
       <c r="A507" s="23" t="s">
         <v>297</v>
       </c>
@@ -16962,7 +16960,7 @@
       </c>
       <c r="G507" s="25"/>
     </row>
-    <row r="508" spans="1:7" customFormat="1">
+    <row r="508" spans="1:7">
       <c r="A508" s="23" t="s">
         <v>1222</v>
       </c>
@@ -16981,7 +16979,7 @@
       <c r="F508" s="25"/>
       <c r="G508" s="25"/>
     </row>
-    <row r="509" spans="1:7" customFormat="1" ht="30">
+    <row r="509" spans="1:7" ht="30">
       <c r="A509" s="23" t="s">
         <v>47</v>
       </c>
@@ -17002,7 +17000,7 @@
       </c>
       <c r="G509" s="25"/>
     </row>
-    <row r="510" spans="1:7" customFormat="1" ht="30">
+    <row r="510" spans="1:7" ht="30">
       <c r="A510" s="23" t="s">
         <v>168</v>
       </c>
@@ -17023,7 +17021,7 @@
       </c>
       <c r="G510" s="25"/>
     </row>
-    <row r="511" spans="1:7" customFormat="1" ht="30">
+    <row r="511" spans="1:7" ht="30">
       <c r="A511" s="23" t="s">
         <v>1026</v>
       </c>
@@ -17042,7 +17040,7 @@
       <c r="F511" s="25"/>
       <c r="G511" s="25"/>
     </row>
-    <row r="512" spans="1:7" customFormat="1" ht="45">
+    <row r="512" spans="1:7" ht="45">
       <c r="A512" s="23" t="s">
         <v>128</v>
       </c>
@@ -17063,7 +17061,7 @@
       </c>
       <c r="G512" s="25"/>
     </row>
-    <row r="513" spans="1:7" customFormat="1" ht="30">
+    <row r="513" spans="1:7" ht="30">
       <c r="A513" s="23" t="s">
         <v>1029</v>
       </c>
@@ -17082,7 +17080,7 @@
       <c r="F513" s="25"/>
       <c r="G513" s="25"/>
     </row>
-    <row r="514" spans="1:7" customFormat="1">
+    <row r="514" spans="1:7">
       <c r="A514" s="23" t="s">
         <v>256</v>
       </c>
@@ -17101,7 +17099,7 @@
       </c>
       <c r="G514" s="25"/>
     </row>
-    <row r="515" spans="1:7" customFormat="1" ht="30">
+    <row r="515" spans="1:7" ht="30">
       <c r="A515" s="23" t="s">
         <v>1414</v>
       </c>
@@ -17120,7 +17118,7 @@
       <c r="F515" s="25"/>
       <c r="G515" s="25"/>
     </row>
-    <row r="516" spans="1:7" customFormat="1" ht="30">
+    <row r="516" spans="1:7" ht="30">
       <c r="A516" s="23" t="s">
         <v>1367</v>
       </c>
@@ -17141,7 +17139,7 @@
       </c>
       <c r="G516" s="25"/>
     </row>
-    <row r="517" spans="1:7" customFormat="1">
+    <row r="517" spans="1:7">
       <c r="A517" s="23" t="s">
         <v>1592</v>
       </c>
@@ -17160,7 +17158,7 @@
       <c r="F517" s="25"/>
       <c r="G517" s="25"/>
     </row>
-    <row r="518" spans="1:7" customFormat="1">
+    <row r="518" spans="1:7">
       <c r="A518" s="23" t="s">
         <v>101</v>
       </c>
@@ -17179,7 +17177,7 @@
       </c>
       <c r="G518" s="25"/>
     </row>
-    <row r="519" spans="1:7" customFormat="1" ht="30">
+    <row r="519" spans="1:7" ht="30">
       <c r="A519" s="23" t="s">
         <v>154</v>
       </c>
@@ -17200,7 +17198,7 @@
       </c>
       <c r="G519" s="25"/>
     </row>
-    <row r="520" spans="1:7" customFormat="1" ht="33.75">
+    <row r="520" spans="1:7" ht="33.75">
       <c r="A520" s="23" t="s">
         <v>770</v>
       </c>
@@ -17240,7 +17238,7 @@
       </c>
       <c r="G521" s="25"/>
     </row>
-    <row r="522" spans="1:7" customFormat="1" ht="30">
+    <row r="522" spans="1:7" ht="30">
       <c r="A522" s="23" t="s">
         <v>204</v>
       </c>
@@ -17261,7 +17259,7 @@
       </c>
       <c r="G522" s="25"/>
     </row>
-    <row r="523" spans="1:7" customFormat="1" ht="30">
+    <row r="523" spans="1:7" ht="30">
       <c r="A523" s="23" t="s">
         <v>1263</v>
       </c>
@@ -17280,7 +17278,7 @@
       <c r="F523" s="25"/>
       <c r="G523" s="25"/>
     </row>
-    <row r="524" spans="1:7" customFormat="1" ht="30">
+    <row r="524" spans="1:7" ht="30">
       <c r="A524" s="23" t="s">
         <v>1041</v>
       </c>
@@ -17299,7 +17297,7 @@
       <c r="F524" s="25"/>
       <c r="G524" s="25"/>
     </row>
-    <row r="525" spans="1:7" customFormat="1" ht="30">
+    <row r="525" spans="1:7" ht="30">
       <c r="A525" s="23" t="s">
         <v>1248</v>
       </c>
@@ -17318,7 +17316,7 @@
       <c r="F525" s="25"/>
       <c r="G525" s="25"/>
     </row>
-    <row r="526" spans="1:7" customFormat="1" ht="30">
+    <row r="526" spans="1:7" ht="30">
       <c r="A526" s="23" t="s">
         <v>81</v>
       </c>
@@ -17339,7 +17337,7 @@
       </c>
       <c r="G526" s="25"/>
     </row>
-    <row r="527" spans="1:7" customFormat="1" ht="30">
+    <row r="527" spans="1:7" ht="30">
       <c r="A527" s="23" t="s">
         <v>845</v>
       </c>
@@ -17362,7 +17360,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="528" spans="1:7" customFormat="1" ht="45">
+    <row r="528" spans="1:7" ht="45">
       <c r="A528" s="23" t="s">
         <v>1315</v>
       </c>
@@ -17381,7 +17379,7 @@
       <c r="F528" s="25"/>
       <c r="G528" s="25"/>
     </row>
-    <row r="529" spans="1:7" customFormat="1" ht="60">
+    <row r="529" spans="1:7" ht="60">
       <c r="A529" s="23" t="s">
         <v>1311</v>
       </c>
@@ -17400,7 +17398,7 @@
       <c r="F529" s="25"/>
       <c r="G529" s="25"/>
     </row>
-    <row r="530" spans="1:7" customFormat="1" ht="30">
+    <row r="530" spans="1:7" ht="30">
       <c r="A530" s="23" t="s">
         <v>864</v>
       </c>
@@ -17423,7 +17421,7 @@
         <v>869</v>
       </c>
     </row>
-    <row r="531" spans="1:7" customFormat="1" ht="30">
+    <row r="531" spans="1:7" ht="30">
       <c r="A531" s="23" t="s">
         <v>363</v>
       </c>
@@ -17444,7 +17442,7 @@
       </c>
       <c r="G531" s="25"/>
     </row>
-    <row r="532" spans="1:7" customFormat="1">
+    <row r="532" spans="1:7">
       <c r="A532" s="23" t="s">
         <v>586</v>
       </c>
@@ -17465,7 +17463,7 @@
       </c>
       <c r="G532" s="25"/>
     </row>
-    <row r="533" spans="1:7" customFormat="1">
+    <row r="533" spans="1:7">
       <c r="A533" s="23" t="s">
         <v>789</v>
       </c>
@@ -17486,7 +17484,7 @@
       </c>
       <c r="G533" s="25"/>
     </row>
-    <row r="534" spans="1:7" customFormat="1" ht="30">
+    <row r="534" spans="1:7" ht="30">
       <c r="A534" s="23" t="s">
         <v>1313</v>
       </c>
@@ -17505,7 +17503,7 @@
       <c r="F534" s="25"/>
       <c r="G534" s="25"/>
     </row>
-    <row r="535" spans="1:7" customFormat="1" ht="30">
+    <row r="535" spans="1:7" ht="30">
       <c r="A535" s="23" t="s">
         <v>174</v>
       </c>
@@ -17526,7 +17524,7 @@
       </c>
       <c r="G535" s="25"/>
     </row>
-    <row r="536" spans="1:7" customFormat="1" ht="45">
+    <row r="536" spans="1:7" ht="45">
       <c r="A536" s="23" t="s">
         <v>493</v>
       </c>
@@ -17547,7 +17545,7 @@
       </c>
       <c r="G536" s="25"/>
     </row>
-    <row r="537" spans="1:7" customFormat="1" ht="33.75">
+    <row r="537" spans="1:7" ht="33.75">
       <c r="A537" s="23" t="s">
         <v>191</v>
       </c>
@@ -17568,7 +17566,7 @@
       </c>
       <c r="G537" s="25"/>
     </row>
-    <row r="538" spans="1:7" customFormat="1" ht="33.75">
+    <row r="538" spans="1:7" ht="33.75">
       <c r="A538" s="23" t="s">
         <v>854</v>
       </c>
@@ -17591,7 +17589,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="539" spans="1:7" customFormat="1" ht="30">
+    <row r="539" spans="1:7" ht="30">
       <c r="A539" s="23" t="s">
         <v>1181</v>
       </c>
@@ -17610,7 +17608,7 @@
       <c r="F539" s="25"/>
       <c r="G539" s="25"/>
     </row>
-    <row r="540" spans="1:7" customFormat="1" ht="67.5">
+    <row r="540" spans="1:7" ht="67.5">
       <c r="A540" s="23" t="s">
         <v>361</v>
       </c>
@@ -17631,7 +17629,7 @@
       </c>
       <c r="G540" s="25"/>
     </row>
-    <row r="541" spans="1:7" customFormat="1">
+    <row r="541" spans="1:7">
       <c r="A541" s="23" t="s">
         <v>1193</v>
       </c>
@@ -17650,7 +17648,7 @@
       <c r="F541" s="25"/>
       <c r="G541" s="25"/>
     </row>
-    <row r="542" spans="1:7" customFormat="1">
+    <row r="542" spans="1:7">
       <c r="A542" s="23" t="s">
         <v>7</v>
       </c>
@@ -17671,7 +17669,7 @@
       </c>
       <c r="G542" s="25"/>
     </row>
-    <row r="543" spans="1:7" customFormat="1" ht="30">
+    <row r="543" spans="1:7" ht="30">
       <c r="A543" s="23" t="s">
         <v>305</v>
       </c>
@@ -17692,7 +17690,7 @@
       </c>
       <c r="G543" s="25"/>
     </row>
-    <row r="544" spans="1:7" customFormat="1">
+    <row r="544" spans="1:7">
       <c r="A544" s="23" t="s">
         <v>310</v>
       </c>
@@ -17713,7 +17711,7 @@
       </c>
       <c r="G544" s="25"/>
     </row>
-    <row r="545" spans="1:16384" customFormat="1">
+    <row r="545" spans="1:16384">
       <c r="A545" s="23" t="s">
         <v>321</v>
       </c>
@@ -17734,7 +17732,7 @@
       </c>
       <c r="G545" s="25"/>
     </row>
-    <row r="546" spans="1:16384" customFormat="1" ht="45">
+    <row r="546" spans="1:16384" ht="45">
       <c r="A546" s="23" t="s">
         <v>136</v>
       </c>
@@ -17755,7 +17753,7 @@
       </c>
       <c r="G546" s="25"/>
     </row>
-    <row r="547" spans="1:16384" customFormat="1" ht="69.75">
+    <row r="547" spans="1:16384" ht="69.75">
       <c r="A547" s="30" t="s">
         <v>1786</v>
       </c>
@@ -17776,7 +17774,7 @@
       </c>
       <c r="G547" s="25"/>
     </row>
-    <row r="548" spans="1:16384" customFormat="1">
+    <row r="548" spans="1:16384">
       <c r="A548" s="23" t="s">
         <v>309</v>
       </c>
@@ -17797,7 +17795,7 @@
       </c>
       <c r="G548" s="25"/>
     </row>
-    <row r="549" spans="1:16384" customFormat="1" ht="60">
+    <row r="549" spans="1:16384" ht="60">
       <c r="A549" s="23" t="s">
         <v>1233</v>
       </c>
@@ -17816,7 +17814,7 @@
       <c r="F549" s="25"/>
       <c r="G549" s="25"/>
     </row>
-    <row r="550" spans="1:16384" customFormat="1" ht="30">
+    <row r="550" spans="1:16384" ht="30">
       <c r="A550" s="23" t="s">
         <v>244</v>
       </c>
@@ -17837,7 +17835,7 @@
       </c>
       <c r="G550" s="25"/>
     </row>
-    <row r="551" spans="1:16384" customFormat="1">
+    <row r="551" spans="1:16384">
       <c r="A551" s="23" t="s">
         <v>470</v>
       </c>
@@ -17856,7 +17854,7 @@
       </c>
       <c r="G551" s="25"/>
     </row>
-    <row r="552" spans="1:16384" customFormat="1" ht="30">
+    <row r="552" spans="1:16384" ht="30">
       <c r="A552" s="23" t="s">
         <v>85</v>
       </c>
@@ -17875,7 +17873,7 @@
       </c>
       <c r="G552" s="25"/>
     </row>
-    <row r="553" spans="1:16384" customFormat="1">
+    <row r="553" spans="1:16384">
       <c r="A553" s="23" t="s">
         <v>1068</v>
       </c>
@@ -17890,7 +17888,7 @@
       <c r="F553" s="25"/>
       <c r="G553" s="25"/>
     </row>
-    <row r="554" spans="1:16384" customFormat="1" ht="30">
+    <row r="554" spans="1:16384" ht="30">
       <c r="A554" s="23" t="s">
         <v>887</v>
       </c>
@@ -17913,7 +17911,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="555" spans="1:16384" customFormat="1">
+    <row r="555" spans="1:16384">
       <c r="A555" s="23" t="s">
         <v>1498</v>
       </c>
@@ -17932,7 +17930,7 @@
       <c r="F555" s="25"/>
       <c r="G555" s="25"/>
     </row>
-    <row r="556" spans="1:16384" customFormat="1">
+    <row r="556" spans="1:16384">
       <c r="A556" s="23" t="s">
         <v>1011</v>
       </c>
@@ -17951,7 +17949,7 @@
       <c r="F556" s="25"/>
       <c r="G556" s="25"/>
     </row>
-    <row r="557" spans="1:16384" customFormat="1" ht="45">
+    <row r="557" spans="1:16384" ht="45">
       <c r="A557" s="23" t="s">
         <v>1298</v>
       </c>
@@ -17970,7 +17968,7 @@
       <c r="F557" s="25"/>
       <c r="G557" s="25"/>
     </row>
-    <row r="558" spans="1:16384" customFormat="1" ht="30">
+    <row r="558" spans="1:16384" ht="30">
       <c r="A558" s="34" t="s">
         <v>1703</v>
       </c>
@@ -17989,7 +17987,7 @@
       <c r="F558" s="35"/>
       <c r="G558" s="37"/>
     </row>
-    <row r="559" spans="1:16384" customFormat="1" ht="38.25">
+    <row r="559" spans="1:16384" ht="38.25">
       <c r="A559" s="38" t="s">
         <v>1706</v>
       </c>
@@ -34385,7 +34383,7 @@
       <c r="XFC559" s="18"/>
       <c r="XFD559" s="19"/>
     </row>
-    <row r="560" spans="1:16384" customFormat="1">
+    <row r="560" spans="1:16384">
       <c r="A560" s="34" t="s">
         <v>1707</v>
       </c>
@@ -34404,7 +34402,7 @@
       <c r="F560" s="35"/>
       <c r="G560" s="37"/>
     </row>
-    <row r="561" spans="1:16384" customFormat="1" ht="51">
+    <row r="561" spans="1:16384" ht="51">
       <c r="A561" s="38" t="s">
         <v>1722</v>
       </c>
@@ -50800,7 +50798,7 @@
       <c r="XFC561" s="18"/>
       <c r="XFD561" s="19"/>
     </row>
-    <row r="562" spans="1:16384" customFormat="1" ht="56.25">
+    <row r="562" spans="1:16384" ht="56.25">
       <c r="A562" s="34" t="s">
         <v>1723</v>
       </c>
@@ -50819,7 +50817,7 @@
       <c r="F562" s="40"/>
       <c r="G562" s="41"/>
     </row>
-    <row r="563" spans="1:16384" customFormat="1" ht="30">
+    <row r="563" spans="1:16384" ht="30">
       <c r="A563" s="38" t="s">
         <v>1724</v>
       </c>
@@ -50836,7 +50834,7 @@
       <c r="F563" s="40"/>
       <c r="G563" s="41"/>
     </row>
-    <row r="564" spans="1:16384" customFormat="1">
+    <row r="564" spans="1:16384">
       <c r="A564" s="34" t="s">
         <v>1725</v>
       </c>
@@ -50853,7 +50851,7 @@
       <c r="F564" s="40"/>
       <c r="G564" s="41"/>
     </row>
-    <row r="565" spans="1:16384" customFormat="1" ht="30">
+    <row r="565" spans="1:16384" ht="30">
       <c r="A565" s="38" t="s">
         <v>1726</v>
       </c>
@@ -50870,7 +50868,7 @@
       <c r="F565" s="40"/>
       <c r="G565" s="41"/>
     </row>
-    <row r="566" spans="1:16384" customFormat="1">
+    <row r="566" spans="1:16384">
       <c r="A566" s="34" t="s">
         <v>1727</v>
       </c>
@@ -50887,7 +50885,7 @@
       <c r="F566" s="40"/>
       <c r="G566" s="41"/>
     </row>
-    <row r="567" spans="1:16384" customFormat="1">
+    <row r="567" spans="1:16384">
       <c r="A567" s="38" t="s">
         <v>1728</v>
       </c>
@@ -50904,7 +50902,7 @@
       <c r="F567" s="40"/>
       <c r="G567" s="41"/>
     </row>
-    <row r="568" spans="1:16384" customFormat="1">
+    <row r="568" spans="1:16384">
       <c r="A568" s="34" t="s">
         <v>1729</v>
       </c>
@@ -50921,7 +50919,7 @@
       <c r="F568" s="40"/>
       <c r="G568" s="41"/>
     </row>
-    <row r="569" spans="1:16384" customFormat="1" ht="30">
+    <row r="569" spans="1:16384" ht="30">
       <c r="A569" s="38" t="s">
         <v>1730</v>
       </c>
@@ -50938,7 +50936,7 @@
       <c r="F569" s="40"/>
       <c r="G569" s="41"/>
     </row>
-    <row r="570" spans="1:16384" customFormat="1">
+    <row r="570" spans="1:16384">
       <c r="A570" s="34" t="s">
         <v>1731</v>
       </c>
@@ -50955,7 +50953,7 @@
       <c r="F570" s="40"/>
       <c r="G570" s="41"/>
     </row>
-    <row r="571" spans="1:16384" customFormat="1" ht="45">
+    <row r="571" spans="1:16384" ht="45">
       <c r="A571" s="38" t="s">
         <v>1734</v>
       </c>
@@ -50974,7 +50972,7 @@
       <c r="F571" s="40"/>
       <c r="G571" s="41"/>
     </row>
-    <row r="572" spans="1:16384" customFormat="1" ht="30">
+    <row r="572" spans="1:16384" ht="30">
       <c r="A572" s="34" t="s">
         <v>1737</v>
       </c>
@@ -50991,7 +50989,7 @@
       <c r="F572" s="40"/>
       <c r="G572" s="41"/>
     </row>
-    <row r="573" spans="1:16384" customFormat="1" ht="38.25">
+    <row r="573" spans="1:16384" ht="38.25">
       <c r="A573" s="38" t="s">
         <v>1740</v>
       </c>
@@ -51010,7 +51008,7 @@
       <c r="F573" s="40"/>
       <c r="G573" s="41"/>
     </row>
-    <row r="574" spans="1:16384" customFormat="1" ht="30">
+    <row r="574" spans="1:16384" ht="30">
       <c r="A574" s="34" t="s">
         <v>1742</v>
       </c>
@@ -51027,7 +51025,7 @@
       <c r="F574" s="40"/>
       <c r="G574" s="41"/>
     </row>
-    <row r="575" spans="1:16384" customFormat="1" ht="60">
+    <row r="575" spans="1:16384" ht="60">
       <c r="A575" s="38" t="s">
         <v>1745</v>
       </c>
@@ -51044,7 +51042,7 @@
       <c r="F575" s="40"/>
       <c r="G575" s="41"/>
     </row>
-    <row r="576" spans="1:16384" customFormat="1" ht="85.5">
+    <row r="576" spans="1:16384" ht="85.5">
       <c r="A576" s="34" t="s">
         <v>1792</v>
       </c>
@@ -51079,22 +51077,6 @@
       </c>
       <c r="F577" s="10"/>
       <c r="G577"/>
-    </row>
-    <row r="578" spans="1:7" customFormat="1">
-      <c r="A578" s="11"/>
-      <c r="B578" s="12"/>
-      <c r="C578" s="13"/>
-      <c r="D578" s="14"/>
-      <c r="E578" s="3"/>
-      <c r="F578" s="10"/>
-    </row>
-    <row r="579" spans="1:7" customFormat="1">
-      <c r="A579" s="11"/>
-      <c r="B579" s="12"/>
-      <c r="C579" s="13"/>
-      <c r="D579" s="14"/>
-      <c r="E579" s="3"/>
-      <c r="F579" s="10"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:E273">

</xml_diff>